<commit_message>
-Ajout Onglet  pour décrire les informations des pays africains
</commit_message>
<xml_diff>
--- a/President game.xlsx
+++ b/President game.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Lancement du jeu" sheetId="1" r:id="rId1"/>
@@ -12,13 +12,18 @@
     <sheet name="Situation à gérer" sheetId="3" r:id="rId3"/>
     <sheet name="Interface" sheetId="4" r:id="rId4"/>
     <sheet name="Evenements" sheetId="5" r:id="rId5"/>
+    <sheet name="Recueil informations" sheetId="6" r:id="rId6"/>
+    <sheet name="Africa " sheetId="7" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <definedNames>
+    <definedName name="Categorie_Liste">'Africa '!$H$4:$H$23</definedName>
+  </definedNames>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="152">
   <si>
     <t>Nombres de postes ministeriels</t>
   </si>
@@ -233,13 +238,256 @@
   </si>
   <si>
     <t>Conference de presse</t>
+  </si>
+  <si>
+    <t>Pseudo</t>
+  </si>
+  <si>
+    <t>Sexe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Joeur </t>
+  </si>
+  <si>
+    <t>Configuration Jeu</t>
+  </si>
+  <si>
+    <t>Pays</t>
+  </si>
+  <si>
+    <t>Superficie</t>
+  </si>
+  <si>
+    <t>Populatiuon</t>
+  </si>
+  <si>
+    <t>Zone géographique</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Table Pays </t>
+  </si>
+  <si>
+    <t>Population</t>
+  </si>
+  <si>
+    <t>Régime</t>
+  </si>
+  <si>
+    <t>indice économique</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pseudo </t>
+  </si>
+  <si>
+    <t>Fênetre  1</t>
+  </si>
+  <si>
+    <t>Fênetre 2</t>
+  </si>
+  <si>
+    <t>Nom pays</t>
+  </si>
+  <si>
+    <t>Zone Géopolitique</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Indice économique </t>
+  </si>
+  <si>
+    <t>Zone 1</t>
+  </si>
+  <si>
+    <t>Zone 2</t>
+  </si>
+  <si>
+    <t>Zone 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Regime </t>
+  </si>
+  <si>
+    <t>zone 1</t>
+  </si>
+  <si>
+    <t>13 M</t>
+  </si>
+  <si>
+    <t>libérale</t>
+  </si>
+  <si>
+    <t>Informations Par Pays</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Commentaires </t>
+  </si>
+  <si>
+    <t>Nom du pays</t>
+  </si>
+  <si>
+    <t>Date d'indépendance</t>
+  </si>
+  <si>
+    <t>Colonisateur</t>
+  </si>
+  <si>
+    <t>Monnaie</t>
+  </si>
+  <si>
+    <t>langue officielle</t>
+  </si>
+  <si>
+    <t>Principales dialectes</t>
+  </si>
+  <si>
+    <t>Pays limitrophes</t>
+  </si>
+  <si>
+    <t>Pays cotiers (OUI/NON))</t>
+  </si>
+  <si>
+    <t>Drapeau</t>
+  </si>
+  <si>
+    <t>Devise nationale</t>
+  </si>
+  <si>
+    <t xml:space="preserve">emblème </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Division géographique </t>
+  </si>
+  <si>
+    <t xml:space="preserve">région , département, nombre, nom </t>
+  </si>
+  <si>
+    <t>Ressources naturelles</t>
+  </si>
+  <si>
+    <t>Capitale</t>
+  </si>
+  <si>
+    <t>Climat</t>
+  </si>
+  <si>
+    <t>niveau sportif ( par type de sport )</t>
+  </si>
+  <si>
+    <t>célébrités</t>
+  </si>
+  <si>
+    <t>épidémies</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Monuments historique </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Appartenance aux organisations internationales </t>
+  </si>
+  <si>
+    <t>taux d'alphabétisation</t>
+  </si>
+  <si>
+    <t>universités</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Problèmes sociaux </t>
+  </si>
+  <si>
+    <t>dette extérieure</t>
+  </si>
+  <si>
+    <t>PIB</t>
+  </si>
+  <si>
+    <t>Pollution</t>
+  </si>
+  <si>
+    <t>corruption</t>
+  </si>
+  <si>
+    <t xml:space="preserve">relations diplomatiques avec le pays i </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Particulaités </t>
+  </si>
+  <si>
+    <t>religions</t>
+  </si>
+  <si>
+    <t>stabilité politique</t>
+  </si>
+  <si>
+    <t xml:space="preserve">taux de natalité </t>
+  </si>
+  <si>
+    <t>taux de mortalité</t>
+  </si>
+  <si>
+    <t>espérance vie</t>
+  </si>
+  <si>
+    <t>Catégorie</t>
+  </si>
+  <si>
+    <t>Géographique</t>
+  </si>
+  <si>
+    <t>Internationale</t>
+  </si>
+  <si>
+    <t>Economique</t>
+  </si>
+  <si>
+    <t>Sociale</t>
+  </si>
+  <si>
+    <t>Politique</t>
+  </si>
+  <si>
+    <t>Taux d'exportation</t>
+  </si>
+  <si>
+    <t>Taux importation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Produits de premiers nécessité </t>
+  </si>
+  <si>
+    <t>Pour chaque produit donner taux d'importation</t>
+  </si>
+  <si>
+    <t>Infrastructure</t>
+  </si>
+  <si>
+    <t>catastrophes naturelles</t>
+  </si>
+  <si>
+    <t>Géopolitique</t>
+  </si>
+  <si>
+    <t>Santé</t>
+  </si>
+  <si>
+    <t>Educatiion</t>
+  </si>
+  <si>
+    <t>chômage , grêve, manifestations (donner la sensibilité )</t>
+  </si>
+  <si>
+    <t>Environnement</t>
+  </si>
+  <si>
+    <t>5 villes principale</t>
+  </si>
+  <si>
+    <t>Autres</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -254,8 +502,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -292,8 +548,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="9">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -387,11 +661,63 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -437,6 +763,24 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -455,24 +799,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -482,11 +808,47 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="9" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -494,6 +856,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Button" lockText="1"/>
 </file>
 
 <file path=xl/diagrams/colors1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3795,6 +4161,556 @@
       <dsp:cNvGrpSpPr/>
     </dsp:nvGrpSpPr>
     <dsp:grpSpPr/>
+    <dsp:sp modelId="{293579B0-8FDA-4D34-A67F-F2368242682D}">
+      <dsp:nvSpPr>
+        <dsp:cNvPr id="0" name=""/>
+        <dsp:cNvSpPr/>
+      </dsp:nvSpPr>
+      <dsp:spPr>
+        <a:xfrm>
+          <a:off x="265" y="1311708"/>
+          <a:ext cx="2332406" cy="548407"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst>
+            <a:gd name="adj" fmla="val 10000"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent3"/>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="38000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+        <a:scene3d>
+          <a:camera prst="orthographicFront"/>
+          <a:lightRig rig="flat" dir="t"/>
+        </a:scene3d>
+        <a:sp3d prstMaterial="dkEdge">
+          <a:bevelT w="8200" h="38100"/>
+        </a:sp3d>
+      </dsp:spPr>
+      <dsp:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="2">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </dsp:style>
+      <dsp:txBody>
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="6985" tIns="6985" rIns="6985" bIns="6985" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr lvl="0" algn="ctr" defTabSz="488950">
+            <a:lnSpc>
+              <a:spcPct val="90000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPct val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPct val="35000"/>
+            </a:spcAft>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100" kern="1200"/>
+            <a:t>Configuration du profil du Joueur</a:t>
+          </a:r>
+        </a:p>
+      </dsp:txBody>
+      <dsp:txXfrm>
+        <a:off x="16327" y="1327770"/>
+        <a:ext cx="2300282" cy="516283"/>
+      </dsp:txXfrm>
+    </dsp:sp>
+    <dsp:sp modelId="{87AF48A4-8861-42BC-B140-54C2C125EFC6}">
+      <dsp:nvSpPr>
+        <dsp:cNvPr id="0" name=""/>
+        <dsp:cNvSpPr/>
+      </dsp:nvSpPr>
+      <dsp:spPr>
+        <a:xfrm rot="19316383">
+          <a:off x="2206692" y="1187575"/>
+          <a:ext cx="1184921" cy="66181"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst>
+            <a:path>
+              <a:moveTo>
+                <a:pt x="0" y="33090"/>
+              </a:moveTo>
+              <a:lnTo>
+                <a:pt x="1184921" y="33090"/>
+              </a:lnTo>
+            </a:path>
+          </a:pathLst>
+        </a:custGeom>
+        <a:noFill/>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="dk1">
+              <a:shade val="60000"/>
+              <a:hueOff val="0"/>
+              <a:satOff val="0"/>
+              <a:lumOff val="0"/>
+              <a:alphaOff val="0"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:effectLst/>
+      </dsp:spPr>
+      <dsp:style>
+        <a:lnRef idx="2">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor"/>
+      </dsp:style>
+      <dsp:txBody>
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="12700" tIns="0" rIns="12700" bIns="0" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr lvl="0" algn="ctr" defTabSz="222250">
+            <a:lnSpc>
+              <a:spcPct val="90000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPct val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPct val="35000"/>
+            </a:spcAft>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR" sz="500" kern="1200"/>
+        </a:p>
+      </dsp:txBody>
+      <dsp:txXfrm>
+        <a:off x="2769530" y="1191043"/>
+        <a:ext cx="59246" cy="59246"/>
+      </dsp:txXfrm>
+    </dsp:sp>
+    <dsp:sp modelId="{2F462459-C933-484D-A7B8-FE757D7A787C}">
+      <dsp:nvSpPr>
+        <dsp:cNvPr id="0" name=""/>
+        <dsp:cNvSpPr/>
+      </dsp:nvSpPr>
+      <dsp:spPr>
+        <a:xfrm>
+          <a:off x="3265634" y="514381"/>
+          <a:ext cx="4453846" cy="682077"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst>
+            <a:gd name="adj" fmla="val 10000"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFF00"/>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="38000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+        <a:scene3d>
+          <a:camera prst="orthographicFront"/>
+          <a:lightRig rig="flat" dir="t"/>
+        </a:scene3d>
+        <a:sp3d prstMaterial="dkEdge">
+          <a:bevelT w="8200" h="38100"/>
+        </a:sp3d>
+      </dsp:spPr>
+      <dsp:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="2">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </dsp:style>
+      <dsp:txBody>
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="6985" tIns="6985" rIns="6985" bIns="6985" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr lvl="0" algn="ctr" defTabSz="488950">
+            <a:lnSpc>
+              <a:spcPct val="90000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPct val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPct val="35000"/>
+            </a:spcAft>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100" b="1" kern="1200"/>
+            <a:t>PSEUDO  DU JOUEUR    </a:t>
+          </a:r>
+          <a:endParaRPr lang="fr-FR" sz="1100" kern="1200"/>
+        </a:p>
+      </dsp:txBody>
+      <dsp:txXfrm>
+        <a:off x="3285611" y="534358"/>
+        <a:ext cx="4413892" cy="642123"/>
+      </dsp:txXfrm>
+    </dsp:sp>
+    <dsp:sp modelId="{9A12F15A-DD69-4747-986B-EC2A2040FC04}">
+      <dsp:nvSpPr>
+        <dsp:cNvPr id="0" name=""/>
+        <dsp:cNvSpPr/>
+      </dsp:nvSpPr>
+      <dsp:spPr>
+        <a:xfrm rot="162699">
+          <a:off x="2332149" y="1574915"/>
+          <a:ext cx="934008" cy="66181"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst>
+            <a:path>
+              <a:moveTo>
+                <a:pt x="0" y="33090"/>
+              </a:moveTo>
+              <a:lnTo>
+                <a:pt x="934008" y="33090"/>
+              </a:lnTo>
+            </a:path>
+          </a:pathLst>
+        </a:custGeom>
+        <a:noFill/>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="dk1">
+              <a:shade val="60000"/>
+              <a:hueOff val="0"/>
+              <a:satOff val="0"/>
+              <a:lumOff val="0"/>
+              <a:alphaOff val="0"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:effectLst/>
+      </dsp:spPr>
+      <dsp:style>
+        <a:lnRef idx="2">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor"/>
+      </dsp:style>
+      <dsp:txBody>
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="12700" tIns="0" rIns="12700" bIns="0" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr lvl="0" algn="ctr" defTabSz="222250">
+            <a:lnSpc>
+              <a:spcPct val="90000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPct val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPct val="35000"/>
+            </a:spcAft>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR" sz="500" kern="1200"/>
+        </a:p>
+      </dsp:txBody>
+      <dsp:txXfrm>
+        <a:off x="2775803" y="1584656"/>
+        <a:ext cx="46700" cy="46700"/>
+      </dsp:txXfrm>
+    </dsp:sp>
+    <dsp:sp modelId="{0801CC26-B71E-45B6-95A0-1021BF843F5E}">
+      <dsp:nvSpPr>
+        <dsp:cNvPr id="0" name=""/>
+        <dsp:cNvSpPr/>
+      </dsp:nvSpPr>
+      <dsp:spPr>
+        <a:xfrm>
+          <a:off x="3265634" y="1371389"/>
+          <a:ext cx="4468400" cy="517421"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst>
+            <a:gd name="adj" fmla="val 10000"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFF00"/>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="38000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+        <a:scene3d>
+          <a:camera prst="orthographicFront"/>
+          <a:lightRig rig="flat" dir="t"/>
+        </a:scene3d>
+        <a:sp3d prstMaterial="dkEdge">
+          <a:bevelT w="8200" h="38100"/>
+        </a:sp3d>
+      </dsp:spPr>
+      <dsp:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="2">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </dsp:style>
+      <dsp:txBody>
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="6985" tIns="6985" rIns="6985" bIns="6985" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr lvl="0" algn="ctr" defTabSz="488950">
+            <a:lnSpc>
+              <a:spcPct val="90000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPct val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPct val="35000"/>
+            </a:spcAft>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100" b="1" kern="1200"/>
+            <a:t>SEXE  </a:t>
+          </a:r>
+        </a:p>
+      </dsp:txBody>
+      <dsp:txXfrm>
+        <a:off x="3280789" y="1386544"/>
+        <a:ext cx="4438090" cy="487111"/>
+      </dsp:txXfrm>
+    </dsp:sp>
+    <dsp:sp modelId="{7C99A380-E6F6-4F99-BD1F-7BBDA45513C5}">
+      <dsp:nvSpPr>
+        <dsp:cNvPr id="0" name=""/>
+        <dsp:cNvSpPr/>
+      </dsp:nvSpPr>
+      <dsp:spPr>
+        <a:xfrm rot="2463779">
+          <a:off x="2180467" y="1959228"/>
+          <a:ext cx="1237370" cy="66181"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst>
+            <a:path>
+              <a:moveTo>
+                <a:pt x="0" y="33090"/>
+              </a:moveTo>
+              <a:lnTo>
+                <a:pt x="1237370" y="33090"/>
+              </a:lnTo>
+            </a:path>
+          </a:pathLst>
+        </a:custGeom>
+        <a:noFill/>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="dk1">
+              <a:shade val="60000"/>
+              <a:hueOff val="0"/>
+              <a:satOff val="0"/>
+              <a:lumOff val="0"/>
+              <a:alphaOff val="0"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:effectLst/>
+      </dsp:spPr>
+      <dsp:style>
+        <a:lnRef idx="2">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor"/>
+      </dsp:style>
+      <dsp:txBody>
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="12700" tIns="0" rIns="12700" bIns="0" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr lvl="0" algn="ctr" defTabSz="222250">
+            <a:lnSpc>
+              <a:spcPct val="90000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPct val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPct val="35000"/>
+            </a:spcAft>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR" sz="500" kern="1200"/>
+        </a:p>
+      </dsp:txBody>
+      <dsp:txXfrm>
+        <a:off x="2768218" y="1961385"/>
+        <a:ext cx="61868" cy="61868"/>
+      </dsp:txXfrm>
+    </dsp:sp>
+    <dsp:sp modelId="{0B42F808-76D1-48A4-BB9E-1FCE3B026DBC}">
+      <dsp:nvSpPr>
+        <dsp:cNvPr id="0" name=""/>
+        <dsp:cNvSpPr/>
+      </dsp:nvSpPr>
+      <dsp:spPr>
+        <a:xfrm>
+          <a:off x="3265634" y="2101875"/>
+          <a:ext cx="4373495" cy="593702"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst>
+            <a:gd name="adj" fmla="val 10000"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFF00"/>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="38000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+        <a:scene3d>
+          <a:camera prst="orthographicFront"/>
+          <a:lightRig rig="flat" dir="t"/>
+        </a:scene3d>
+        <a:sp3d prstMaterial="dkEdge">
+          <a:bevelT w="8200" h="38100"/>
+        </a:sp3d>
+      </dsp:spPr>
+      <dsp:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="2">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </dsp:style>
+      <dsp:txBody>
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="6985" tIns="6985" rIns="6985" bIns="6985" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr lvl="0" algn="ctr" defTabSz="488950">
+            <a:lnSpc>
+              <a:spcPct val="90000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPct val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPct val="35000"/>
+            </a:spcAft>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100" b="1" kern="1200"/>
+            <a:t>AVATAR</a:t>
+          </a:r>
+        </a:p>
+      </dsp:txBody>
+      <dsp:txXfrm>
+        <a:off x="3283023" y="2119264"/>
+        <a:ext cx="4338717" cy="558924"/>
+      </dsp:txXfrm>
+    </dsp:sp>
   </dsp:spTree>
 </dsp:drawing>
 </file>
@@ -3807,6 +4723,2449 @@
       <dsp:cNvGrpSpPr/>
     </dsp:nvGrpSpPr>
     <dsp:grpSpPr/>
+    <dsp:sp modelId="{293579B0-8FDA-4D34-A67F-F2368242682D}">
+      <dsp:nvSpPr>
+        <dsp:cNvPr id="0" name=""/>
+        <dsp:cNvSpPr/>
+      </dsp:nvSpPr>
+      <dsp:spPr>
+        <a:xfrm>
+          <a:off x="2100" y="5863403"/>
+          <a:ext cx="2144148" cy="504142"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst>
+            <a:gd name="adj" fmla="val 10000"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent3"/>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="38000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+        <a:scene3d>
+          <a:camera prst="orthographicFront"/>
+          <a:lightRig rig="flat" dir="t"/>
+        </a:scene3d>
+        <a:sp3d prstMaterial="dkEdge">
+          <a:bevelT w="8200" h="38100"/>
+        </a:sp3d>
+      </dsp:spPr>
+      <dsp:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="2">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </dsp:style>
+      <dsp:txBody>
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="6985" tIns="6985" rIns="6985" bIns="6985" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr lvl="0" algn="ctr" defTabSz="488950">
+            <a:lnSpc>
+              <a:spcPct val="90000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPct val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPct val="35000"/>
+            </a:spcAft>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100" kern="1200"/>
+            <a:t>Configuration de la partie</a:t>
+          </a:r>
+        </a:p>
+      </dsp:txBody>
+      <dsp:txXfrm>
+        <a:off x="16866" y="5878169"/>
+        <a:ext cx="2114616" cy="474610"/>
+      </dsp:txXfrm>
+    </dsp:sp>
+    <dsp:sp modelId="{87AF48A4-8861-42BC-B140-54C2C125EFC6}">
+      <dsp:nvSpPr>
+        <dsp:cNvPr id="0" name=""/>
+        <dsp:cNvSpPr/>
+      </dsp:nvSpPr>
+      <dsp:spPr>
+        <a:xfrm rot="16910600">
+          <a:off x="592619" y="4194127"/>
+          <a:ext cx="3909663" cy="16259"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst>
+            <a:path>
+              <a:moveTo>
+                <a:pt x="0" y="8129"/>
+              </a:moveTo>
+              <a:lnTo>
+                <a:pt x="3909663" y="8129"/>
+              </a:lnTo>
+            </a:path>
+          </a:pathLst>
+        </a:custGeom>
+        <a:noFill/>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="dk1">
+              <a:shade val="60000"/>
+              <a:hueOff val="0"/>
+              <a:satOff val="0"/>
+              <a:lumOff val="0"/>
+              <a:alphaOff val="0"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:effectLst/>
+      </dsp:spPr>
+      <dsp:style>
+        <a:lnRef idx="2">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor"/>
+      </dsp:style>
+      <dsp:txBody>
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="12700" tIns="0" rIns="12700" bIns="0" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr lvl="0" algn="ctr" defTabSz="400050">
+            <a:lnSpc>
+              <a:spcPct val="90000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPct val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPct val="35000"/>
+            </a:spcAft>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR" sz="900" kern="1200"/>
+        </a:p>
+      </dsp:txBody>
+      <dsp:txXfrm>
+        <a:off x="2449709" y="4104515"/>
+        <a:ext cx="195483" cy="195483"/>
+      </dsp:txXfrm>
+    </dsp:sp>
+    <dsp:sp modelId="{2F462459-C933-484D-A7B8-FE757D7A787C}">
+      <dsp:nvSpPr>
+        <dsp:cNvPr id="0" name=""/>
+        <dsp:cNvSpPr/>
+      </dsp:nvSpPr>
+      <dsp:spPr>
+        <a:xfrm>
+          <a:off x="2948652" y="1975527"/>
+          <a:ext cx="4094358" cy="627023"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst>
+            <a:gd name="adj" fmla="val 10000"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFF00"/>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="38000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+        <a:scene3d>
+          <a:camera prst="orthographicFront"/>
+          <a:lightRig rig="flat" dir="t"/>
+        </a:scene3d>
+        <a:sp3d prstMaterial="dkEdge">
+          <a:bevelT w="8200" h="38100"/>
+        </a:sp3d>
+      </dsp:spPr>
+      <dsp:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="2">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </dsp:style>
+      <dsp:txBody>
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="6985" tIns="6985" rIns="6985" bIns="6985" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr lvl="0" algn="ctr" defTabSz="488950">
+            <a:lnSpc>
+              <a:spcPct val="90000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPct val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPct val="35000"/>
+            </a:spcAft>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100" b="1" kern="1200"/>
+            <a:t>TAILLE  DE  LA  POPULATION  </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100" kern="1200"/>
+            <a:t>(plage de valeurs ) </a:t>
+          </a:r>
+        </a:p>
+      </dsp:txBody>
+      <dsp:txXfrm>
+        <a:off x="2967017" y="1993892"/>
+        <a:ext cx="4057628" cy="590293"/>
+      </dsp:txXfrm>
+    </dsp:sp>
+    <dsp:sp modelId="{E093353F-D98B-4AA1-95A6-75570749C0F9}">
+      <dsp:nvSpPr>
+        <dsp:cNvPr id="0" name=""/>
+        <dsp:cNvSpPr/>
+      </dsp:nvSpPr>
+      <dsp:spPr>
+        <a:xfrm rot="18541931">
+          <a:off x="6826022" y="1825653"/>
+          <a:ext cx="1172144" cy="16259"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst>
+            <a:path>
+              <a:moveTo>
+                <a:pt x="0" y="8129"/>
+              </a:moveTo>
+              <a:lnTo>
+                <a:pt x="1172144" y="8129"/>
+              </a:lnTo>
+            </a:path>
+          </a:pathLst>
+        </a:custGeom>
+        <a:noFill/>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="dk1">
+              <a:shade val="80000"/>
+              <a:hueOff val="0"/>
+              <a:satOff val="0"/>
+              <a:lumOff val="0"/>
+              <a:alphaOff val="0"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:effectLst/>
+      </dsp:spPr>
+      <dsp:style>
+        <a:lnRef idx="2">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor"/>
+      </dsp:style>
+      <dsp:txBody>
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="12700" tIns="0" rIns="12700" bIns="0" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr lvl="0" algn="ctr" defTabSz="222250">
+            <a:lnSpc>
+              <a:spcPct val="90000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPct val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPct val="35000"/>
+            </a:spcAft>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR" sz="500" kern="1200"/>
+        </a:p>
+      </dsp:txBody>
+      <dsp:txXfrm>
+        <a:off x="7382790" y="1804479"/>
+        <a:ext cx="58607" cy="58607"/>
+      </dsp:txXfrm>
+    </dsp:sp>
+    <dsp:sp modelId="{AE94E6C6-3040-492D-B358-C18046AB2EBC}">
+      <dsp:nvSpPr>
+        <dsp:cNvPr id="0" name=""/>
+        <dsp:cNvSpPr/>
+      </dsp:nvSpPr>
+      <dsp:spPr>
+        <a:xfrm>
+          <a:off x="7781177" y="1253603"/>
+          <a:ext cx="2144148" cy="249846"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst>
+            <a:gd name="adj" fmla="val 10000"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:gradFill rotWithShape="0">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="lt1">
+                <a:hueOff val="0"/>
+                <a:satOff val="0"/>
+                <a:lumOff val="0"/>
+                <a:alphaOff val="0"/>
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="lt1">
+                <a:hueOff val="0"/>
+                <a:satOff val="0"/>
+                <a:lumOff val="0"/>
+                <a:alphaOff val="0"/>
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="lt1">
+                <a:hueOff val="0"/>
+                <a:satOff val="0"/>
+                <a:lumOff val="0"/>
+                <a:alphaOff val="0"/>
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="38000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+        <a:scene3d>
+          <a:camera prst="orthographicFront"/>
+          <a:lightRig rig="flat" dir="t"/>
+        </a:scene3d>
+        <a:sp3d prstMaterial="dkEdge">
+          <a:bevelT w="8200" h="38100"/>
+        </a:sp3d>
+      </dsp:spPr>
+      <dsp:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="2">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </dsp:style>
+      <dsp:txBody>
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="6985" tIns="6985" rIns="6985" bIns="6985" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr lvl="0" algn="ctr" defTabSz="488950">
+            <a:lnSpc>
+              <a:spcPct val="90000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPct val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPct val="35000"/>
+            </a:spcAft>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100" kern="1200"/>
+            <a:t>0 à 5 millions</a:t>
+          </a:r>
+        </a:p>
+      </dsp:txBody>
+      <dsp:txXfrm>
+        <a:off x="7788495" y="1260921"/>
+        <a:ext cx="2129512" cy="235210"/>
+      </dsp:txXfrm>
+    </dsp:sp>
+    <dsp:sp modelId="{D0802D8A-17E0-42FF-8F46-C0B190274122}">
+      <dsp:nvSpPr>
+        <dsp:cNvPr id="0" name=""/>
+        <dsp:cNvSpPr/>
+      </dsp:nvSpPr>
+      <dsp:spPr>
+        <a:xfrm rot="19867668">
+          <a:off x="6993269" y="2087683"/>
+          <a:ext cx="800340" cy="16259"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst>
+            <a:path>
+              <a:moveTo>
+                <a:pt x="0" y="8129"/>
+              </a:moveTo>
+              <a:lnTo>
+                <a:pt x="800340" y="8129"/>
+              </a:lnTo>
+            </a:path>
+          </a:pathLst>
+        </a:custGeom>
+        <a:noFill/>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="dk1">
+              <a:shade val="80000"/>
+              <a:hueOff val="0"/>
+              <a:satOff val="0"/>
+              <a:lumOff val="0"/>
+              <a:alphaOff val="0"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:effectLst/>
+      </dsp:spPr>
+      <dsp:style>
+        <a:lnRef idx="2">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor"/>
+      </dsp:style>
+      <dsp:txBody>
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="12700" tIns="0" rIns="12700" bIns="0" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr lvl="0" algn="ctr" defTabSz="222250">
+            <a:lnSpc>
+              <a:spcPct val="90000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPct val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPct val="35000"/>
+            </a:spcAft>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR" sz="500" kern="1200"/>
+        </a:p>
+      </dsp:txBody>
+      <dsp:txXfrm>
+        <a:off x="7373431" y="2075805"/>
+        <a:ext cx="40017" cy="40017"/>
+      </dsp:txXfrm>
+    </dsp:sp>
+    <dsp:sp modelId="{FB3B5045-7F40-480B-A83E-702B616FA88D}">
+      <dsp:nvSpPr>
+        <dsp:cNvPr id="0" name=""/>
+        <dsp:cNvSpPr/>
+      </dsp:nvSpPr>
+      <dsp:spPr>
+        <a:xfrm>
+          <a:off x="7743868" y="1767823"/>
+          <a:ext cx="2144148" cy="269530"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst>
+            <a:gd name="adj" fmla="val 10000"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:gradFill rotWithShape="0">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="lt1">
+                <a:hueOff val="0"/>
+                <a:satOff val="0"/>
+                <a:lumOff val="0"/>
+                <a:alphaOff val="0"/>
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="lt1">
+                <a:hueOff val="0"/>
+                <a:satOff val="0"/>
+                <a:lumOff val="0"/>
+                <a:alphaOff val="0"/>
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="lt1">
+                <a:hueOff val="0"/>
+                <a:satOff val="0"/>
+                <a:lumOff val="0"/>
+                <a:alphaOff val="0"/>
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="38000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+        <a:scene3d>
+          <a:camera prst="orthographicFront"/>
+          <a:lightRig rig="flat" dir="t"/>
+        </a:scene3d>
+        <a:sp3d prstMaterial="dkEdge">
+          <a:bevelT w="8200" h="38100"/>
+        </a:sp3d>
+      </dsp:spPr>
+      <dsp:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="2">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </dsp:style>
+      <dsp:txBody>
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="6985" tIns="6985" rIns="6985" bIns="6985" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr lvl="0" algn="ctr" defTabSz="488950">
+            <a:lnSpc>
+              <a:spcPct val="90000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPct val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPct val="35000"/>
+            </a:spcAft>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100" kern="1200"/>
+            <a:t>5 a 100 millions</a:t>
+          </a:r>
+        </a:p>
+      </dsp:txBody>
+      <dsp:txXfrm>
+        <a:off x="7751762" y="1775717"/>
+        <a:ext cx="2128360" cy="253742"/>
+      </dsp:txXfrm>
+    </dsp:sp>
+    <dsp:sp modelId="{0B20FA40-1E51-45FB-8061-C664A47C365E}">
+      <dsp:nvSpPr>
+        <dsp:cNvPr id="0" name=""/>
+        <dsp:cNvSpPr/>
+      </dsp:nvSpPr>
+      <dsp:spPr>
+        <a:xfrm rot="790488">
+          <a:off x="7033178" y="2366053"/>
+          <a:ext cx="747131" cy="16259"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst>
+            <a:path>
+              <a:moveTo>
+                <a:pt x="0" y="8129"/>
+              </a:moveTo>
+              <a:lnTo>
+                <a:pt x="747131" y="8129"/>
+              </a:lnTo>
+            </a:path>
+          </a:pathLst>
+        </a:custGeom>
+        <a:noFill/>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="dk1">
+              <a:shade val="80000"/>
+              <a:hueOff val="0"/>
+              <a:satOff val="0"/>
+              <a:lumOff val="0"/>
+              <a:alphaOff val="0"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:effectLst/>
+      </dsp:spPr>
+      <dsp:style>
+        <a:lnRef idx="2">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor"/>
+      </dsp:style>
+      <dsp:txBody>
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="12700" tIns="0" rIns="12700" bIns="0" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr lvl="0" algn="ctr" defTabSz="222250">
+            <a:lnSpc>
+              <a:spcPct val="90000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPct val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPct val="35000"/>
+            </a:spcAft>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR" sz="500" kern="1200"/>
+        </a:p>
+      </dsp:txBody>
+      <dsp:txXfrm>
+        <a:off x="7388066" y="2355504"/>
+        <a:ext cx="37356" cy="37356"/>
+      </dsp:txXfrm>
+    </dsp:sp>
+    <dsp:sp modelId="{92014794-B5AE-4341-8D1D-1BDCCA634B2C}">
+      <dsp:nvSpPr>
+        <dsp:cNvPr id="0" name=""/>
+        <dsp:cNvSpPr/>
+      </dsp:nvSpPr>
+      <dsp:spPr>
+        <a:xfrm>
+          <a:off x="7770477" y="2297706"/>
+          <a:ext cx="2144148" cy="323241"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst>
+            <a:gd name="adj" fmla="val 10000"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:gradFill rotWithShape="0">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="lt1">
+                <a:hueOff val="0"/>
+                <a:satOff val="0"/>
+                <a:lumOff val="0"/>
+                <a:alphaOff val="0"/>
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="lt1">
+                <a:hueOff val="0"/>
+                <a:satOff val="0"/>
+                <a:lumOff val="0"/>
+                <a:alphaOff val="0"/>
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="lt1">
+                <a:hueOff val="0"/>
+                <a:satOff val="0"/>
+                <a:lumOff val="0"/>
+                <a:alphaOff val="0"/>
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="38000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+        <a:scene3d>
+          <a:camera prst="orthographicFront"/>
+          <a:lightRig rig="flat" dir="t"/>
+        </a:scene3d>
+        <a:sp3d prstMaterial="dkEdge">
+          <a:bevelT w="8200" h="38100"/>
+        </a:sp3d>
+      </dsp:spPr>
+      <dsp:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="2">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </dsp:style>
+      <dsp:txBody>
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="6985" tIns="6985" rIns="6985" bIns="6985" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr lvl="0" algn="ctr" defTabSz="488950">
+            <a:lnSpc>
+              <a:spcPct val="90000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPct val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPct val="35000"/>
+            </a:spcAft>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100" kern="1200"/>
+            <a:t>100 à 500 millions</a:t>
+          </a:r>
+        </a:p>
+      </dsp:txBody>
+      <dsp:txXfrm>
+        <a:off x="7779944" y="2307173"/>
+        <a:ext cx="2125214" cy="304307"/>
+      </dsp:txXfrm>
+    </dsp:sp>
+    <dsp:sp modelId="{57CBFA0B-0A90-47FC-B128-F11D82854EA5}">
+      <dsp:nvSpPr>
+        <dsp:cNvPr id="0" name=""/>
+        <dsp:cNvSpPr/>
+      </dsp:nvSpPr>
+      <dsp:spPr>
+        <a:xfrm rot="2850557">
+          <a:off x="6884099" y="2641983"/>
+          <a:ext cx="979335" cy="16259"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst>
+            <a:path>
+              <a:moveTo>
+                <a:pt x="0" y="8129"/>
+              </a:moveTo>
+              <a:lnTo>
+                <a:pt x="979335" y="8129"/>
+              </a:lnTo>
+            </a:path>
+          </a:pathLst>
+        </a:custGeom>
+        <a:noFill/>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="dk1">
+              <a:shade val="80000"/>
+              <a:hueOff val="0"/>
+              <a:satOff val="0"/>
+              <a:lumOff val="0"/>
+              <a:alphaOff val="0"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:effectLst/>
+      </dsp:spPr>
+      <dsp:style>
+        <a:lnRef idx="2">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor"/>
+      </dsp:style>
+      <dsp:txBody>
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="12700" tIns="0" rIns="12700" bIns="0" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr lvl="0" algn="ctr" defTabSz="222250">
+            <a:lnSpc>
+              <a:spcPct val="90000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPct val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPct val="35000"/>
+            </a:spcAft>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR" sz="500" kern="1200"/>
+        </a:p>
+      </dsp:txBody>
+      <dsp:txXfrm>
+        <a:off x="7349284" y="2625630"/>
+        <a:ext cx="48966" cy="48966"/>
+      </dsp:txXfrm>
+    </dsp:sp>
+    <dsp:sp modelId="{1ADB50A0-DCBF-4264-A54F-18BD42C70618}">
+      <dsp:nvSpPr>
+        <dsp:cNvPr id="0" name=""/>
+        <dsp:cNvSpPr/>
+      </dsp:nvSpPr>
+      <dsp:spPr>
+        <a:xfrm>
+          <a:off x="7704523" y="2879564"/>
+          <a:ext cx="2144148" cy="263247"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst>
+            <a:gd name="adj" fmla="val 10000"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:gradFill rotWithShape="0">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="lt1">
+                <a:hueOff val="0"/>
+                <a:satOff val="0"/>
+                <a:lumOff val="0"/>
+                <a:alphaOff val="0"/>
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="lt1">
+                <a:hueOff val="0"/>
+                <a:satOff val="0"/>
+                <a:lumOff val="0"/>
+                <a:alphaOff val="0"/>
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="lt1">
+                <a:hueOff val="0"/>
+                <a:satOff val="0"/>
+                <a:lumOff val="0"/>
+                <a:alphaOff val="0"/>
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="38000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+        <a:scene3d>
+          <a:camera prst="orthographicFront"/>
+          <a:lightRig rig="flat" dir="t"/>
+        </a:scene3d>
+        <a:sp3d prstMaterial="dkEdge">
+          <a:bevelT w="8200" h="38100"/>
+        </a:sp3d>
+      </dsp:spPr>
+      <dsp:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="2">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </dsp:style>
+      <dsp:txBody>
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="6985" tIns="6985" rIns="6985" bIns="6985" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr lvl="0" algn="ctr" defTabSz="488950">
+            <a:lnSpc>
+              <a:spcPct val="90000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPct val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPct val="35000"/>
+            </a:spcAft>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100" kern="1200"/>
+            <a:t>500 à 1000 millions</a:t>
+          </a:r>
+        </a:p>
+      </dsp:txBody>
+      <dsp:txXfrm>
+        <a:off x="7712233" y="2887274"/>
+        <a:ext cx="2128728" cy="247827"/>
+      </dsp:txXfrm>
+    </dsp:sp>
+    <dsp:sp modelId="{0B10DC64-8DA8-4A97-8911-A7D6D433850B}">
+      <dsp:nvSpPr>
+        <dsp:cNvPr id="0" name=""/>
+        <dsp:cNvSpPr/>
+      </dsp:nvSpPr>
+      <dsp:spPr>
+        <a:xfrm rot="3594787">
+          <a:off x="6700613" y="2874999"/>
+          <a:ext cx="1373195" cy="16259"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst>
+            <a:path>
+              <a:moveTo>
+                <a:pt x="0" y="8129"/>
+              </a:moveTo>
+              <a:lnTo>
+                <a:pt x="1373195" y="8129"/>
+              </a:lnTo>
+            </a:path>
+          </a:pathLst>
+        </a:custGeom>
+        <a:noFill/>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="dk1">
+              <a:shade val="80000"/>
+              <a:hueOff val="0"/>
+              <a:satOff val="0"/>
+              <a:lumOff val="0"/>
+              <a:alphaOff val="0"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:effectLst/>
+      </dsp:spPr>
+      <dsp:style>
+        <a:lnRef idx="2">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor"/>
+      </dsp:style>
+      <dsp:txBody>
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="12700" tIns="0" rIns="12700" bIns="0" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr lvl="0" algn="ctr" defTabSz="222250">
+            <a:lnSpc>
+              <a:spcPct val="90000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPct val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPct val="35000"/>
+            </a:spcAft>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR" sz="500" kern="1200"/>
+        </a:p>
+      </dsp:txBody>
+      <dsp:txXfrm>
+        <a:off x="7352881" y="2848799"/>
+        <a:ext cx="68659" cy="68659"/>
+      </dsp:txXfrm>
+    </dsp:sp>
+    <dsp:sp modelId="{4018FF83-3A39-4F74-AAA2-E8D5D5C59D1D}">
+      <dsp:nvSpPr>
+        <dsp:cNvPr id="0" name=""/>
+        <dsp:cNvSpPr/>
+      </dsp:nvSpPr>
+      <dsp:spPr>
+        <a:xfrm>
+          <a:off x="7731411" y="3344694"/>
+          <a:ext cx="2144148" cy="265048"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst>
+            <a:gd name="adj" fmla="val 10000"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:gradFill rotWithShape="0">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="lt1">
+                <a:hueOff val="0"/>
+                <a:satOff val="0"/>
+                <a:lumOff val="0"/>
+                <a:alphaOff val="0"/>
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="lt1">
+                <a:hueOff val="0"/>
+                <a:satOff val="0"/>
+                <a:lumOff val="0"/>
+                <a:alphaOff val="0"/>
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="lt1">
+                <a:hueOff val="0"/>
+                <a:satOff val="0"/>
+                <a:lumOff val="0"/>
+                <a:alphaOff val="0"/>
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="38000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+        <a:scene3d>
+          <a:camera prst="orthographicFront"/>
+          <a:lightRig rig="flat" dir="t"/>
+        </a:scene3d>
+        <a:sp3d prstMaterial="dkEdge">
+          <a:bevelT w="8200" h="38100"/>
+        </a:sp3d>
+      </dsp:spPr>
+      <dsp:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="2">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </dsp:style>
+      <dsp:txBody>
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="6985" tIns="6985" rIns="6985" bIns="6985" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr lvl="0" algn="ctr" defTabSz="488950">
+            <a:lnSpc>
+              <a:spcPct val="90000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPct val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPct val="35000"/>
+            </a:spcAft>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100" kern="1200"/>
+            <a:t>1 à 1,5 milliards</a:t>
+          </a:r>
+        </a:p>
+      </dsp:txBody>
+      <dsp:txXfrm>
+        <a:off x="7739174" y="3352457"/>
+        <a:ext cx="2128622" cy="249522"/>
+      </dsp:txXfrm>
+    </dsp:sp>
+    <dsp:sp modelId="{9A12F15A-DD69-4747-986B-EC2A2040FC04}">
+      <dsp:nvSpPr>
+        <dsp:cNvPr id="0" name=""/>
+        <dsp:cNvSpPr/>
+      </dsp:nvSpPr>
+      <dsp:spPr>
+        <a:xfrm rot="1119628">
+          <a:off x="2122454" y="6252166"/>
+          <a:ext cx="905246" cy="16259"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst>
+            <a:path>
+              <a:moveTo>
+                <a:pt x="0" y="8129"/>
+              </a:moveTo>
+              <a:lnTo>
+                <a:pt x="905246" y="8129"/>
+              </a:lnTo>
+            </a:path>
+          </a:pathLst>
+        </a:custGeom>
+        <a:noFill/>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="dk1">
+              <a:shade val="60000"/>
+              <a:hueOff val="0"/>
+              <a:satOff val="0"/>
+              <a:lumOff val="0"/>
+              <a:alphaOff val="0"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:effectLst/>
+      </dsp:spPr>
+      <dsp:style>
+        <a:lnRef idx="2">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor"/>
+      </dsp:style>
+      <dsp:txBody>
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="12700" tIns="0" rIns="12700" bIns="0" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr lvl="0" algn="ctr" defTabSz="222250">
+            <a:lnSpc>
+              <a:spcPct val="90000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPct val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPct val="35000"/>
+            </a:spcAft>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR" sz="500" kern="1200"/>
+        </a:p>
+      </dsp:txBody>
+      <dsp:txXfrm>
+        <a:off x="2552446" y="6237665"/>
+        <a:ext cx="45262" cy="45262"/>
+      </dsp:txXfrm>
+    </dsp:sp>
+    <dsp:sp modelId="{0801CC26-B71E-45B6-95A0-1021BF843F5E}">
+      <dsp:nvSpPr>
+        <dsp:cNvPr id="0" name=""/>
+        <dsp:cNvSpPr/>
+      </dsp:nvSpPr>
+      <dsp:spPr>
+        <a:xfrm>
+          <a:off x="3003907" y="6083891"/>
+          <a:ext cx="4107737" cy="642451"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst>
+            <a:gd name="adj" fmla="val 10000"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFF00"/>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="38000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+        <a:scene3d>
+          <a:camera prst="orthographicFront"/>
+          <a:lightRig rig="flat" dir="t"/>
+        </a:scene3d>
+        <a:sp3d prstMaterial="dkEdge">
+          <a:bevelT w="8200" h="38100"/>
+        </a:sp3d>
+      </dsp:spPr>
+      <dsp:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="2">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </dsp:style>
+      <dsp:txBody>
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="6985" tIns="6985" rIns="6985" bIns="6985" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr lvl="0" algn="ctr" defTabSz="488950">
+            <a:lnSpc>
+              <a:spcPct val="90000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPct val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPct val="35000"/>
+            </a:spcAft>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100" b="1" kern="1200"/>
+            <a:t>INDICE  ECONOMIQUE   (1 à 10) </a:t>
+          </a:r>
+        </a:p>
+      </dsp:txBody>
+      <dsp:txXfrm>
+        <a:off x="3022724" y="6102708"/>
+        <a:ext cx="4070103" cy="604817"/>
+      </dsp:txXfrm>
+    </dsp:sp>
+    <dsp:sp modelId="{5FD72AEF-E9A7-4420-B47E-2EB98EFAB197}">
+      <dsp:nvSpPr>
+        <dsp:cNvPr id="0" name=""/>
+        <dsp:cNvSpPr/>
+      </dsp:nvSpPr>
+      <dsp:spPr>
+        <a:xfrm rot="18930367">
+          <a:off x="6939305" y="5975667"/>
+          <a:ext cx="1202339" cy="16259"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst>
+            <a:path>
+              <a:moveTo>
+                <a:pt x="0" y="8129"/>
+              </a:moveTo>
+              <a:lnTo>
+                <a:pt x="1202339" y="8129"/>
+              </a:lnTo>
+            </a:path>
+          </a:pathLst>
+        </a:custGeom>
+        <a:noFill/>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="dk1">
+              <a:shade val="80000"/>
+              <a:hueOff val="0"/>
+              <a:satOff val="0"/>
+              <a:lumOff val="0"/>
+              <a:alphaOff val="0"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:effectLst/>
+      </dsp:spPr>
+      <dsp:style>
+        <a:lnRef idx="2">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor"/>
+      </dsp:style>
+      <dsp:txBody>
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="12700" tIns="0" rIns="12700" bIns="0" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr lvl="0" algn="ctr" defTabSz="222250">
+            <a:lnSpc>
+              <a:spcPct val="90000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPct val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPct val="35000"/>
+            </a:spcAft>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR" sz="500" kern="1200"/>
+        </a:p>
+      </dsp:txBody>
+      <dsp:txXfrm>
+        <a:off x="7510416" y="5953739"/>
+        <a:ext cx="60116" cy="60116"/>
+      </dsp:txXfrm>
+    </dsp:sp>
+    <dsp:sp modelId="{7A1CC12C-133D-475D-9848-5042A028D89E}">
+      <dsp:nvSpPr>
+        <dsp:cNvPr id="0" name=""/>
+        <dsp:cNvSpPr/>
+      </dsp:nvSpPr>
+      <dsp:spPr>
+        <a:xfrm>
+          <a:off x="7969304" y="5381849"/>
+          <a:ext cx="2144148" cy="361256"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst>
+            <a:gd name="adj" fmla="val 10000"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:gradFill rotWithShape="0">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="lt1">
+                <a:hueOff val="0"/>
+                <a:satOff val="0"/>
+                <a:lumOff val="0"/>
+                <a:alphaOff val="0"/>
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="lt1">
+                <a:hueOff val="0"/>
+                <a:satOff val="0"/>
+                <a:lumOff val="0"/>
+                <a:alphaOff val="0"/>
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="lt1">
+                <a:hueOff val="0"/>
+                <a:satOff val="0"/>
+                <a:lumOff val="0"/>
+                <a:alphaOff val="0"/>
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="38000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+        <a:scene3d>
+          <a:camera prst="orthographicFront"/>
+          <a:lightRig rig="flat" dir="t"/>
+        </a:scene3d>
+        <a:sp3d prstMaterial="dkEdge">
+          <a:bevelT w="8200" h="38100"/>
+        </a:sp3d>
+      </dsp:spPr>
+      <dsp:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="2">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </dsp:style>
+      <dsp:txBody>
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="6985" tIns="6985" rIns="6985" bIns="6985" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr lvl="0" algn="ctr" defTabSz="488950">
+            <a:lnSpc>
+              <a:spcPct val="90000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPct val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPct val="35000"/>
+            </a:spcAft>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100" kern="1200"/>
+            <a:t>1 à 3 (Pays sous developpé . Ex: Afrique, amerique du sud ...)</a:t>
+          </a:r>
+        </a:p>
+      </dsp:txBody>
+      <dsp:txXfrm>
+        <a:off x="7979885" y="5392430"/>
+        <a:ext cx="2122986" cy="340094"/>
+      </dsp:txXfrm>
+    </dsp:sp>
+    <dsp:sp modelId="{945BE33B-F2BA-4D41-952F-BD2ECC797E1B}">
+      <dsp:nvSpPr>
+        <dsp:cNvPr id="0" name=""/>
+        <dsp:cNvSpPr/>
+      </dsp:nvSpPr>
+      <dsp:spPr>
+        <a:xfrm rot="20421473">
+          <a:off x="7085150" y="6243933"/>
+          <a:ext cx="910649" cy="16259"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst>
+            <a:path>
+              <a:moveTo>
+                <a:pt x="0" y="8129"/>
+              </a:moveTo>
+              <a:lnTo>
+                <a:pt x="910649" y="8129"/>
+              </a:lnTo>
+            </a:path>
+          </a:pathLst>
+        </a:custGeom>
+        <a:noFill/>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="dk1">
+              <a:shade val="80000"/>
+              <a:hueOff val="0"/>
+              <a:satOff val="0"/>
+              <a:lumOff val="0"/>
+              <a:alphaOff val="0"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:effectLst/>
+      </dsp:spPr>
+      <dsp:style>
+        <a:lnRef idx="2">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor"/>
+      </dsp:style>
+      <dsp:txBody>
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="12700" tIns="0" rIns="12700" bIns="0" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr lvl="0" algn="ctr" defTabSz="222250">
+            <a:lnSpc>
+              <a:spcPct val="90000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPct val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPct val="35000"/>
+            </a:spcAft>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR" sz="500" kern="1200"/>
+        </a:p>
+      </dsp:txBody>
+      <dsp:txXfrm>
+        <a:off x="7517708" y="6229296"/>
+        <a:ext cx="45532" cy="45532"/>
+      </dsp:txXfrm>
+    </dsp:sp>
+    <dsp:sp modelId="{2933335C-2338-4FCE-A89D-762E7EC82638}">
+      <dsp:nvSpPr>
+        <dsp:cNvPr id="0" name=""/>
+        <dsp:cNvSpPr/>
+      </dsp:nvSpPr>
+      <dsp:spPr>
+        <a:xfrm>
+          <a:off x="7969304" y="5903917"/>
+          <a:ext cx="2144148" cy="390181"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst>
+            <a:gd name="adj" fmla="val 10000"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:gradFill rotWithShape="0">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="lt1">
+                <a:hueOff val="0"/>
+                <a:satOff val="0"/>
+                <a:lumOff val="0"/>
+                <a:alphaOff val="0"/>
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="lt1">
+                <a:hueOff val="0"/>
+                <a:satOff val="0"/>
+                <a:lumOff val="0"/>
+                <a:alphaOff val="0"/>
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="lt1">
+                <a:hueOff val="0"/>
+                <a:satOff val="0"/>
+                <a:lumOff val="0"/>
+                <a:alphaOff val="0"/>
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="38000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+        <a:scene3d>
+          <a:camera prst="orthographicFront"/>
+          <a:lightRig rig="flat" dir="t"/>
+        </a:scene3d>
+        <a:sp3d prstMaterial="dkEdge">
+          <a:bevelT w="8200" h="38100"/>
+        </a:sp3d>
+      </dsp:spPr>
+      <dsp:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="2">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </dsp:style>
+      <dsp:txBody>
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="6985" tIns="6985" rIns="6985" bIns="6985" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr lvl="0" algn="ctr" defTabSz="488950">
+            <a:lnSpc>
+              <a:spcPct val="90000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPct val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPct val="35000"/>
+            </a:spcAft>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100" kern="1200"/>
+            <a:t>3 à 5 (Pays en voie de  developpement. Ex afrique du Sud)</a:t>
+          </a:r>
+        </a:p>
+      </dsp:txBody>
+      <dsp:txXfrm>
+        <a:off x="7980732" y="5915345"/>
+        <a:ext cx="2121292" cy="367325"/>
+      </dsp:txXfrm>
+    </dsp:sp>
+    <dsp:sp modelId="{AF0086F9-2B36-43F7-A66A-B9A0BE27A8E3}">
+      <dsp:nvSpPr>
+        <dsp:cNvPr id="0" name=""/>
+        <dsp:cNvSpPr/>
+      </dsp:nvSpPr>
+      <dsp:spPr>
+        <a:xfrm rot="985966">
+          <a:off x="7093382" y="6523465"/>
+          <a:ext cx="894184" cy="16259"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst>
+            <a:path>
+              <a:moveTo>
+                <a:pt x="0" y="8129"/>
+              </a:moveTo>
+              <a:lnTo>
+                <a:pt x="894184" y="8129"/>
+              </a:lnTo>
+            </a:path>
+          </a:pathLst>
+        </a:custGeom>
+        <a:noFill/>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="dk1">
+              <a:shade val="80000"/>
+              <a:hueOff val="0"/>
+              <a:satOff val="0"/>
+              <a:lumOff val="0"/>
+              <a:alphaOff val="0"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:effectLst/>
+      </dsp:spPr>
+      <dsp:style>
+        <a:lnRef idx="2">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor"/>
+      </dsp:style>
+      <dsp:txBody>
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="12700" tIns="0" rIns="12700" bIns="0" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr lvl="0" algn="ctr" defTabSz="222250">
+            <a:lnSpc>
+              <a:spcPct val="90000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPct val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPct val="35000"/>
+            </a:spcAft>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR" sz="500" kern="1200"/>
+        </a:p>
+      </dsp:txBody>
+      <dsp:txXfrm>
+        <a:off x="7518120" y="6509240"/>
+        <a:ext cx="44709" cy="44709"/>
+      </dsp:txXfrm>
+    </dsp:sp>
+    <dsp:sp modelId="{F7780ED9-E600-44DC-A64D-AFC229741D87}">
+      <dsp:nvSpPr>
+        <dsp:cNvPr id="0" name=""/>
+        <dsp:cNvSpPr/>
+      </dsp:nvSpPr>
+      <dsp:spPr>
+        <a:xfrm>
+          <a:off x="7969304" y="6454910"/>
+          <a:ext cx="2144148" cy="406326"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst>
+            <a:gd name="adj" fmla="val 10000"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:gradFill rotWithShape="0">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="lt1">
+                <a:hueOff val="0"/>
+                <a:satOff val="0"/>
+                <a:lumOff val="0"/>
+                <a:alphaOff val="0"/>
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="lt1">
+                <a:hueOff val="0"/>
+                <a:satOff val="0"/>
+                <a:lumOff val="0"/>
+                <a:alphaOff val="0"/>
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="lt1">
+                <a:hueOff val="0"/>
+                <a:satOff val="0"/>
+                <a:lumOff val="0"/>
+                <a:alphaOff val="0"/>
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="38000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+        <a:scene3d>
+          <a:camera prst="orthographicFront"/>
+          <a:lightRig rig="flat" dir="t"/>
+        </a:scene3d>
+        <a:sp3d prstMaterial="dkEdge">
+          <a:bevelT w="8200" h="38100"/>
+        </a:sp3d>
+      </dsp:spPr>
+      <dsp:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="2">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </dsp:style>
+      <dsp:txBody>
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="6985" tIns="6985" rIns="6985" bIns="6985" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr lvl="0" algn="ctr" defTabSz="488950">
+            <a:lnSpc>
+              <a:spcPct val="90000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPct val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPct val="35000"/>
+            </a:spcAft>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100" kern="1200"/>
+            <a:t>5 à 8 ( Pays développés. Exemple europe</a:t>
+          </a:r>
+        </a:p>
+      </dsp:txBody>
+      <dsp:txXfrm>
+        <a:off x="7981205" y="6466811"/>
+        <a:ext cx="2120346" cy="382524"/>
+      </dsp:txXfrm>
+    </dsp:sp>
+    <dsp:sp modelId="{3A4589C2-A47E-400B-85B3-7DB71B612B67}">
+      <dsp:nvSpPr>
+        <dsp:cNvPr id="0" name=""/>
+        <dsp:cNvSpPr/>
+      </dsp:nvSpPr>
+      <dsp:spPr>
+        <a:xfrm rot="2623052">
+          <a:off x="6947149" y="6807037"/>
+          <a:ext cx="1186651" cy="16259"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst>
+            <a:path>
+              <a:moveTo>
+                <a:pt x="0" y="8129"/>
+              </a:moveTo>
+              <a:lnTo>
+                <a:pt x="1186651" y="8129"/>
+              </a:lnTo>
+            </a:path>
+          </a:pathLst>
+        </a:custGeom>
+        <a:noFill/>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="dk1">
+              <a:shade val="80000"/>
+              <a:hueOff val="0"/>
+              <a:satOff val="0"/>
+              <a:lumOff val="0"/>
+              <a:alphaOff val="0"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:effectLst/>
+      </dsp:spPr>
+      <dsp:style>
+        <a:lnRef idx="2">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor"/>
+      </dsp:style>
+      <dsp:txBody>
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="12700" tIns="0" rIns="12700" bIns="0" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr lvl="0" algn="ctr" defTabSz="222250">
+            <a:lnSpc>
+              <a:spcPct val="90000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPct val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPct val="35000"/>
+            </a:spcAft>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR" sz="500" kern="1200"/>
+        </a:p>
+      </dsp:txBody>
+      <dsp:txXfrm>
+        <a:off x="7510808" y="6785500"/>
+        <a:ext cx="59332" cy="59332"/>
+      </dsp:txXfrm>
+    </dsp:sp>
+    <dsp:sp modelId="{82382562-971E-447C-94BE-1FD567D8B4CE}">
+      <dsp:nvSpPr>
+        <dsp:cNvPr id="0" name=""/>
+        <dsp:cNvSpPr/>
+      </dsp:nvSpPr>
+      <dsp:spPr>
+        <a:xfrm>
+          <a:off x="7969304" y="7022047"/>
+          <a:ext cx="2144148" cy="406337"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst>
+            <a:gd name="adj" fmla="val 10000"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:gradFill rotWithShape="0">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="lt1">
+                <a:hueOff val="0"/>
+                <a:satOff val="0"/>
+                <a:lumOff val="0"/>
+                <a:alphaOff val="0"/>
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="lt1">
+                <a:hueOff val="0"/>
+                <a:satOff val="0"/>
+                <a:lumOff val="0"/>
+                <a:alphaOff val="0"/>
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="lt1">
+                <a:hueOff val="0"/>
+                <a:satOff val="0"/>
+                <a:lumOff val="0"/>
+                <a:alphaOff val="0"/>
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="38000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+        <a:scene3d>
+          <a:camera prst="orthographicFront"/>
+          <a:lightRig rig="flat" dir="t"/>
+        </a:scene3d>
+        <a:sp3d prstMaterial="dkEdge">
+          <a:bevelT w="8200" h="38100"/>
+        </a:sp3d>
+      </dsp:spPr>
+      <dsp:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="2">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </dsp:style>
+      <dsp:txBody>
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="6985" tIns="6985" rIns="6985" bIns="6985" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr lvl="0" algn="ctr" defTabSz="488950">
+            <a:lnSpc>
+              <a:spcPct val="90000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPct val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPct val="35000"/>
+            </a:spcAft>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100" kern="1200"/>
+            <a:t>9 à 10  (Puissance économique )</a:t>
+          </a:r>
+        </a:p>
+      </dsp:txBody>
+      <dsp:txXfrm>
+        <a:off x="7981205" y="7033948"/>
+        <a:ext cx="2120346" cy="382535"/>
+      </dsp:txXfrm>
+    </dsp:sp>
+    <dsp:sp modelId="{7C99A380-E6F6-4F99-BD1F-7BBDA45513C5}">
+      <dsp:nvSpPr>
+        <dsp:cNvPr id="0" name=""/>
+        <dsp:cNvSpPr/>
+      </dsp:nvSpPr>
+      <dsp:spPr>
+        <a:xfrm rot="4421793">
+          <a:off x="949844" y="7703805"/>
+          <a:ext cx="3326692" cy="16259"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst>
+            <a:path>
+              <a:moveTo>
+                <a:pt x="0" y="8129"/>
+              </a:moveTo>
+              <a:lnTo>
+                <a:pt x="3326692" y="8129"/>
+              </a:lnTo>
+            </a:path>
+          </a:pathLst>
+        </a:custGeom>
+        <a:noFill/>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="dk1">
+              <a:shade val="60000"/>
+              <a:hueOff val="0"/>
+              <a:satOff val="0"/>
+              <a:lumOff val="0"/>
+              <a:alphaOff val="0"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:effectLst/>
+      </dsp:spPr>
+      <dsp:style>
+        <a:lnRef idx="2">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor"/>
+      </dsp:style>
+      <dsp:txBody>
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="12700" tIns="0" rIns="12700" bIns="0" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr lvl="0" algn="ctr" defTabSz="400050">
+            <a:lnSpc>
+              <a:spcPct val="90000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPct val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPct val="35000"/>
+            </a:spcAft>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR" sz="900" kern="1200"/>
+        </a:p>
+      </dsp:txBody>
+      <dsp:txXfrm>
+        <a:off x="2530022" y="7628768"/>
+        <a:ext cx="166334" cy="166334"/>
+      </dsp:txXfrm>
+    </dsp:sp>
+    <dsp:sp modelId="{0B42F808-76D1-48A4-BB9E-1FCE3B026DBC}">
+      <dsp:nvSpPr>
+        <dsp:cNvPr id="0" name=""/>
+        <dsp:cNvSpPr/>
+      </dsp:nvSpPr>
+      <dsp:spPr>
+        <a:xfrm>
+          <a:off x="3080132" y="9103126"/>
+          <a:ext cx="4020492" cy="410540"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst>
+            <a:gd name="adj" fmla="val 10000"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFF00"/>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="38000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+        <a:scene3d>
+          <a:camera prst="orthographicFront"/>
+          <a:lightRig rig="flat" dir="t"/>
+        </a:scene3d>
+        <a:sp3d prstMaterial="dkEdge">
+          <a:bevelT w="8200" h="38100"/>
+        </a:sp3d>
+      </dsp:spPr>
+      <dsp:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="2">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </dsp:style>
+      <dsp:txBody>
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="6985" tIns="6985" rIns="6985" bIns="6985" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr lvl="0" algn="ctr" defTabSz="488950">
+            <a:lnSpc>
+              <a:spcPct val="90000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPct val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPct val="35000"/>
+            </a:spcAft>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100" b="1" kern="1200"/>
+            <a:t>AXES  DE  GOUVERNANCE ( à cocher )</a:t>
+          </a:r>
+        </a:p>
+      </dsp:txBody>
+      <dsp:txXfrm>
+        <a:off x="3092156" y="9115150"/>
+        <a:ext cx="3996444" cy="386492"/>
+      </dsp:txXfrm>
+    </dsp:sp>
+    <dsp:sp modelId="{BF5A9F46-CFBF-4075-874A-B4152BE5026B}">
+      <dsp:nvSpPr>
+        <dsp:cNvPr id="0" name=""/>
+        <dsp:cNvSpPr/>
+      </dsp:nvSpPr>
+      <dsp:spPr>
+        <a:xfrm rot="33485">
+          <a:off x="7100606" y="9303996"/>
+          <a:ext cx="766054" cy="16259"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst>
+            <a:path>
+              <a:moveTo>
+                <a:pt x="0" y="8129"/>
+              </a:moveTo>
+              <a:lnTo>
+                <a:pt x="766054" y="8129"/>
+              </a:lnTo>
+            </a:path>
+          </a:pathLst>
+        </a:custGeom>
+        <a:noFill/>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="dk1">
+              <a:shade val="80000"/>
+              <a:hueOff val="0"/>
+              <a:satOff val="0"/>
+              <a:lumOff val="0"/>
+              <a:alphaOff val="0"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:effectLst/>
+      </dsp:spPr>
+      <dsp:style>
+        <a:lnRef idx="2">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor"/>
+      </dsp:style>
+      <dsp:txBody>
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="12700" tIns="0" rIns="12700" bIns="0" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr lvl="0" algn="ctr" defTabSz="222250">
+            <a:lnSpc>
+              <a:spcPct val="90000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPct val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPct val="35000"/>
+            </a:spcAft>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR" sz="500" kern="1200"/>
+        </a:p>
+      </dsp:txBody>
+      <dsp:txXfrm>
+        <a:off x="7464482" y="9292975"/>
+        <a:ext cx="38302" cy="38302"/>
+      </dsp:txXfrm>
+    </dsp:sp>
+    <dsp:sp modelId="{FFFAF596-BF24-4562-B5D6-2C39DE2E488F}">
+      <dsp:nvSpPr>
+        <dsp:cNvPr id="0" name=""/>
+        <dsp:cNvSpPr/>
+      </dsp:nvSpPr>
+      <dsp:spPr>
+        <a:xfrm>
+          <a:off x="7866642" y="8779820"/>
+          <a:ext cx="2144148" cy="1072074"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst>
+            <a:gd name="adj" fmla="val 10000"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:gradFill rotWithShape="0">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="lt1">
+                <a:hueOff val="0"/>
+                <a:satOff val="0"/>
+                <a:lumOff val="0"/>
+                <a:alphaOff val="0"/>
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="lt1">
+                <a:hueOff val="0"/>
+                <a:satOff val="0"/>
+                <a:lumOff val="0"/>
+                <a:alphaOff val="0"/>
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="lt1">
+                <a:hueOff val="0"/>
+                <a:satOff val="0"/>
+                <a:lumOff val="0"/>
+                <a:alphaOff val="0"/>
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="38000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+        <a:scene3d>
+          <a:camera prst="orthographicFront"/>
+          <a:lightRig rig="flat" dir="t"/>
+        </a:scene3d>
+        <a:sp3d prstMaterial="dkEdge">
+          <a:bevelT w="8200" h="38100"/>
+        </a:sp3d>
+      </dsp:spPr>
+      <dsp:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="2">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </dsp:style>
+      <dsp:txBody>
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="6985" tIns="6985" rIns="6985" bIns="6985" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr lvl="0" algn="ctr" defTabSz="488950">
+            <a:lnSpc>
+              <a:spcPct val="90000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPct val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPct val="35000"/>
+            </a:spcAft>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100" kern="1200"/>
+            <a:t>Economique /  Social  / Environnemental / Securité  /stratégies   Internationales  </a:t>
+          </a:r>
+        </a:p>
+      </dsp:txBody>
+      <dsp:txXfrm>
+        <a:off x="7898042" y="8811220"/>
+        <a:ext cx="2081348" cy="1009274"/>
+      </dsp:txXfrm>
+    </dsp:sp>
   </dsp:spTree>
 </dsp:drawing>
 </file>
@@ -7214,6 +10573,82 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>247649</xdr:colOff>
+          <xdr:row>28</xdr:row>
+          <xdr:rowOff>85725</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>923924</xdr:colOff>
+          <xdr:row>29</xdr:row>
+          <xdr:rowOff>133350</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="3073" name="Button 1" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s3073"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="27432" rIns="27432" bIns="27432" anchor="ctr" upright="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="ctr" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:r>
+                <a:rPr lang="fr-FR" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                  <a:solidFill>
+                    <a:srgbClr val="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="Calibri"/>
+                </a:rPr>
+                <a:t>Initialiser le jeu </a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:clientData fPrintsWithSheet="0"/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+</xdr:wsDr>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A2:C267" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="A2:C267"/>
+  <tableColumns count="3">
+    <tableColumn id="1" name="Informations Par Pays"/>
+    <tableColumn id="3" name="Catégorie"/>
+    <tableColumn id="2" name="Commentaires "/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
@@ -7503,7 +10938,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="F4:W15"/>
   <sheetViews>
-    <sheetView topLeftCell="A48" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A44" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="U55" sqref="U55"/>
     </sheetView>
   </sheetViews>
@@ -7637,11 +11072,11 @@
   </cols>
   <sheetData>
     <row r="2" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="H2" s="21" t="s">
+      <c r="H2" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="I2" s="22"/>
-      <c r="J2" s="23"/>
+      <c r="I2" s="28"/>
+      <c r="J2" s="29"/>
       <c r="L2" s="15" t="s">
         <v>10</v>
       </c>
@@ -7649,9 +11084,9 @@
       <c r="N2" s="17"/>
     </row>
     <row r="3" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="H3" s="24"/>
-      <c r="I3" s="25"/>
-      <c r="J3" s="26"/>
+      <c r="H3" s="30"/>
+      <c r="I3" s="31"/>
+      <c r="J3" s="32"/>
       <c r="L3" s="18"/>
       <c r="M3" s="19"/>
       <c r="N3" s="20"/>
@@ -7669,11 +11104,11 @@
       <c r="N5" s="17"/>
     </row>
     <row r="6" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="D6" s="27" t="s">
+      <c r="D6" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="E6" s="28"/>
-      <c r="F6" s="29"/>
+      <c r="E6" s="22"/>
+      <c r="F6" s="23"/>
       <c r="G6" s="3"/>
       <c r="H6" s="18"/>
       <c r="I6" s="19"/>
@@ -7684,9 +11119,9 @@
       <c r="N6" s="20"/>
     </row>
     <row r="7" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="D7" s="30"/>
-      <c r="E7" s="31"/>
-      <c r="F7" s="32"/>
+      <c r="D7" s="24"/>
+      <c r="E7" s="25"/>
+      <c r="F7" s="26"/>
       <c r="G7" s="3"/>
       <c r="H7" s="4"/>
       <c r="I7" s="4"/>
@@ -7697,11 +11132,11 @@
       <c r="N7" s="4"/>
     </row>
     <row r="8" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="H8" s="21" t="s">
+      <c r="H8" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="I8" s="22"/>
-      <c r="J8" s="23"/>
+      <c r="I8" s="28"/>
+      <c r="J8" s="29"/>
       <c r="L8" s="15" t="s">
         <v>2</v>
       </c>
@@ -7714,9 +11149,9 @@
       </c>
       <c r="E9" s="33"/>
       <c r="F9" s="33"/>
-      <c r="H9" s="24"/>
-      <c r="I9" s="25"/>
-      <c r="J9" s="26"/>
+      <c r="H9" s="30"/>
+      <c r="I9" s="31"/>
+      <c r="J9" s="32"/>
       <c r="L9" s="18"/>
       <c r="M9" s="19"/>
       <c r="N9" s="20"/>
@@ -7730,27 +11165,27 @@
       <c r="D11" s="34"/>
       <c r="E11" s="34"/>
       <c r="F11" s="34"/>
-      <c r="H11" s="21" t="s">
+      <c r="H11" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="I11" s="22"/>
-      <c r="J11" s="23"/>
-      <c r="L11" s="21" t="s">
+      <c r="I11" s="28"/>
+      <c r="J11" s="29"/>
+      <c r="L11" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="M11" s="22"/>
-      <c r="N11" s="23"/>
+      <c r="M11" s="28"/>
+      <c r="N11" s="29"/>
     </row>
     <row r="12" spans="4:14" x14ac:dyDescent="0.25">
       <c r="D12" s="34"/>
       <c r="E12" s="34"/>
       <c r="F12" s="34"/>
-      <c r="H12" s="24"/>
-      <c r="I12" s="25"/>
-      <c r="J12" s="26"/>
-      <c r="L12" s="24"/>
-      <c r="M12" s="25"/>
-      <c r="N12" s="26"/>
+      <c r="H12" s="30"/>
+      <c r="I12" s="31"/>
+      <c r="J12" s="32"/>
+      <c r="L12" s="30"/>
+      <c r="M12" s="31"/>
+      <c r="N12" s="32"/>
     </row>
     <row r="13" spans="4:14" x14ac:dyDescent="0.25">
       <c r="D13" s="34"/>
@@ -7792,11 +11227,11 @@
       <c r="D17" s="34"/>
       <c r="E17" s="34"/>
       <c r="F17" s="34"/>
-      <c r="H17" s="21" t="s">
+      <c r="H17" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="I17" s="22"/>
-      <c r="J17" s="23"/>
+      <c r="I17" s="28"/>
+      <c r="J17" s="29"/>
       <c r="L17" s="15" t="s">
         <v>14</v>
       </c>
@@ -7804,19 +11239,19 @@
       <c r="N17" s="17"/>
     </row>
     <row r="18" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="H18" s="24"/>
-      <c r="I18" s="25"/>
-      <c r="J18" s="26"/>
+      <c r="H18" s="30"/>
+      <c r="I18" s="31"/>
+      <c r="J18" s="32"/>
       <c r="L18" s="18"/>
       <c r="M18" s="19"/>
       <c r="N18" s="20"/>
     </row>
     <row r="20" spans="4:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H20" s="21" t="s">
+      <c r="H20" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="I20" s="22"/>
-      <c r="J20" s="23"/>
+      <c r="I20" s="28"/>
+      <c r="J20" s="29"/>
       <c r="L20" s="15" t="s">
         <v>28</v>
       </c>
@@ -7824,9 +11259,9 @@
       <c r="N20" s="17"/>
     </row>
     <row r="21" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="H21" s="24"/>
-      <c r="I21" s="25"/>
-      <c r="J21" s="26"/>
+      <c r="H21" s="30"/>
+      <c r="I21" s="31"/>
+      <c r="J21" s="32"/>
       <c r="L21" s="18"/>
       <c r="M21" s="19"/>
       <c r="N21" s="20"/>
@@ -7925,6 +11360,18 @@
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="H35:J36"/>
+    <mergeCell ref="L20:N21"/>
+    <mergeCell ref="L17:N18"/>
+    <mergeCell ref="L23:N24"/>
+    <mergeCell ref="L26:N27"/>
+    <mergeCell ref="L29:N30"/>
+    <mergeCell ref="L32:N33"/>
+    <mergeCell ref="H26:J27"/>
+    <mergeCell ref="H29:J30"/>
+    <mergeCell ref="H32:J33"/>
+    <mergeCell ref="H23:J24"/>
+    <mergeCell ref="H20:J21"/>
     <mergeCell ref="L14:N15"/>
     <mergeCell ref="D6:F7"/>
     <mergeCell ref="H2:J3"/>
@@ -7938,18 +11385,6 @@
     <mergeCell ref="L5:N6"/>
     <mergeCell ref="L8:N9"/>
     <mergeCell ref="L11:N12"/>
-    <mergeCell ref="H35:J36"/>
-    <mergeCell ref="L20:N21"/>
-    <mergeCell ref="L17:N18"/>
-    <mergeCell ref="L23:N24"/>
-    <mergeCell ref="L26:N27"/>
-    <mergeCell ref="L29:N30"/>
-    <mergeCell ref="L32:N33"/>
-    <mergeCell ref="H26:J27"/>
-    <mergeCell ref="H29:J30"/>
-    <mergeCell ref="H32:J33"/>
-    <mergeCell ref="H23:J24"/>
-    <mergeCell ref="H20:J21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -8206,7 +11641,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:L22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
@@ -8747,4 +12182,699 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:V31"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.7109375" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="37" t="s">
+        <v>73</v>
+      </c>
+      <c r="E3" s="37" t="s">
+        <v>74</v>
+      </c>
+      <c r="H3" s="37" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B4" s="38" t="s">
+        <v>71</v>
+      </c>
+      <c r="H4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B5" s="38" t="s">
+        <v>72</v>
+      </c>
+      <c r="H5" t="s">
+        <v>77</v>
+      </c>
+      <c r="K5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="39" t="s">
+        <v>45</v>
+      </c>
+      <c r="H6" s="36" t="s">
+        <v>78</v>
+      </c>
+      <c r="I6" s="36" t="s">
+        <v>76</v>
+      </c>
+      <c r="J6" s="36" t="s">
+        <v>80</v>
+      </c>
+      <c r="K6" s="36" t="s">
+        <v>81</v>
+      </c>
+      <c r="L6" s="36" t="s">
+        <v>82</v>
+      </c>
+      <c r="M6" s="36"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="H7" t="str">
+        <f>B23</f>
+        <v>zone 1</v>
+      </c>
+      <c r="I7">
+        <f>B24</f>
+        <v>192722</v>
+      </c>
+      <c r="J7" t="str">
+        <f>B25</f>
+        <v>13 M</v>
+      </c>
+      <c r="K7" t="str">
+        <f>B27</f>
+        <v>libérale</v>
+      </c>
+      <c r="L7">
+        <f>B26</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="40"/>
+      <c r="B10" s="40"/>
+      <c r="C10" s="40"/>
+      <c r="D10" s="40"/>
+    </row>
+    <row r="11" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="40" t="s">
+        <v>83</v>
+      </c>
+      <c r="B11" s="41"/>
+      <c r="C11" s="40"/>
+      <c r="D11" s="42"/>
+    </row>
+    <row r="12" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="40"/>
+      <c r="B12" s="40"/>
+      <c r="C12" s="40"/>
+      <c r="D12" s="43"/>
+    </row>
+    <row r="13" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="40" t="s">
+        <v>72</v>
+      </c>
+      <c r="B13" s="41"/>
+      <c r="C13" s="40"/>
+      <c r="D13" s="44"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" s="40"/>
+      <c r="B14" s="40"/>
+      <c r="C14" s="40"/>
+      <c r="D14" s="40"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" s="40"/>
+      <c r="B15" s="40"/>
+      <c r="C15" s="40"/>
+      <c r="D15" s="40"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" s="40"/>
+      <c r="B16" s="40"/>
+      <c r="C16" s="40"/>
+      <c r="D16" s="40"/>
+    </row>
+    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="21" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="40"/>
+      <c r="B21" s="40"/>
+      <c r="C21" s="40"/>
+      <c r="D21" s="40"/>
+      <c r="E21" s="40"/>
+    </row>
+    <row r="22" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="40" t="s">
+        <v>86</v>
+      </c>
+      <c r="B22" s="41"/>
+      <c r="C22" s="40"/>
+      <c r="D22" s="40"/>
+      <c r="E22" s="40"/>
+    </row>
+    <row r="23" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="40" t="s">
+        <v>87</v>
+      </c>
+      <c r="B23" s="45" t="s">
+        <v>93</v>
+      </c>
+      <c r="C23" s="40"/>
+      <c r="D23" s="40"/>
+      <c r="E23" s="40"/>
+      <c r="V23" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="24" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="40" t="s">
+        <v>76</v>
+      </c>
+      <c r="B24" s="46">
+        <v>192722</v>
+      </c>
+      <c r="C24" s="40"/>
+      <c r="D24" s="40"/>
+      <c r="E24" s="40"/>
+      <c r="V24" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="25" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="40" t="s">
+        <v>80</v>
+      </c>
+      <c r="B25" s="45" t="s">
+        <v>94</v>
+      </c>
+      <c r="C25" s="40"/>
+      <c r="D25" s="40"/>
+      <c r="E25" s="40"/>
+      <c r="V25" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="26" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="40" t="s">
+        <v>88</v>
+      </c>
+      <c r="B26" s="45">
+        <v>2</v>
+      </c>
+      <c r="C26" s="40"/>
+      <c r="D26" s="40"/>
+      <c r="E26" s="40"/>
+    </row>
+    <row r="27" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="40" t="s">
+        <v>92</v>
+      </c>
+      <c r="B27" s="45" t="s">
+        <v>95</v>
+      </c>
+      <c r="C27" s="40"/>
+      <c r="D27" s="40"/>
+      <c r="E27" s="40"/>
+    </row>
+    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A28" s="40"/>
+      <c r="B28" s="40"/>
+      <c r="C28" s="40"/>
+      <c r="D28" s="40"/>
+      <c r="E28" s="40"/>
+    </row>
+    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A29" s="40"/>
+      <c r="B29" s="40"/>
+      <c r="C29" s="40"/>
+      <c r="D29" s="40"/>
+      <c r="E29" s="40"/>
+    </row>
+    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A30" s="40"/>
+      <c r="B30" s="40"/>
+      <c r="C30" s="40"/>
+      <c r="D30" s="40"/>
+      <c r="E30" s="40"/>
+    </row>
+    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A31" s="40"/>
+      <c r="B31" s="40"/>
+      <c r="C31" s="40"/>
+      <c r="D31" s="40"/>
+      <c r="E31" s="40"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="D11:D13"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x14">
+      <controls>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="3073" r:id="rId4" name="Button 1">
+              <controlPr defaultSize="0" print="0" autoFill="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>3</xdr:col>
+                    <xdr:colOff>247650</xdr:colOff>
+                    <xdr:row>28</xdr:row>
+                    <xdr:rowOff>85725</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>4</xdr:col>
+                    <xdr:colOff>923925</xdr:colOff>
+                    <xdr:row>29</xdr:row>
+                    <xdr:rowOff>133350</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+      </controls>
+    </mc:Choice>
+  </mc:AlternateContent>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:H42"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="B44" sqref="B44"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="51.7109375" customWidth="1"/>
+    <col min="3" max="3" width="48.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="36" t="s">
+        <v>96</v>
+      </c>
+      <c r="B2" s="36" t="s">
+        <v>133</v>
+      </c>
+      <c r="C2" s="36" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="47" t="s">
+        <v>98</v>
+      </c>
+      <c r="B3" s="47" t="s">
+        <v>138</v>
+      </c>
+      <c r="C3" s="36"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>99</v>
+      </c>
+      <c r="B4" s="47" t="s">
+        <v>145</v>
+      </c>
+      <c r="H4" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>100</v>
+      </c>
+      <c r="B5" s="47" t="s">
+        <v>145</v>
+      </c>
+      <c r="H5" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>81</v>
+      </c>
+      <c r="B6" s="47" t="s">
+        <v>138</v>
+      </c>
+      <c r="H6" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>101</v>
+      </c>
+      <c r="B7" s="47" t="s">
+        <v>136</v>
+      </c>
+      <c r="H7" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>102</v>
+      </c>
+      <c r="B8" s="47" t="s">
+        <v>145</v>
+      </c>
+      <c r="H8" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>103</v>
+      </c>
+      <c r="B9" s="47" t="s">
+        <v>137</v>
+      </c>
+      <c r="H9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>104</v>
+      </c>
+      <c r="B10" s="47" t="s">
+        <v>134</v>
+      </c>
+      <c r="H10" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>105</v>
+      </c>
+      <c r="B11" s="47" t="s">
+        <v>134</v>
+      </c>
+      <c r="H11" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>106</v>
+      </c>
+      <c r="B12" s="47" t="s">
+        <v>138</v>
+      </c>
+      <c r="H12" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>107</v>
+      </c>
+      <c r="B13" s="47" t="s">
+        <v>138</v>
+      </c>
+      <c r="H13" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>108</v>
+      </c>
+      <c r="B14" s="47" t="s">
+        <v>138</v>
+      </c>
+      <c r="H14" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>109</v>
+      </c>
+      <c r="B15" s="47" t="s">
+        <v>134</v>
+      </c>
+      <c r="C15" t="s">
+        <v>110</v>
+      </c>
+      <c r="H15" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>111</v>
+      </c>
+      <c r="B16" s="47" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>112</v>
+      </c>
+      <c r="B17" s="47" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>113</v>
+      </c>
+      <c r="B18" s="47" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>114</v>
+      </c>
+      <c r="B19" s="47" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>115</v>
+      </c>
+      <c r="B20" s="47" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>116</v>
+      </c>
+      <c r="B21" s="47" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>117</v>
+      </c>
+      <c r="B22" s="47" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>118</v>
+      </c>
+      <c r="B23" s="47" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>119</v>
+      </c>
+      <c r="B24" s="47" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>120</v>
+      </c>
+      <c r="B25" s="47" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>121</v>
+      </c>
+      <c r="B26" s="47" t="s">
+        <v>137</v>
+      </c>
+      <c r="C26" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>122</v>
+      </c>
+      <c r="B27" s="47" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>123</v>
+      </c>
+      <c r="B28" s="47" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>124</v>
+      </c>
+      <c r="B29" s="47" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>125</v>
+      </c>
+      <c r="B30" s="47" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>126</v>
+      </c>
+      <c r="B31" s="47" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>127</v>
+      </c>
+      <c r="B32" s="47" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>128</v>
+      </c>
+      <c r="B33" s="47" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>129</v>
+      </c>
+      <c r="B34" s="47" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>130</v>
+      </c>
+      <c r="B35" s="47" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>131</v>
+      </c>
+      <c r="B36" s="47" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>132</v>
+      </c>
+      <c r="B37" s="47" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>139</v>
+      </c>
+      <c r="B38" s="47" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>140</v>
+      </c>
+      <c r="B39" s="47" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>141</v>
+      </c>
+      <c r="B40" s="47" t="s">
+        <v>137</v>
+      </c>
+      <c r="C40" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>144</v>
+      </c>
+      <c r="B41" s="47" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>150</v>
+      </c>
+      <c r="B42" s="47" t="s">
+        <v>134</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3:B42">
+      <formula1>Categorie_Liste</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add Senegal tab Information
</commit_message>
<xml_diff>
--- a/President game.xlsx
+++ b/President game.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950" firstSheet="2" activeTab="7"/>
+    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950" firstSheet="2" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Lancement du jeu" sheetId="1" r:id="rId1"/>
@@ -15,6 +15,7 @@
     <sheet name="Recueil informations" sheetId="6" r:id="rId6"/>
     <sheet name="Africa " sheetId="7" r:id="rId7"/>
     <sheet name="Benin" sheetId="8" r:id="rId8"/>
+    <sheet name="Senegal" sheetId="9" r:id="rId9"/>
   </sheets>
   <definedNames>
     <definedName name="Categorie_Liste">'Africa '!$H$4:$H$23</definedName>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="495" uniqueCount="201">
   <si>
     <t>Nombres de postes ministeriels</t>
   </si>
@@ -560,6 +561,75 @@
   </si>
   <si>
     <t>A quantifier</t>
+  </si>
+  <si>
+    <t>informations</t>
+  </si>
+  <si>
+    <t>Sénégal</t>
+  </si>
+  <si>
+    <t>présidentiel  (suffrage direct)</t>
+  </si>
+  <si>
+    <t>CFA</t>
+  </si>
+  <si>
+    <t>Wolof, Pular, Sérère, Diola, Maninké</t>
+  </si>
+  <si>
+    <t>Mauritanie (Nord), Mali (Est) , Guinée Conakry (Sud) Guinnée Bissau (Sud), Gambie ( Enclave)</t>
+  </si>
+  <si>
+    <t>Oui</t>
+  </si>
+  <si>
+    <t>img</t>
+  </si>
+  <si>
+    <t>Un peuple, un But, une Foi</t>
+  </si>
+  <si>
+    <t>Baobab, Lion</t>
+  </si>
+  <si>
+    <t>Régions ( 14), 45 départements</t>
+  </si>
+  <si>
+    <t>Or, Phasphate, Fer, Ressources maritimes</t>
+  </si>
+  <si>
+    <t>Dakar</t>
+  </si>
+  <si>
+    <t>Tropicale</t>
+  </si>
+  <si>
+    <t>Foot (3)  Basket (4), Athletisme (1), Lutte (5)</t>
+  </si>
+  <si>
+    <t>Leopold Sedar S, Abdou Diouf, Abdoulaye Wade, Macky Sall, Youssou Ndour</t>
+  </si>
+  <si>
+    <t>Paludisme, Choléra</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gorée, Monument de la renaissance, </t>
+  </si>
+  <si>
+    <t>CEDEAO, UEMOA, UA, ANOCI, ONU ( et branches)</t>
+  </si>
+  <si>
+    <t>adultes (50%)  Primaires (79%)</t>
+  </si>
+  <si>
+    <t>UCAD, UGB, Thies, Bambey, Zinguinchor</t>
+  </si>
+  <si>
+    <t>Grève enseignants ( depuis 2012 ), mendicité, transport urbain</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Islam (94%)  Chistianisme </t>
   </si>
 </sst>
 </file>
@@ -802,7 +872,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -833,6 +903,7 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="9" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -857,6 +928,24 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -873,24 +962,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -911,12 +982,31 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="3">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -7748,7 +7838,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A2:C267" totalsRowShown="0" headerRowDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A2:C267" totalsRowShown="0" headerRowDxfId="2">
   <autoFilter ref="A2:C267"/>
   <tableColumns count="3">
     <tableColumn id="1" name="Informations Par Pays"/>
@@ -7760,13 +7850,26 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tableau13" displayName="Tableau13" ref="A2:D267" totalsRowShown="0" headerRowDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tableau13" displayName="Tableau13" ref="A2:D267" totalsRowShown="0" headerRowDxfId="1">
   <autoFilter ref="A2:D267"/>
   <tableColumns count="4">
     <tableColumn id="1" name="Informations Par Pays"/>
     <tableColumn id="3" name="Catégorie"/>
     <tableColumn id="2" name="Commentaires "/>
     <tableColumn id="4" name="Informations"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tableau14" displayName="Tableau14" ref="A2:D267" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="A2:D267"/>
+  <tableColumns count="4">
+    <tableColumn id="1" name="Informations Par Pays"/>
+    <tableColumn id="3" name="Catégorie"/>
+    <tableColumn id="4" name="Commentaires "/>
+    <tableColumn id="2" name="informations"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -8081,91 +8184,91 @@
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
-      <c r="Q5" s="22" t="s">
+      <c r="Q5" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="R5" s="22"/>
-      <c r="S5" s="22"/>
-      <c r="T5" s="22"/>
-      <c r="U5" s="22"/>
-      <c r="V5" s="22"/>
-      <c r="W5" s="22"/>
+      <c r="R5" s="23"/>
+      <c r="S5" s="23"/>
+      <c r="T5" s="23"/>
+      <c r="U5" s="23"/>
+      <c r="V5" s="23"/>
+      <c r="W5" s="23"/>
     </row>
     <row r="6" spans="6:23" x14ac:dyDescent="0.25">
-      <c r="Q6" s="22"/>
-      <c r="R6" s="22"/>
-      <c r="S6" s="22"/>
-      <c r="T6" s="22"/>
-      <c r="U6" s="22"/>
-      <c r="V6" s="22"/>
-      <c r="W6" s="22"/>
+      <c r="Q6" s="23"/>
+      <c r="R6" s="23"/>
+      <c r="S6" s="23"/>
+      <c r="T6" s="23"/>
+      <c r="U6" s="23"/>
+      <c r="V6" s="23"/>
+      <c r="W6" s="23"/>
     </row>
     <row r="7" spans="6:23" x14ac:dyDescent="0.25">
-      <c r="Q7" s="22"/>
-      <c r="R7" s="22"/>
-      <c r="S7" s="22"/>
-      <c r="T7" s="22"/>
-      <c r="U7" s="22"/>
-      <c r="V7" s="22"/>
-      <c r="W7" s="22"/>
+      <c r="Q7" s="23"/>
+      <c r="R7" s="23"/>
+      <c r="S7" s="23"/>
+      <c r="T7" s="23"/>
+      <c r="U7" s="23"/>
+      <c r="V7" s="23"/>
+      <c r="W7" s="23"/>
     </row>
     <row r="9" spans="6:23" x14ac:dyDescent="0.25">
-      <c r="Q9" s="22" t="s">
+      <c r="Q9" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="R9" s="22"/>
-      <c r="S9" s="22"/>
-      <c r="T9" s="22"/>
-      <c r="U9" s="22"/>
-      <c r="V9" s="22"/>
-      <c r="W9" s="22"/>
+      <c r="R9" s="23"/>
+      <c r="S9" s="23"/>
+      <c r="T9" s="23"/>
+      <c r="U9" s="23"/>
+      <c r="V9" s="23"/>
+      <c r="W9" s="23"/>
     </row>
     <row r="10" spans="6:23" x14ac:dyDescent="0.25">
-      <c r="Q10" s="22"/>
-      <c r="R10" s="22"/>
-      <c r="S10" s="22"/>
-      <c r="T10" s="22"/>
-      <c r="U10" s="22"/>
-      <c r="V10" s="22"/>
-      <c r="W10" s="22"/>
+      <c r="Q10" s="23"/>
+      <c r="R10" s="23"/>
+      <c r="S10" s="23"/>
+      <c r="T10" s="23"/>
+      <c r="U10" s="23"/>
+      <c r="V10" s="23"/>
+      <c r="W10" s="23"/>
     </row>
     <row r="11" spans="6:23" x14ac:dyDescent="0.25">
-      <c r="Q11" s="22"/>
-      <c r="R11" s="22"/>
-      <c r="S11" s="22"/>
-      <c r="T11" s="22"/>
-      <c r="U11" s="22"/>
-      <c r="V11" s="22"/>
-      <c r="W11" s="22"/>
+      <c r="Q11" s="23"/>
+      <c r="R11" s="23"/>
+      <c r="S11" s="23"/>
+      <c r="T11" s="23"/>
+      <c r="U11" s="23"/>
+      <c r="V11" s="23"/>
+      <c r="W11" s="23"/>
     </row>
     <row r="13" spans="6:23" x14ac:dyDescent="0.25">
-      <c r="Q13" s="23" t="s">
+      <c r="Q13" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="R13" s="23"/>
-      <c r="S13" s="23"/>
-      <c r="T13" s="23"/>
-      <c r="U13" s="23"/>
-      <c r="V13" s="23"/>
-      <c r="W13" s="23"/>
+      <c r="R13" s="24"/>
+      <c r="S13" s="24"/>
+      <c r="T13" s="24"/>
+      <c r="U13" s="24"/>
+      <c r="V13" s="24"/>
+      <c r="W13" s="24"/>
     </row>
     <row r="14" spans="6:23" x14ac:dyDescent="0.25">
-      <c r="Q14" s="23"/>
-      <c r="R14" s="23"/>
-      <c r="S14" s="23"/>
-      <c r="T14" s="23"/>
-      <c r="U14" s="23"/>
-      <c r="V14" s="23"/>
-      <c r="W14" s="23"/>
+      <c r="Q14" s="24"/>
+      <c r="R14" s="24"/>
+      <c r="S14" s="24"/>
+      <c r="T14" s="24"/>
+      <c r="U14" s="24"/>
+      <c r="V14" s="24"/>
+      <c r="W14" s="24"/>
     </row>
     <row r="15" spans="6:23" x14ac:dyDescent="0.25">
-      <c r="Q15" s="23"/>
-      <c r="R15" s="23"/>
-      <c r="S15" s="23"/>
-      <c r="T15" s="23"/>
-      <c r="U15" s="23"/>
-      <c r="V15" s="23"/>
-      <c r="W15" s="23"/>
+      <c r="Q15" s="24"/>
+      <c r="R15" s="24"/>
+      <c r="S15" s="24"/>
+      <c r="T15" s="24"/>
+      <c r="U15" s="24"/>
+      <c r="V15" s="24"/>
+      <c r="W15" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -8195,56 +8298,56 @@
   </cols>
   <sheetData>
     <row r="2" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="H2" s="30" t="s">
+      <c r="H2" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="I2" s="31"/>
-      <c r="J2" s="32"/>
-      <c r="L2" s="24" t="s">
+      <c r="I2" s="38"/>
+      <c r="J2" s="39"/>
+      <c r="L2" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="M2" s="25"/>
-      <c r="N2" s="26"/>
+      <c r="M2" s="26"/>
+      <c r="N2" s="27"/>
     </row>
     <row r="3" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="H3" s="33"/>
-      <c r="I3" s="34"/>
-      <c r="J3" s="35"/>
-      <c r="L3" s="27"/>
-      <c r="M3" s="28"/>
-      <c r="N3" s="29"/>
+      <c r="H3" s="40"/>
+      <c r="I3" s="41"/>
+      <c r="J3" s="42"/>
+      <c r="L3" s="28"/>
+      <c r="M3" s="29"/>
+      <c r="N3" s="30"/>
     </row>
     <row r="5" spans="4:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H5" s="24" t="s">
+      <c r="H5" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="I5" s="25"/>
-      <c r="J5" s="26"/>
-      <c r="L5" s="24" t="s">
+      <c r="I5" s="26"/>
+      <c r="J5" s="27"/>
+      <c r="L5" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="M5" s="25"/>
-      <c r="N5" s="26"/>
+      <c r="M5" s="26"/>
+      <c r="N5" s="27"/>
     </row>
     <row r="6" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="D6" s="36" t="s">
+      <c r="D6" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="E6" s="37"/>
-      <c r="F6" s="38"/>
+      <c r="E6" s="32"/>
+      <c r="F6" s="33"/>
       <c r="G6" s="3"/>
-      <c r="H6" s="27"/>
-      <c r="I6" s="28"/>
-      <c r="J6" s="29"/>
+      <c r="H6" s="28"/>
+      <c r="I6" s="29"/>
+      <c r="J6" s="30"/>
       <c r="K6" s="4"/>
-      <c r="L6" s="27"/>
-      <c r="M6" s="28"/>
-      <c r="N6" s="29"/>
+      <c r="L6" s="28"/>
+      <c r="M6" s="29"/>
+      <c r="N6" s="30"/>
     </row>
     <row r="7" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="D7" s="39"/>
-      <c r="E7" s="40"/>
-      <c r="F7" s="41"/>
+      <c r="D7" s="34"/>
+      <c r="E7" s="35"/>
+      <c r="F7" s="36"/>
       <c r="G7" s="3"/>
       <c r="H7" s="4"/>
       <c r="I7" s="4"/>
@@ -8255,234 +8358,246 @@
       <c r="N7" s="4"/>
     </row>
     <row r="8" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="H8" s="30" t="s">
+      <c r="H8" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="I8" s="31"/>
-      <c r="J8" s="32"/>
-      <c r="L8" s="24" t="s">
+      <c r="I8" s="38"/>
+      <c r="J8" s="39"/>
+      <c r="L8" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="M8" s="25"/>
-      <c r="N8" s="26"/>
+      <c r="M8" s="26"/>
+      <c r="N8" s="27"/>
     </row>
     <row r="9" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="D9" s="42" t="s">
+      <c r="D9" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="E9" s="42"/>
-      <c r="F9" s="42"/>
-      <c r="H9" s="33"/>
-      <c r="I9" s="34"/>
-      <c r="J9" s="35"/>
-      <c r="L9" s="27"/>
-      <c r="M9" s="28"/>
-      <c r="N9" s="29"/>
+      <c r="E9" s="43"/>
+      <c r="F9" s="43"/>
+      <c r="H9" s="40"/>
+      <c r="I9" s="41"/>
+      <c r="J9" s="42"/>
+      <c r="L9" s="28"/>
+      <c r="M9" s="29"/>
+      <c r="N9" s="30"/>
     </row>
     <row r="10" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="D10" s="43"/>
-      <c r="E10" s="43"/>
-      <c r="F10" s="43"/>
+      <c r="D10" s="44"/>
+      <c r="E10" s="44"/>
+      <c r="F10" s="44"/>
     </row>
     <row r="11" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="D11" s="43"/>
-      <c r="E11" s="43"/>
-      <c r="F11" s="43"/>
-      <c r="H11" s="30" t="s">
+      <c r="D11" s="44"/>
+      <c r="E11" s="44"/>
+      <c r="F11" s="44"/>
+      <c r="H11" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="I11" s="31"/>
-      <c r="J11" s="32"/>
-      <c r="L11" s="30" t="s">
+      <c r="I11" s="38"/>
+      <c r="J11" s="39"/>
+      <c r="L11" s="37" t="s">
         <v>18</v>
       </c>
-      <c r="M11" s="31"/>
-      <c r="N11" s="32"/>
+      <c r="M11" s="38"/>
+      <c r="N11" s="39"/>
     </row>
     <row r="12" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="D12" s="43"/>
-      <c r="E12" s="43"/>
-      <c r="F12" s="43"/>
-      <c r="H12" s="33"/>
-      <c r="I12" s="34"/>
-      <c r="J12" s="35"/>
-      <c r="L12" s="33"/>
-      <c r="M12" s="34"/>
-      <c r="N12" s="35"/>
+      <c r="D12" s="44"/>
+      <c r="E12" s="44"/>
+      <c r="F12" s="44"/>
+      <c r="H12" s="40"/>
+      <c r="I12" s="41"/>
+      <c r="J12" s="42"/>
+      <c r="L12" s="40"/>
+      <c r="M12" s="41"/>
+      <c r="N12" s="42"/>
     </row>
     <row r="13" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="D13" s="43"/>
-      <c r="E13" s="43"/>
-      <c r="F13" s="43"/>
+      <c r="D13" s="44"/>
+      <c r="E13" s="44"/>
+      <c r="F13" s="44"/>
     </row>
     <row r="14" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="D14" s="43"/>
-      <c r="E14" s="43"/>
-      <c r="F14" s="43"/>
-      <c r="H14" s="24" t="s">
+      <c r="D14" s="44"/>
+      <c r="E14" s="44"/>
+      <c r="F14" s="44"/>
+      <c r="H14" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="I14" s="25"/>
-      <c r="J14" s="26"/>
-      <c r="L14" s="24" t="s">
+      <c r="I14" s="26"/>
+      <c r="J14" s="27"/>
+      <c r="L14" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="M14" s="25"/>
-      <c r="N14" s="26"/>
+      <c r="M14" s="26"/>
+      <c r="N14" s="27"/>
     </row>
     <row r="15" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="D15" s="43"/>
-      <c r="E15" s="43"/>
-      <c r="F15" s="43"/>
-      <c r="H15" s="27"/>
-      <c r="I15" s="28"/>
-      <c r="J15" s="29"/>
-      <c r="L15" s="27"/>
-      <c r="M15" s="28"/>
-      <c r="N15" s="29"/>
+      <c r="D15" s="44"/>
+      <c r="E15" s="44"/>
+      <c r="F15" s="44"/>
+      <c r="H15" s="28"/>
+      <c r="I15" s="29"/>
+      <c r="J15" s="30"/>
+      <c r="L15" s="28"/>
+      <c r="M15" s="29"/>
+      <c r="N15" s="30"/>
     </row>
     <row r="16" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="D16" s="43"/>
-      <c r="E16" s="43"/>
-      <c r="F16" s="43"/>
+      <c r="D16" s="44"/>
+      <c r="E16" s="44"/>
+      <c r="F16" s="44"/>
     </row>
     <row r="17" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="D17" s="43"/>
-      <c r="E17" s="43"/>
-      <c r="F17" s="43"/>
-      <c r="H17" s="30" t="s">
+      <c r="D17" s="44"/>
+      <c r="E17" s="44"/>
+      <c r="F17" s="44"/>
+      <c r="H17" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="I17" s="31"/>
-      <c r="J17" s="32"/>
-      <c r="L17" s="24" t="s">
+      <c r="I17" s="38"/>
+      <c r="J17" s="39"/>
+      <c r="L17" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="M17" s="25"/>
-      <c r="N17" s="26"/>
+      <c r="M17" s="26"/>
+      <c r="N17" s="27"/>
     </row>
     <row r="18" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="H18" s="33"/>
-      <c r="I18" s="34"/>
-      <c r="J18" s="35"/>
-      <c r="L18" s="27"/>
-      <c r="M18" s="28"/>
-      <c r="N18" s="29"/>
+      <c r="H18" s="40"/>
+      <c r="I18" s="41"/>
+      <c r="J18" s="42"/>
+      <c r="L18" s="28"/>
+      <c r="M18" s="29"/>
+      <c r="N18" s="30"/>
     </row>
     <row r="20" spans="4:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H20" s="30" t="s">
+      <c r="H20" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="I20" s="31"/>
-      <c r="J20" s="32"/>
-      <c r="L20" s="24" t="s">
+      <c r="I20" s="38"/>
+      <c r="J20" s="39"/>
+      <c r="L20" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="M20" s="25"/>
-      <c r="N20" s="26"/>
+      <c r="M20" s="26"/>
+      <c r="N20" s="27"/>
     </row>
     <row r="21" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="H21" s="33"/>
-      <c r="I21" s="34"/>
-      <c r="J21" s="35"/>
-      <c r="L21" s="27"/>
-      <c r="M21" s="28"/>
-      <c r="N21" s="29"/>
+      <c r="H21" s="40"/>
+      <c r="I21" s="41"/>
+      <c r="J21" s="42"/>
+      <c r="L21" s="28"/>
+      <c r="M21" s="29"/>
+      <c r="N21" s="30"/>
     </row>
     <row r="23" spans="4:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H23" s="24" t="s">
+      <c r="H23" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="I23" s="25"/>
-      <c r="J23" s="26"/>
-      <c r="L23" s="24" t="s">
+      <c r="I23" s="26"/>
+      <c r="J23" s="27"/>
+      <c r="L23" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="M23" s="25"/>
-      <c r="N23" s="26"/>
+      <c r="M23" s="26"/>
+      <c r="N23" s="27"/>
     </row>
     <row r="24" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="H24" s="27"/>
-      <c r="I24" s="28"/>
-      <c r="J24" s="29"/>
-      <c r="L24" s="27"/>
-      <c r="M24" s="28"/>
-      <c r="N24" s="29"/>
+      <c r="H24" s="28"/>
+      <c r="I24" s="29"/>
+      <c r="J24" s="30"/>
+      <c r="L24" s="28"/>
+      <c r="M24" s="29"/>
+      <c r="N24" s="30"/>
     </row>
     <row r="26" spans="4:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H26" s="24" t="s">
+      <c r="H26" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="I26" s="25"/>
-      <c r="J26" s="26"/>
-      <c r="L26" s="24" t="s">
+      <c r="I26" s="26"/>
+      <c r="J26" s="27"/>
+      <c r="L26" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="M26" s="25"/>
-      <c r="N26" s="26"/>
+      <c r="M26" s="26"/>
+      <c r="N26" s="27"/>
     </row>
     <row r="27" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="H27" s="27"/>
-      <c r="I27" s="28"/>
-      <c r="J27" s="29"/>
-      <c r="L27" s="27"/>
-      <c r="M27" s="28"/>
-      <c r="N27" s="29"/>
+      <c r="H27" s="28"/>
+      <c r="I27" s="29"/>
+      <c r="J27" s="30"/>
+      <c r="L27" s="28"/>
+      <c r="M27" s="29"/>
+      <c r="N27" s="30"/>
     </row>
     <row r="29" spans="4:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H29" s="24" t="s">
+      <c r="H29" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="I29" s="25"/>
-      <c r="J29" s="26"/>
-      <c r="L29" s="24" t="s">
+      <c r="I29" s="26"/>
+      <c r="J29" s="27"/>
+      <c r="L29" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="M29" s="25"/>
-      <c r="N29" s="26"/>
+      <c r="M29" s="26"/>
+      <c r="N29" s="27"/>
     </row>
     <row r="30" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="H30" s="27"/>
-      <c r="I30" s="28"/>
-      <c r="J30" s="29"/>
-      <c r="L30" s="27"/>
-      <c r="M30" s="28"/>
-      <c r="N30" s="29"/>
+      <c r="H30" s="28"/>
+      <c r="I30" s="29"/>
+      <c r="J30" s="30"/>
+      <c r="L30" s="28"/>
+      <c r="M30" s="29"/>
+      <c r="N30" s="30"/>
     </row>
     <row r="32" spans="4:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H32" s="24" t="s">
+      <c r="H32" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="I32" s="25"/>
-      <c r="J32" s="26"/>
-      <c r="L32" s="24" t="s">
+      <c r="I32" s="26"/>
+      <c r="J32" s="27"/>
+      <c r="L32" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="M32" s="25"/>
-      <c r="N32" s="26"/>
+      <c r="M32" s="26"/>
+      <c r="N32" s="27"/>
     </row>
     <row r="33" spans="8:14" x14ac:dyDescent="0.25">
-      <c r="H33" s="27"/>
-      <c r="I33" s="28"/>
-      <c r="J33" s="29"/>
-      <c r="L33" s="27"/>
-      <c r="M33" s="28"/>
-      <c r="N33" s="29"/>
+      <c r="H33" s="28"/>
+      <c r="I33" s="29"/>
+      <c r="J33" s="30"/>
+      <c r="L33" s="28"/>
+      <c r="M33" s="29"/>
+      <c r="N33" s="30"/>
     </row>
     <row r="35" spans="8:14" x14ac:dyDescent="0.25">
-      <c r="H35" s="24" t="s">
+      <c r="H35" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="I35" s="25"/>
-      <c r="J35" s="26"/>
+      <c r="I35" s="26"/>
+      <c r="J35" s="27"/>
     </row>
     <row r="36" spans="8:14" x14ac:dyDescent="0.25">
-      <c r="H36" s="27"/>
-      <c r="I36" s="28"/>
-      <c r="J36" s="29"/>
+      <c r="H36" s="28"/>
+      <c r="I36" s="29"/>
+      <c r="J36" s="30"/>
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="H35:J36"/>
+    <mergeCell ref="L20:N21"/>
+    <mergeCell ref="L17:N18"/>
+    <mergeCell ref="L23:N24"/>
+    <mergeCell ref="L26:N27"/>
+    <mergeCell ref="L29:N30"/>
+    <mergeCell ref="L32:N33"/>
+    <mergeCell ref="H26:J27"/>
+    <mergeCell ref="H29:J30"/>
+    <mergeCell ref="H32:J33"/>
+    <mergeCell ref="H23:J24"/>
+    <mergeCell ref="H20:J21"/>
     <mergeCell ref="L14:N15"/>
     <mergeCell ref="D6:F7"/>
     <mergeCell ref="H2:J3"/>
@@ -8496,18 +8611,6 @@
     <mergeCell ref="L5:N6"/>
     <mergeCell ref="L8:N9"/>
     <mergeCell ref="L11:N12"/>
-    <mergeCell ref="H35:J36"/>
-    <mergeCell ref="L20:N21"/>
-    <mergeCell ref="L17:N18"/>
-    <mergeCell ref="L23:N24"/>
-    <mergeCell ref="L26:N27"/>
-    <mergeCell ref="L29:N30"/>
-    <mergeCell ref="L32:N33"/>
-    <mergeCell ref="H26:J27"/>
-    <mergeCell ref="H29:J30"/>
-    <mergeCell ref="H32:J33"/>
-    <mergeCell ref="H23:J24"/>
-    <mergeCell ref="H20:J21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -8804,10 +8907,10 @@
       <c r="G4" s="10"/>
       <c r="H4" s="10"/>
       <c r="I4" s="10"/>
-      <c r="J4" s="44" t="s">
+      <c r="J4" s="45" t="s">
         <v>45</v>
       </c>
-      <c r="K4" s="44"/>
+      <c r="K4" s="45"/>
       <c r="L4" s="10"/>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.25">
@@ -8823,8 +8926,8 @@
       <c r="G5" s="10"/>
       <c r="H5" s="10"/>
       <c r="I5" s="10"/>
-      <c r="J5" s="44"/>
-      <c r="K5" s="44"/>
+      <c r="J5" s="45"/>
+      <c r="K5" s="45"/>
       <c r="L5" s="10"/>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.25">
@@ -8840,8 +8943,8 @@
       <c r="G6" s="10"/>
       <c r="H6" s="10"/>
       <c r="I6" s="10"/>
-      <c r="J6" s="44"/>
-      <c r="K6" s="44"/>
+      <c r="J6" s="45"/>
+      <c r="K6" s="45"/>
       <c r="L6" s="10"/>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.25">
@@ -8855,8 +8958,8 @@
       <c r="G7" s="10"/>
       <c r="H7" s="10"/>
       <c r="I7" s="10"/>
-      <c r="J7" s="44"/>
-      <c r="K7" s="44"/>
+      <c r="J7" s="45"/>
+      <c r="K7" s="45"/>
       <c r="L7" s="10"/>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.25">
@@ -8868,8 +8971,8 @@
       <c r="G8" s="10"/>
       <c r="H8" s="10"/>
       <c r="I8" s="10"/>
-      <c r="J8" s="44"/>
-      <c r="K8" s="44"/>
+      <c r="J8" s="45"/>
+      <c r="K8" s="45"/>
       <c r="L8" s="10"/>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.25">
@@ -8885,8 +8988,8 @@
       <c r="G9" s="10"/>
       <c r="H9" s="10"/>
       <c r="I9" s="10"/>
-      <c r="J9" s="44"/>
-      <c r="K9" s="44"/>
+      <c r="J9" s="45"/>
+      <c r="K9" s="45"/>
       <c r="L9" s="10"/>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.25">
@@ -8902,8 +9005,8 @@
       <c r="G10" s="10"/>
       <c r="H10" s="10"/>
       <c r="I10" s="10"/>
-      <c r="J10" s="44"/>
-      <c r="K10" s="44"/>
+      <c r="J10" s="45"/>
+      <c r="K10" s="45"/>
       <c r="L10" s="10"/>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.25">
@@ -8919,8 +9022,8 @@
       <c r="G11" s="10"/>
       <c r="H11" s="10"/>
       <c r="I11" s="10"/>
-      <c r="J11" s="44"/>
-      <c r="K11" s="44"/>
+      <c r="J11" s="45"/>
+      <c r="K11" s="45"/>
       <c r="L11" s="10"/>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.25">
@@ -9412,13 +9515,13 @@
       </c>
       <c r="B11" s="18"/>
       <c r="C11" s="17"/>
-      <c r="D11" s="45"/>
+      <c r="D11" s="46"/>
     </row>
     <row r="12" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="17"/>
       <c r="B12" s="17"/>
       <c r="C12" s="17"/>
-      <c r="D12" s="46"/>
+      <c r="D12" s="47"/>
     </row>
     <row r="13" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="17" t="s">
@@ -9426,7 +9529,7 @@
       </c>
       <c r="B13" s="18"/>
       <c r="C13" s="17"/>
-      <c r="D13" s="47"/>
+      <c r="D13" s="48"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="17"/>
@@ -10006,7 +10109,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:H42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="B47" sqref="B47"/>
     </sheetView>
   </sheetViews>
@@ -10049,7 +10152,7 @@
       <c r="B4" s="21" t="s">
         <v>144</v>
       </c>
-      <c r="D4" s="48">
+      <c r="D4" s="22">
         <v>22129</v>
       </c>
       <c r="H4" t="s">
@@ -10479,6 +10582,491 @@
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>149</v>
+      </c>
+      <c r="B42" s="21" t="s">
+        <v>133</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3:B42">
+      <formula1>Categorie_Liste</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:I42"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="51.7109375" customWidth="1"/>
+    <col min="3" max="4" width="48.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>132</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="21" t="s">
+        <v>98</v>
+      </c>
+      <c r="B3" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>99</v>
+      </c>
+      <c r="B4" s="21" t="s">
+        <v>144</v>
+      </c>
+      <c r="D4" s="22">
+        <v>22010</v>
+      </c>
+      <c r="I4" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>100</v>
+      </c>
+      <c r="B5" s="21" t="s">
+        <v>144</v>
+      </c>
+      <c r="D5" t="s">
+        <v>153</v>
+      </c>
+      <c r="I5" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>81</v>
+      </c>
+      <c r="B6" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="D6" t="s">
+        <v>180</v>
+      </c>
+      <c r="I6" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>101</v>
+      </c>
+      <c r="B7" s="21" t="s">
+        <v>135</v>
+      </c>
+      <c r="D7" t="s">
+        <v>181</v>
+      </c>
+      <c r="I7" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>102</v>
+      </c>
+      <c r="B8" s="21" t="s">
+        <v>144</v>
+      </c>
+      <c r="D8" t="s">
+        <v>156</v>
+      </c>
+      <c r="I8" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>103</v>
+      </c>
+      <c r="B9" s="21" t="s">
+        <v>136</v>
+      </c>
+      <c r="D9" t="s">
+        <v>182</v>
+      </c>
+      <c r="I9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>104</v>
+      </c>
+      <c r="B10" s="21" t="s">
+        <v>133</v>
+      </c>
+      <c r="D10" t="s">
+        <v>183</v>
+      </c>
+      <c r="I10" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>105</v>
+      </c>
+      <c r="B11" s="21" t="s">
+        <v>133</v>
+      </c>
+      <c r="D11" t="s">
+        <v>184</v>
+      </c>
+      <c r="I11" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>106</v>
+      </c>
+      <c r="B12" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="D12" t="s">
+        <v>185</v>
+      </c>
+      <c r="I12" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>107</v>
+      </c>
+      <c r="B13" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="D13" t="s">
+        <v>186</v>
+      </c>
+      <c r="I13" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>108</v>
+      </c>
+      <c r="B14" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="D14" t="s">
+        <v>187</v>
+      </c>
+      <c r="I14" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>109</v>
+      </c>
+      <c r="B15" s="21" t="s">
+        <v>133</v>
+      </c>
+      <c r="C15" t="s">
+        <v>162</v>
+      </c>
+      <c r="D15" t="s">
+        <v>188</v>
+      </c>
+      <c r="I15" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>110</v>
+      </c>
+      <c r="B16" s="21" t="s">
+        <v>135</v>
+      </c>
+      <c r="D16" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>111</v>
+      </c>
+      <c r="B17" s="21" t="s">
+        <v>144</v>
+      </c>
+      <c r="D17" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>112</v>
+      </c>
+      <c r="B18" s="21" t="s">
+        <v>133</v>
+      </c>
+      <c r="D18" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>113</v>
+      </c>
+      <c r="B19" s="21" t="s">
+        <v>136</v>
+      </c>
+      <c r="D19" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>114</v>
+      </c>
+      <c r="B20" s="21" t="s">
+        <v>136</v>
+      </c>
+      <c r="D20" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>115</v>
+      </c>
+      <c r="B21" s="21" t="s">
+        <v>145</v>
+      </c>
+      <c r="D21" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>116</v>
+      </c>
+      <c r="B22" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="D22" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>117</v>
+      </c>
+      <c r="B23" s="21" t="s">
+        <v>144</v>
+      </c>
+      <c r="D23" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>118</v>
+      </c>
+      <c r="B24" s="21" t="s">
+        <v>146</v>
+      </c>
+      <c r="D24" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>119</v>
+      </c>
+      <c r="B25" s="21" t="s">
+        <v>146</v>
+      </c>
+      <c r="D25" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>120</v>
+      </c>
+      <c r="B26" s="21" t="s">
+        <v>136</v>
+      </c>
+      <c r="C26" s="49" t="s">
+        <v>147</v>
+      </c>
+      <c r="D26" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>121</v>
+      </c>
+      <c r="B27" s="21" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>122</v>
+      </c>
+      <c r="B28" s="21" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>123</v>
+      </c>
+      <c r="B29" s="21" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>124</v>
+      </c>
+      <c r="B30" s="21" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>125</v>
+      </c>
+      <c r="B31" s="21" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>126</v>
+      </c>
+      <c r="B32" s="21" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>127</v>
+      </c>
+      <c r="B33" s="21" t="s">
+        <v>136</v>
+      </c>
+      <c r="D33" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>128</v>
+      </c>
+      <c r="B34" s="21" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>129</v>
+      </c>
+      <c r="B35" s="21" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>130</v>
+      </c>
+      <c r="B36" s="21" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>131</v>
+      </c>
+      <c r="B37" s="21" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>138</v>
+      </c>
+      <c r="B38" s="21" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>139</v>
+      </c>
+      <c r="B39" s="21" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>140</v>
+      </c>
+      <c r="B40" s="21" t="s">
+        <v>136</v>
+      </c>
+      <c r="C40" t="s">
+        <v>141</v>
+      </c>
+      <c r="D40" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>143</v>
+      </c>
+      <c r="B41" s="21" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>149</v>
       </c>

</xml_diff>

<commit_message>
Préparation d'une formulaire pour aider le remplissae et la collecte d'info
</commit_message>
<xml_diff>
--- a/President game.xlsx
+++ b/President game.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950" firstSheet="2" activeTab="8"/>
+    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950" firstSheet="2" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Lancement du jeu" sheetId="1" r:id="rId1"/>
@@ -16,6 +16,7 @@
     <sheet name="Africa " sheetId="7" r:id="rId7"/>
     <sheet name="Benin" sheetId="8" r:id="rId8"/>
     <sheet name="Senegal" sheetId="9" r:id="rId9"/>
+    <sheet name="Senegal_Formulaire" sheetId="10" r:id="rId10"/>
   </sheets>
   <definedNames>
     <definedName name="Categorie_Liste">'Africa '!$H$4:$H$23</definedName>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="495" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="526" uniqueCount="230">
   <si>
     <t>Nombres de postes ministeriels</t>
   </si>
@@ -629,14 +630,101 @@
     <t>Grève enseignants ( depuis 2012 ), mendicité, transport urbain</t>
   </si>
   <si>
-    <t xml:space="preserve">Islam (94%)  Chistianisme </t>
+    <t>Dakar 2 eme ville plus polluée en Afrique</t>
+  </si>
+  <si>
+    <t>7 sur une échelle de 10</t>
+  </si>
+  <si>
+    <t>Maroc - Sénégal (8) Sénégal-France (suceuse), Sénégal  - Mali/CI/Guinnée/Gambie (concurrent) avec une forte communauté de part et d'autre</t>
+  </si>
+  <si>
+    <t>Islam (94%)  Chistianisme (6%)</t>
+  </si>
+  <si>
+    <t>2 alternances politique , 0 coup d’etat</t>
+  </si>
+  <si>
+    <t>informations Générales</t>
+  </si>
+  <si>
+    <t>SENEGAL</t>
+  </si>
+  <si>
+    <t>DAKAR</t>
+  </si>
+  <si>
+    <t>Nom :</t>
+  </si>
+  <si>
+    <t>Capitale :</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zone </t>
+  </si>
+  <si>
+    <t>192 722 KM²</t>
+  </si>
+  <si>
+    <t>Afrique Occidentale</t>
+  </si>
+  <si>
+    <t>Situation Géographique</t>
+  </si>
+  <si>
+    <t>Sud</t>
+  </si>
+  <si>
+    <t>Nord</t>
+  </si>
+  <si>
+    <t>Est</t>
+  </si>
+  <si>
+    <t>Ouest</t>
+  </si>
+  <si>
+    <t>Enclave</t>
+  </si>
+  <si>
+    <t>Mauritanie</t>
+  </si>
+  <si>
+    <t>Guinnée Conakry, Guinnée Bisseau</t>
+  </si>
+  <si>
+    <t>Mali</t>
+  </si>
+  <si>
+    <t>Océan Atlantique</t>
+  </si>
+  <si>
+    <t>Gambie</t>
+  </si>
+  <si>
+    <t>Océans, Mers, Fleuves, Lacs</t>
+  </si>
+  <si>
+    <t>Océan(s)</t>
+  </si>
+  <si>
+    <t>Mer(s)</t>
+  </si>
+  <si>
+    <t>Fleuve(s)</t>
+  </si>
+  <si>
+    <t>Lac(s)</t>
+  </si>
+  <si>
+    <t>Atlantique</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -665,8 +753,23 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Adobe Kaiti Std R"/>
+      <family val="1"/>
+      <charset val="128"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Century"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -721,8 +824,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="13">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -868,11 +983,48 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -904,6 +1056,9 @@
     <xf numFmtId="3" fontId="0" fillId="9" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -928,6 +1083,24 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -944,24 +1117,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -982,8 +1137,29 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -7837,6 +8013,121 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>257175</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Image 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="7877175" y="771525"/>
+          <a:ext cx="1038225" cy="695325"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>409575</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Image 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="7962900" y="1619250"/>
+          <a:ext cx="828675" cy="981075"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A2:C267" totalsRowShown="0" headerRowDxfId="2">
   <autoFilter ref="A2:C267"/>
@@ -8184,97 +8475,662 @@
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
-      <c r="Q5" s="23" t="s">
+      <c r="Q5" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="R5" s="23"/>
-      <c r="S5" s="23"/>
-      <c r="T5" s="23"/>
-      <c r="U5" s="23"/>
-      <c r="V5" s="23"/>
-      <c r="W5" s="23"/>
+      <c r="R5" s="24"/>
+      <c r="S5" s="24"/>
+      <c r="T5" s="24"/>
+      <c r="U5" s="24"/>
+      <c r="V5" s="24"/>
+      <c r="W5" s="24"/>
     </row>
     <row r="6" spans="6:23" x14ac:dyDescent="0.25">
-      <c r="Q6" s="23"/>
-      <c r="R6" s="23"/>
-      <c r="S6" s="23"/>
-      <c r="T6" s="23"/>
-      <c r="U6" s="23"/>
-      <c r="V6" s="23"/>
-      <c r="W6" s="23"/>
+      <c r="Q6" s="24"/>
+      <c r="R6" s="24"/>
+      <c r="S6" s="24"/>
+      <c r="T6" s="24"/>
+      <c r="U6" s="24"/>
+      <c r="V6" s="24"/>
+      <c r="W6" s="24"/>
     </row>
     <row r="7" spans="6:23" x14ac:dyDescent="0.25">
-      <c r="Q7" s="23"/>
-      <c r="R7" s="23"/>
-      <c r="S7" s="23"/>
-      <c r="T7" s="23"/>
-      <c r="U7" s="23"/>
-      <c r="V7" s="23"/>
-      <c r="W7" s="23"/>
+      <c r="Q7" s="24"/>
+      <c r="R7" s="24"/>
+      <c r="S7" s="24"/>
+      <c r="T7" s="24"/>
+      <c r="U7" s="24"/>
+      <c r="V7" s="24"/>
+      <c r="W7" s="24"/>
     </row>
     <row r="9" spans="6:23" x14ac:dyDescent="0.25">
-      <c r="Q9" s="23" t="s">
+      <c r="Q9" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="R9" s="23"/>
-      <c r="S9" s="23"/>
-      <c r="T9" s="23"/>
-      <c r="U9" s="23"/>
-      <c r="V9" s="23"/>
-      <c r="W9" s="23"/>
+      <c r="R9" s="24"/>
+      <c r="S9" s="24"/>
+      <c r="T9" s="24"/>
+      <c r="U9" s="24"/>
+      <c r="V9" s="24"/>
+      <c r="W9" s="24"/>
     </row>
     <row r="10" spans="6:23" x14ac:dyDescent="0.25">
-      <c r="Q10" s="23"/>
-      <c r="R10" s="23"/>
-      <c r="S10" s="23"/>
-      <c r="T10" s="23"/>
-      <c r="U10" s="23"/>
-      <c r="V10" s="23"/>
-      <c r="W10" s="23"/>
+      <c r="Q10" s="24"/>
+      <c r="R10" s="24"/>
+      <c r="S10" s="24"/>
+      <c r="T10" s="24"/>
+      <c r="U10" s="24"/>
+      <c r="V10" s="24"/>
+      <c r="W10" s="24"/>
     </row>
     <row r="11" spans="6:23" x14ac:dyDescent="0.25">
-      <c r="Q11" s="23"/>
-      <c r="R11" s="23"/>
-      <c r="S11" s="23"/>
-      <c r="T11" s="23"/>
-      <c r="U11" s="23"/>
-      <c r="V11" s="23"/>
-      <c r="W11" s="23"/>
+      <c r="Q11" s="24"/>
+      <c r="R11" s="24"/>
+      <c r="S11" s="24"/>
+      <c r="T11" s="24"/>
+      <c r="U11" s="24"/>
+      <c r="V11" s="24"/>
+      <c r="W11" s="24"/>
     </row>
     <row r="13" spans="6:23" x14ac:dyDescent="0.25">
-      <c r="Q13" s="24" t="s">
+      <c r="Q13" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="R13" s="24"/>
-      <c r="S13" s="24"/>
-      <c r="T13" s="24"/>
-      <c r="U13" s="24"/>
-      <c r="V13" s="24"/>
-      <c r="W13" s="24"/>
+      <c r="R13" s="25"/>
+      <c r="S13" s="25"/>
+      <c r="T13" s="25"/>
+      <c r="U13" s="25"/>
+      <c r="V13" s="25"/>
+      <c r="W13" s="25"/>
     </row>
     <row r="14" spans="6:23" x14ac:dyDescent="0.25">
-      <c r="Q14" s="24"/>
-      <c r="R14" s="24"/>
-      <c r="S14" s="24"/>
-      <c r="T14" s="24"/>
-      <c r="U14" s="24"/>
-      <c r="V14" s="24"/>
-      <c r="W14" s="24"/>
+      <c r="Q14" s="25"/>
+      <c r="R14" s="25"/>
+      <c r="S14" s="25"/>
+      <c r="T14" s="25"/>
+      <c r="U14" s="25"/>
+      <c r="V14" s="25"/>
+      <c r="W14" s="25"/>
     </row>
     <row r="15" spans="6:23" x14ac:dyDescent="0.25">
-      <c r="Q15" s="24"/>
-      <c r="R15" s="24"/>
-      <c r="S15" s="24"/>
-      <c r="T15" s="24"/>
-      <c r="U15" s="24"/>
-      <c r="V15" s="24"/>
-      <c r="W15" s="24"/>
+      <c r="Q15" s="25"/>
+      <c r="R15" s="25"/>
+      <c r="S15" s="25"/>
+      <c r="T15" s="25"/>
+      <c r="U15" s="25"/>
+      <c r="V15" s="25"/>
+      <c r="W15" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="Q5:W7"/>
     <mergeCell ref="Q9:W11"/>
     <mergeCell ref="Q13:W15"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N30"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" s="55" t="s">
+        <v>205</v>
+      </c>
+      <c r="B1" s="55"/>
+      <c r="C1" s="55"/>
+      <c r="D1" s="55"/>
+      <c r="E1" s="55"/>
+      <c r="F1" s="55"/>
+      <c r="G1" s="55"/>
+      <c r="H1" s="55"/>
+      <c r="I1" s="55"/>
+      <c r="J1" s="55"/>
+      <c r="K1" s="55"/>
+      <c r="L1" s="55"/>
+      <c r="M1" s="55"/>
+      <c r="N1" s="55"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" s="55"/>
+      <c r="B2" s="55"/>
+      <c r="C2" s="55"/>
+      <c r="D2" s="55"/>
+      <c r="E2" s="55"/>
+      <c r="F2" s="55"/>
+      <c r="G2" s="55"/>
+      <c r="H2" s="55"/>
+      <c r="I2" s="55"/>
+      <c r="J2" s="55"/>
+      <c r="K2" s="55"/>
+      <c r="L2" s="55"/>
+      <c r="M2" s="55"/>
+      <c r="N2" s="55"/>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" s="50"/>
+      <c r="B3" s="50"/>
+      <c r="C3" s="50"/>
+      <c r="D3" s="50"/>
+      <c r="E3" s="50"/>
+      <c r="F3" s="50"/>
+      <c r="G3" s="50"/>
+      <c r="H3" s="50"/>
+      <c r="I3" s="50"/>
+      <c r="J3" s="50"/>
+      <c r="K3" s="50"/>
+      <c r="L3" s="50"/>
+      <c r="M3" s="50"/>
+      <c r="N3" s="50"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" s="50"/>
+      <c r="B4" s="50"/>
+      <c r="C4" s="50"/>
+      <c r="D4" s="50"/>
+      <c r="E4" s="50"/>
+      <c r="F4" s="50"/>
+      <c r="G4" s="50"/>
+      <c r="H4" s="50"/>
+      <c r="I4" s="50"/>
+      <c r="J4" s="50"/>
+      <c r="K4" s="50"/>
+      <c r="L4" s="50"/>
+      <c r="M4" s="50"/>
+      <c r="N4" s="50"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" s="50"/>
+      <c r="B5" s="50"/>
+      <c r="C5" s="54" t="s">
+        <v>208</v>
+      </c>
+      <c r="D5" s="50"/>
+      <c r="E5" s="50"/>
+      <c r="F5" s="51" t="s">
+        <v>206</v>
+      </c>
+      <c r="G5" s="52"/>
+      <c r="H5" s="52"/>
+      <c r="I5" s="53"/>
+      <c r="J5" s="50"/>
+      <c r="K5" s="50"/>
+      <c r="L5" s="50"/>
+      <c r="M5" s="50"/>
+      <c r="N5" s="50"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" s="50"/>
+      <c r="B6" s="50"/>
+      <c r="C6" s="54" t="s">
+        <v>209</v>
+      </c>
+      <c r="D6" s="50"/>
+      <c r="E6" s="50"/>
+      <c r="F6" s="51" t="s">
+        <v>207</v>
+      </c>
+      <c r="G6" s="52"/>
+      <c r="H6" s="52"/>
+      <c r="I6" s="53"/>
+      <c r="J6" s="50"/>
+      <c r="K6" s="50"/>
+      <c r="L6" s="50"/>
+      <c r="M6" s="50"/>
+      <c r="N6" s="50"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" s="50"/>
+      <c r="B7" s="50"/>
+      <c r="C7" s="54" t="s">
+        <v>76</v>
+      </c>
+      <c r="D7" s="50"/>
+      <c r="E7" s="50"/>
+      <c r="F7" s="51" t="s">
+        <v>211</v>
+      </c>
+      <c r="G7" s="52"/>
+      <c r="H7" s="52"/>
+      <c r="I7" s="53"/>
+      <c r="J7" s="50"/>
+      <c r="K7" s="50"/>
+      <c r="L7" s="50"/>
+      <c r="M7" s="50"/>
+      <c r="N7" s="50"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" s="50"/>
+      <c r="B8" s="50"/>
+      <c r="C8" s="54" t="s">
+        <v>210</v>
+      </c>
+      <c r="D8" s="50"/>
+      <c r="E8" s="50"/>
+      <c r="F8" s="51" t="s">
+        <v>212</v>
+      </c>
+      <c r="G8" s="52"/>
+      <c r="H8" s="52"/>
+      <c r="I8" s="53"/>
+      <c r="J8" s="50"/>
+      <c r="K8" s="50"/>
+      <c r="L8" s="50"/>
+      <c r="M8" s="50"/>
+      <c r="N8" s="50"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" s="50"/>
+      <c r="B9" s="50"/>
+      <c r="C9" s="50"/>
+      <c r="D9" s="50"/>
+      <c r="E9" s="50"/>
+      <c r="F9" s="50"/>
+      <c r="G9" s="50"/>
+      <c r="H9" s="50"/>
+      <c r="I9" s="50"/>
+      <c r="J9" s="50"/>
+      <c r="K9" s="50"/>
+      <c r="L9" s="50"/>
+      <c r="M9" s="50"/>
+      <c r="N9" s="50"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" s="50"/>
+      <c r="B10" s="50"/>
+      <c r="C10" s="50"/>
+      <c r="D10" s="50"/>
+      <c r="E10" s="50"/>
+      <c r="F10" s="50"/>
+      <c r="G10" s="50"/>
+      <c r="H10" s="50"/>
+      <c r="I10" s="50"/>
+      <c r="J10" s="50"/>
+      <c r="K10" s="50"/>
+      <c r="L10" s="50"/>
+      <c r="M10" s="50"/>
+      <c r="N10" s="50"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" s="50"/>
+      <c r="B11" s="50"/>
+      <c r="C11" s="50"/>
+      <c r="D11" s="50"/>
+      <c r="E11" s="50"/>
+      <c r="F11" s="50"/>
+      <c r="G11" s="50"/>
+      <c r="H11" s="50"/>
+      <c r="I11" s="50"/>
+      <c r="J11" s="50"/>
+      <c r="K11" s="50"/>
+      <c r="L11" s="50"/>
+      <c r="M11" s="50"/>
+      <c r="N11" s="50"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12" s="50"/>
+      <c r="B12" s="50"/>
+      <c r="C12" s="50"/>
+      <c r="D12" s="50"/>
+      <c r="E12" s="50"/>
+      <c r="F12" s="50"/>
+      <c r="G12" s="50"/>
+      <c r="H12" s="50"/>
+      <c r="I12" s="50"/>
+      <c r="J12" s="50"/>
+      <c r="K12" s="50"/>
+      <c r="L12" s="50"/>
+      <c r="M12" s="50"/>
+      <c r="N12" s="50"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" s="50"/>
+      <c r="B13" s="50"/>
+      <c r="C13" s="50"/>
+      <c r="D13" s="50"/>
+      <c r="E13" s="50"/>
+      <c r="F13" s="50"/>
+      <c r="G13" s="50"/>
+      <c r="H13" s="50"/>
+      <c r="I13" s="50"/>
+      <c r="J13" s="50"/>
+      <c r="K13" s="50"/>
+      <c r="L13" s="50"/>
+      <c r="M13" s="50"/>
+      <c r="N13" s="50"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A14" s="50"/>
+      <c r="B14" s="50"/>
+      <c r="C14" s="50"/>
+      <c r="D14" s="50"/>
+      <c r="E14" s="50"/>
+      <c r="F14" s="50"/>
+      <c r="G14" s="50"/>
+      <c r="H14" s="50"/>
+      <c r="I14" s="50"/>
+      <c r="J14" s="50"/>
+      <c r="K14" s="50"/>
+      <c r="L14" s="50"/>
+      <c r="M14" s="50"/>
+      <c r="N14" s="50"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15" s="55" t="s">
+        <v>213</v>
+      </c>
+      <c r="B15" s="55"/>
+      <c r="C15" s="55"/>
+      <c r="D15" s="55"/>
+      <c r="E15" s="55"/>
+      <c r="F15" s="55"/>
+      <c r="G15" s="55"/>
+      <c r="H15" s="55"/>
+      <c r="I15" s="55"/>
+      <c r="J15" s="55"/>
+      <c r="K15" s="55"/>
+      <c r="L15" s="55"/>
+      <c r="M15" s="55"/>
+      <c r="N15" s="55"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16" s="55"/>
+      <c r="B16" s="55"/>
+      <c r="C16" s="55"/>
+      <c r="D16" s="55"/>
+      <c r="E16" s="55"/>
+      <c r="F16" s="55"/>
+      <c r="G16" s="55"/>
+      <c r="H16" s="55"/>
+      <c r="I16" s="55"/>
+      <c r="J16" s="55"/>
+      <c r="K16" s="55"/>
+      <c r="L16" s="55"/>
+      <c r="M16" s="55"/>
+      <c r="N16" s="55"/>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A17" s="50"/>
+      <c r="B17" s="50"/>
+      <c r="C17" s="50"/>
+      <c r="D17" s="50"/>
+      <c r="E17" s="50"/>
+      <c r="F17" s="50"/>
+      <c r="G17" s="50"/>
+      <c r="H17" s="50"/>
+      <c r="I17" s="50"/>
+      <c r="J17" s="50"/>
+      <c r="K17" s="50"/>
+      <c r="L17" s="50"/>
+      <c r="M17" s="50"/>
+      <c r="N17" s="50"/>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A18" s="50"/>
+      <c r="B18" s="50"/>
+      <c r="C18" s="54" t="s">
+        <v>104</v>
+      </c>
+      <c r="D18" s="50"/>
+      <c r="E18" s="50"/>
+      <c r="F18" s="56" t="s">
+        <v>215</v>
+      </c>
+      <c r="G18" s="57" t="s">
+        <v>219</v>
+      </c>
+      <c r="H18" s="58"/>
+      <c r="I18" s="58"/>
+      <c r="J18" s="58"/>
+      <c r="K18" s="59"/>
+      <c r="L18" s="50"/>
+      <c r="M18" s="50"/>
+      <c r="N18" s="50"/>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A19" s="50"/>
+      <c r="B19" s="50"/>
+      <c r="C19" s="50"/>
+      <c r="D19" s="50"/>
+      <c r="E19" s="50"/>
+      <c r="F19" s="56" t="s">
+        <v>214</v>
+      </c>
+      <c r="G19" s="57" t="s">
+        <v>220</v>
+      </c>
+      <c r="H19" s="58"/>
+      <c r="I19" s="58"/>
+      <c r="J19" s="58"/>
+      <c r="K19" s="59"/>
+      <c r="L19" s="50"/>
+      <c r="M19" s="50"/>
+      <c r="N19" s="50"/>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A20" s="50"/>
+      <c r="B20" s="50"/>
+      <c r="C20" s="50"/>
+      <c r="D20" s="50"/>
+      <c r="E20" s="50"/>
+      <c r="F20" s="56" t="s">
+        <v>216</v>
+      </c>
+      <c r="G20" s="57" t="s">
+        <v>221</v>
+      </c>
+      <c r="H20" s="58"/>
+      <c r="I20" s="58"/>
+      <c r="J20" s="58"/>
+      <c r="K20" s="59"/>
+      <c r="L20" s="50"/>
+      <c r="M20" s="50"/>
+      <c r="N20" s="50"/>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A21" s="50"/>
+      <c r="B21" s="50"/>
+      <c r="C21" s="50"/>
+      <c r="D21" s="50"/>
+      <c r="E21" s="50"/>
+      <c r="F21" s="56" t="s">
+        <v>217</v>
+      </c>
+      <c r="G21" s="57" t="s">
+        <v>222</v>
+      </c>
+      <c r="H21" s="58"/>
+      <c r="I21" s="58"/>
+      <c r="J21" s="58"/>
+      <c r="K21" s="59"/>
+      <c r="L21" s="50"/>
+      <c r="M21" s="50"/>
+      <c r="N21" s="50"/>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A22" s="50"/>
+      <c r="B22" s="50"/>
+      <c r="C22" s="50"/>
+      <c r="D22" s="50"/>
+      <c r="E22" s="50"/>
+      <c r="F22" s="56" t="s">
+        <v>218</v>
+      </c>
+      <c r="G22" s="57" t="s">
+        <v>223</v>
+      </c>
+      <c r="H22" s="58"/>
+      <c r="I22" s="58"/>
+      <c r="J22" s="58"/>
+      <c r="K22" s="59"/>
+      <c r="L22" s="50"/>
+      <c r="M22" s="50"/>
+      <c r="N22" s="50"/>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A23" s="50"/>
+      <c r="B23" s="50"/>
+      <c r="C23" s="50"/>
+      <c r="D23" s="50"/>
+      <c r="E23" s="50"/>
+      <c r="F23" s="50"/>
+      <c r="G23" s="50"/>
+      <c r="H23" s="50"/>
+      <c r="I23" s="50"/>
+      <c r="J23" s="50"/>
+      <c r="K23" s="50"/>
+      <c r="L23" s="50"/>
+      <c r="M23" s="50"/>
+      <c r="N23" s="50"/>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A24" s="50"/>
+      <c r="B24" s="50"/>
+      <c r="C24" s="54" t="s">
+        <v>224</v>
+      </c>
+      <c r="D24" s="50"/>
+      <c r="E24" s="50"/>
+      <c r="F24" s="50" t="s">
+        <v>225</v>
+      </c>
+      <c r="G24" s="57" t="s">
+        <v>229</v>
+      </c>
+      <c r="H24" s="58"/>
+      <c r="I24" s="58"/>
+      <c r="J24" s="58"/>
+      <c r="K24" s="59"/>
+      <c r="L24" s="50"/>
+      <c r="M24" s="50"/>
+      <c r="N24" s="50"/>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A25" s="50"/>
+      <c r="B25" s="50"/>
+      <c r="C25" s="50"/>
+      <c r="D25" s="50"/>
+      <c r="E25" s="50"/>
+      <c r="F25" s="50" t="s">
+        <v>226</v>
+      </c>
+      <c r="G25" s="50"/>
+      <c r="H25" s="50"/>
+      <c r="I25" s="50"/>
+      <c r="J25" s="50"/>
+      <c r="K25" s="50"/>
+      <c r="L25" s="50"/>
+      <c r="M25" s="50"/>
+      <c r="N25" s="50"/>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A26" s="50"/>
+      <c r="B26" s="50"/>
+      <c r="C26" s="50"/>
+      <c r="D26" s="50"/>
+      <c r="E26" s="50"/>
+      <c r="F26" s="50" t="s">
+        <v>227</v>
+      </c>
+      <c r="G26" s="50"/>
+      <c r="H26" s="50"/>
+      <c r="I26" s="50"/>
+      <c r="J26" s="50"/>
+      <c r="K26" s="50"/>
+      <c r="L26" s="50"/>
+      <c r="M26" s="50"/>
+      <c r="N26" s="50"/>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A27" s="50"/>
+      <c r="B27" s="50"/>
+      <c r="C27" s="50"/>
+      <c r="D27" s="50"/>
+      <c r="E27" s="50"/>
+      <c r="F27" s="50" t="s">
+        <v>228</v>
+      </c>
+      <c r="G27" s="50"/>
+      <c r="H27" s="50"/>
+      <c r="I27" s="50"/>
+      <c r="J27" s="50"/>
+      <c r="K27" s="50"/>
+      <c r="L27" s="50"/>
+      <c r="M27" s="50"/>
+      <c r="N27" s="50"/>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A28" s="50"/>
+      <c r="B28" s="50"/>
+      <c r="C28" s="50"/>
+      <c r="D28" s="50"/>
+      <c r="E28" s="50"/>
+      <c r="F28" s="50"/>
+      <c r="G28" s="50"/>
+      <c r="H28" s="50"/>
+      <c r="I28" s="50"/>
+      <c r="J28" s="50"/>
+      <c r="K28" s="50"/>
+      <c r="L28" s="50"/>
+      <c r="M28" s="50"/>
+      <c r="N28" s="50"/>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A29" s="50"/>
+      <c r="B29" s="50"/>
+      <c r="C29" s="50"/>
+      <c r="D29" s="50"/>
+      <c r="E29" s="50"/>
+      <c r="F29" s="50"/>
+      <c r="G29" s="50"/>
+      <c r="H29" s="50"/>
+      <c r="I29" s="50"/>
+      <c r="J29" s="50"/>
+      <c r="K29" s="50"/>
+      <c r="L29" s="50"/>
+      <c r="M29" s="50"/>
+      <c r="N29" s="50"/>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A30" s="50"/>
+      <c r="B30" s="50"/>
+      <c r="C30" s="50"/>
+      <c r="D30" s="50"/>
+      <c r="E30" s="50"/>
+      <c r="F30" s="50"/>
+      <c r="G30" s="50"/>
+      <c r="H30" s="50"/>
+      <c r="I30" s="50"/>
+      <c r="J30" s="50"/>
+      <c r="K30" s="50"/>
+      <c r="L30" s="50"/>
+      <c r="M30" s="50"/>
+      <c r="N30" s="50"/>
+    </row>
+  </sheetData>
+  <mergeCells count="12">
+    <mergeCell ref="G24:K24"/>
+    <mergeCell ref="A15:N16"/>
+    <mergeCell ref="G18:K18"/>
+    <mergeCell ref="G19:K19"/>
+    <mergeCell ref="G20:K20"/>
+    <mergeCell ref="G21:K21"/>
+    <mergeCell ref="G22:K22"/>
+    <mergeCell ref="F5:I5"/>
+    <mergeCell ref="F6:I6"/>
+    <mergeCell ref="F7:I7"/>
+    <mergeCell ref="F8:I8"/>
+    <mergeCell ref="A1:N2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -8298,56 +9154,56 @@
   </cols>
   <sheetData>
     <row r="2" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="H2" s="37" t="s">
+      <c r="H2" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="I2" s="38"/>
-      <c r="J2" s="39"/>
-      <c r="L2" s="25" t="s">
+      <c r="I2" s="33"/>
+      <c r="J2" s="34"/>
+      <c r="L2" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="M2" s="26"/>
-      <c r="N2" s="27"/>
+      <c r="M2" s="27"/>
+      <c r="N2" s="28"/>
     </row>
     <row r="3" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="H3" s="40"/>
-      <c r="I3" s="41"/>
-      <c r="J3" s="42"/>
-      <c r="L3" s="28"/>
-      <c r="M3" s="29"/>
-      <c r="N3" s="30"/>
+      <c r="H3" s="35"/>
+      <c r="I3" s="36"/>
+      <c r="J3" s="37"/>
+      <c r="L3" s="29"/>
+      <c r="M3" s="30"/>
+      <c r="N3" s="31"/>
     </row>
     <row r="5" spans="4:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H5" s="25" t="s">
+      <c r="H5" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="I5" s="26"/>
-      <c r="J5" s="27"/>
-      <c r="L5" s="25" t="s">
+      <c r="I5" s="27"/>
+      <c r="J5" s="28"/>
+      <c r="L5" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="M5" s="26"/>
-      <c r="N5" s="27"/>
+      <c r="M5" s="27"/>
+      <c r="N5" s="28"/>
     </row>
     <row r="6" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="D6" s="31" t="s">
+      <c r="D6" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="E6" s="32"/>
-      <c r="F6" s="33"/>
+      <c r="E6" s="39"/>
+      <c r="F6" s="40"/>
       <c r="G6" s="3"/>
-      <c r="H6" s="28"/>
-      <c r="I6" s="29"/>
-      <c r="J6" s="30"/>
+      <c r="H6" s="29"/>
+      <c r="I6" s="30"/>
+      <c r="J6" s="31"/>
       <c r="K6" s="4"/>
-      <c r="L6" s="28"/>
-      <c r="M6" s="29"/>
-      <c r="N6" s="30"/>
+      <c r="L6" s="29"/>
+      <c r="M6" s="30"/>
+      <c r="N6" s="31"/>
     </row>
     <row r="7" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="D7" s="34"/>
-      <c r="E7" s="35"/>
-      <c r="F7" s="36"/>
+      <c r="D7" s="41"/>
+      <c r="E7" s="42"/>
+      <c r="F7" s="43"/>
       <c r="G7" s="3"/>
       <c r="H7" s="4"/>
       <c r="I7" s="4"/>
@@ -8358,246 +9214,234 @@
       <c r="N7" s="4"/>
     </row>
     <row r="8" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="H8" s="37" t="s">
+      <c r="H8" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="I8" s="38"/>
-      <c r="J8" s="39"/>
-      <c r="L8" s="25" t="s">
+      <c r="I8" s="33"/>
+      <c r="J8" s="34"/>
+      <c r="L8" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="M8" s="26"/>
-      <c r="N8" s="27"/>
+      <c r="M8" s="27"/>
+      <c r="N8" s="28"/>
     </row>
     <row r="9" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="D9" s="43" t="s">
+      <c r="D9" s="44" t="s">
         <v>22</v>
       </c>
-      <c r="E9" s="43"/>
-      <c r="F9" s="43"/>
-      <c r="H9" s="40"/>
-      <c r="I9" s="41"/>
-      <c r="J9" s="42"/>
-      <c r="L9" s="28"/>
-      <c r="M9" s="29"/>
-      <c r="N9" s="30"/>
+      <c r="E9" s="44"/>
+      <c r="F9" s="44"/>
+      <c r="H9" s="35"/>
+      <c r="I9" s="36"/>
+      <c r="J9" s="37"/>
+      <c r="L9" s="29"/>
+      <c r="M9" s="30"/>
+      <c r="N9" s="31"/>
     </row>
     <row r="10" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="D10" s="44"/>
-      <c r="E10" s="44"/>
-      <c r="F10" s="44"/>
+      <c r="D10" s="45"/>
+      <c r="E10" s="45"/>
+      <c r="F10" s="45"/>
     </row>
     <row r="11" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="D11" s="44"/>
-      <c r="E11" s="44"/>
-      <c r="F11" s="44"/>
-      <c r="H11" s="37" t="s">
+      <c r="D11" s="45"/>
+      <c r="E11" s="45"/>
+      <c r="F11" s="45"/>
+      <c r="H11" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="I11" s="38"/>
-      <c r="J11" s="39"/>
-      <c r="L11" s="37" t="s">
+      <c r="I11" s="33"/>
+      <c r="J11" s="34"/>
+      <c r="L11" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="M11" s="38"/>
-      <c r="N11" s="39"/>
+      <c r="M11" s="33"/>
+      <c r="N11" s="34"/>
     </row>
     <row r="12" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="D12" s="44"/>
-      <c r="E12" s="44"/>
-      <c r="F12" s="44"/>
-      <c r="H12" s="40"/>
-      <c r="I12" s="41"/>
-      <c r="J12" s="42"/>
-      <c r="L12" s="40"/>
-      <c r="M12" s="41"/>
-      <c r="N12" s="42"/>
+      <c r="D12" s="45"/>
+      <c r="E12" s="45"/>
+      <c r="F12" s="45"/>
+      <c r="H12" s="35"/>
+      <c r="I12" s="36"/>
+      <c r="J12" s="37"/>
+      <c r="L12" s="35"/>
+      <c r="M12" s="36"/>
+      <c r="N12" s="37"/>
     </row>
     <row r="13" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="D13" s="44"/>
-      <c r="E13" s="44"/>
-      <c r="F13" s="44"/>
+      <c r="D13" s="45"/>
+      <c r="E13" s="45"/>
+      <c r="F13" s="45"/>
     </row>
     <row r="14" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="D14" s="44"/>
-      <c r="E14" s="44"/>
-      <c r="F14" s="44"/>
-      <c r="H14" s="25" t="s">
+      <c r="D14" s="45"/>
+      <c r="E14" s="45"/>
+      <c r="F14" s="45"/>
+      <c r="H14" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="I14" s="26"/>
-      <c r="J14" s="27"/>
-      <c r="L14" s="25" t="s">
+      <c r="I14" s="27"/>
+      <c r="J14" s="28"/>
+      <c r="L14" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="M14" s="26"/>
-      <c r="N14" s="27"/>
+      <c r="M14" s="27"/>
+      <c r="N14" s="28"/>
     </row>
     <row r="15" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="D15" s="44"/>
-      <c r="E15" s="44"/>
-      <c r="F15" s="44"/>
-      <c r="H15" s="28"/>
-      <c r="I15" s="29"/>
-      <c r="J15" s="30"/>
-      <c r="L15" s="28"/>
-      <c r="M15" s="29"/>
-      <c r="N15" s="30"/>
+      <c r="D15" s="45"/>
+      <c r="E15" s="45"/>
+      <c r="F15" s="45"/>
+      <c r="H15" s="29"/>
+      <c r="I15" s="30"/>
+      <c r="J15" s="31"/>
+      <c r="L15" s="29"/>
+      <c r="M15" s="30"/>
+      <c r="N15" s="31"/>
     </row>
     <row r="16" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="D16" s="44"/>
-      <c r="E16" s="44"/>
-      <c r="F16" s="44"/>
+      <c r="D16" s="45"/>
+      <c r="E16" s="45"/>
+      <c r="F16" s="45"/>
     </row>
     <row r="17" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="D17" s="44"/>
-      <c r="E17" s="44"/>
-      <c r="F17" s="44"/>
-      <c r="H17" s="37" t="s">
+      <c r="D17" s="45"/>
+      <c r="E17" s="45"/>
+      <c r="F17" s="45"/>
+      <c r="H17" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="I17" s="38"/>
-      <c r="J17" s="39"/>
-      <c r="L17" s="25" t="s">
+      <c r="I17" s="33"/>
+      <c r="J17" s="34"/>
+      <c r="L17" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="M17" s="26"/>
-      <c r="N17" s="27"/>
+      <c r="M17" s="27"/>
+      <c r="N17" s="28"/>
     </row>
     <row r="18" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="H18" s="40"/>
-      <c r="I18" s="41"/>
-      <c r="J18" s="42"/>
-      <c r="L18" s="28"/>
-      <c r="M18" s="29"/>
-      <c r="N18" s="30"/>
+      <c r="H18" s="35"/>
+      <c r="I18" s="36"/>
+      <c r="J18" s="37"/>
+      <c r="L18" s="29"/>
+      <c r="M18" s="30"/>
+      <c r="N18" s="31"/>
     </row>
     <row r="20" spans="4:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H20" s="37" t="s">
+      <c r="H20" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="I20" s="38"/>
-      <c r="J20" s="39"/>
-      <c r="L20" s="25" t="s">
+      <c r="I20" s="33"/>
+      <c r="J20" s="34"/>
+      <c r="L20" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="M20" s="26"/>
-      <c r="N20" s="27"/>
+      <c r="M20" s="27"/>
+      <c r="N20" s="28"/>
     </row>
     <row r="21" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="H21" s="40"/>
-      <c r="I21" s="41"/>
-      <c r="J21" s="42"/>
-      <c r="L21" s="28"/>
-      <c r="M21" s="29"/>
-      <c r="N21" s="30"/>
+      <c r="H21" s="35"/>
+      <c r="I21" s="36"/>
+      <c r="J21" s="37"/>
+      <c r="L21" s="29"/>
+      <c r="M21" s="30"/>
+      <c r="N21" s="31"/>
     </row>
     <row r="23" spans="4:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H23" s="25" t="s">
+      <c r="H23" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="I23" s="26"/>
-      <c r="J23" s="27"/>
-      <c r="L23" s="25" t="s">
+      <c r="I23" s="27"/>
+      <c r="J23" s="28"/>
+      <c r="L23" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="M23" s="26"/>
-      <c r="N23" s="27"/>
+      <c r="M23" s="27"/>
+      <c r="N23" s="28"/>
     </row>
     <row r="24" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="H24" s="28"/>
-      <c r="I24" s="29"/>
-      <c r="J24" s="30"/>
-      <c r="L24" s="28"/>
-      <c r="M24" s="29"/>
-      <c r="N24" s="30"/>
+      <c r="H24" s="29"/>
+      <c r="I24" s="30"/>
+      <c r="J24" s="31"/>
+      <c r="L24" s="29"/>
+      <c r="M24" s="30"/>
+      <c r="N24" s="31"/>
     </row>
     <row r="26" spans="4:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H26" s="25" t="s">
+      <c r="H26" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="I26" s="26"/>
-      <c r="J26" s="27"/>
-      <c r="L26" s="25" t="s">
+      <c r="I26" s="27"/>
+      <c r="J26" s="28"/>
+      <c r="L26" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="M26" s="26"/>
-      <c r="N26" s="27"/>
+      <c r="M26" s="27"/>
+      <c r="N26" s="28"/>
     </row>
     <row r="27" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="H27" s="28"/>
-      <c r="I27" s="29"/>
-      <c r="J27" s="30"/>
-      <c r="L27" s="28"/>
-      <c r="M27" s="29"/>
-      <c r="N27" s="30"/>
+      <c r="H27" s="29"/>
+      <c r="I27" s="30"/>
+      <c r="J27" s="31"/>
+      <c r="L27" s="29"/>
+      <c r="M27" s="30"/>
+      <c r="N27" s="31"/>
     </row>
     <row r="29" spans="4:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H29" s="25" t="s">
+      <c r="H29" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="I29" s="26"/>
-      <c r="J29" s="27"/>
-      <c r="L29" s="25" t="s">
+      <c r="I29" s="27"/>
+      <c r="J29" s="28"/>
+      <c r="L29" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="M29" s="26"/>
-      <c r="N29" s="27"/>
+      <c r="M29" s="27"/>
+      <c r="N29" s="28"/>
     </row>
     <row r="30" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="H30" s="28"/>
-      <c r="I30" s="29"/>
-      <c r="J30" s="30"/>
-      <c r="L30" s="28"/>
-      <c r="M30" s="29"/>
-      <c r="N30" s="30"/>
+      <c r="H30" s="29"/>
+      <c r="I30" s="30"/>
+      <c r="J30" s="31"/>
+      <c r="L30" s="29"/>
+      <c r="M30" s="30"/>
+      <c r="N30" s="31"/>
     </row>
     <row r="32" spans="4:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H32" s="25" t="s">
+      <c r="H32" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="I32" s="26"/>
-      <c r="J32" s="27"/>
-      <c r="L32" s="25" t="s">
+      <c r="I32" s="27"/>
+      <c r="J32" s="28"/>
+      <c r="L32" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="M32" s="26"/>
-      <c r="N32" s="27"/>
+      <c r="M32" s="27"/>
+      <c r="N32" s="28"/>
     </row>
     <row r="33" spans="8:14" x14ac:dyDescent="0.25">
-      <c r="H33" s="28"/>
-      <c r="I33" s="29"/>
-      <c r="J33" s="30"/>
-      <c r="L33" s="28"/>
-      <c r="M33" s="29"/>
-      <c r="N33" s="30"/>
+      <c r="H33" s="29"/>
+      <c r="I33" s="30"/>
+      <c r="J33" s="31"/>
+      <c r="L33" s="29"/>
+      <c r="M33" s="30"/>
+      <c r="N33" s="31"/>
     </row>
     <row r="35" spans="8:14" x14ac:dyDescent="0.25">
-      <c r="H35" s="25" t="s">
+      <c r="H35" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="I35" s="26"/>
-      <c r="J35" s="27"/>
+      <c r="I35" s="27"/>
+      <c r="J35" s="28"/>
     </row>
     <row r="36" spans="8:14" x14ac:dyDescent="0.25">
-      <c r="H36" s="28"/>
-      <c r="I36" s="29"/>
-      <c r="J36" s="30"/>
+      <c r="H36" s="29"/>
+      <c r="I36" s="30"/>
+      <c r="J36" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="H35:J36"/>
-    <mergeCell ref="L20:N21"/>
-    <mergeCell ref="L17:N18"/>
-    <mergeCell ref="L23:N24"/>
-    <mergeCell ref="L26:N27"/>
-    <mergeCell ref="L29:N30"/>
-    <mergeCell ref="L32:N33"/>
-    <mergeCell ref="H26:J27"/>
-    <mergeCell ref="H29:J30"/>
-    <mergeCell ref="H32:J33"/>
-    <mergeCell ref="H23:J24"/>
-    <mergeCell ref="H20:J21"/>
     <mergeCell ref="L14:N15"/>
     <mergeCell ref="D6:F7"/>
     <mergeCell ref="H2:J3"/>
@@ -8611,6 +9455,18 @@
     <mergeCell ref="L5:N6"/>
     <mergeCell ref="L8:N9"/>
     <mergeCell ref="L11:N12"/>
+    <mergeCell ref="H35:J36"/>
+    <mergeCell ref="L20:N21"/>
+    <mergeCell ref="L17:N18"/>
+    <mergeCell ref="L23:N24"/>
+    <mergeCell ref="L26:N27"/>
+    <mergeCell ref="L29:N30"/>
+    <mergeCell ref="L32:N33"/>
+    <mergeCell ref="H26:J27"/>
+    <mergeCell ref="H29:J30"/>
+    <mergeCell ref="H32:J33"/>
+    <mergeCell ref="H23:J24"/>
+    <mergeCell ref="H20:J21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -8907,10 +9763,10 @@
       <c r="G4" s="10"/>
       <c r="H4" s="10"/>
       <c r="I4" s="10"/>
-      <c r="J4" s="45" t="s">
+      <c r="J4" s="46" t="s">
         <v>45</v>
       </c>
-      <c r="K4" s="45"/>
+      <c r="K4" s="46"/>
       <c r="L4" s="10"/>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.25">
@@ -8926,8 +9782,8 @@
       <c r="G5" s="10"/>
       <c r="H5" s="10"/>
       <c r="I5" s="10"/>
-      <c r="J5" s="45"/>
-      <c r="K5" s="45"/>
+      <c r="J5" s="46"/>
+      <c r="K5" s="46"/>
       <c r="L5" s="10"/>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.25">
@@ -8943,8 +9799,8 @@
       <c r="G6" s="10"/>
       <c r="H6" s="10"/>
       <c r="I6" s="10"/>
-      <c r="J6" s="45"/>
-      <c r="K6" s="45"/>
+      <c r="J6" s="46"/>
+      <c r="K6" s="46"/>
       <c r="L6" s="10"/>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.25">
@@ -8958,8 +9814,8 @@
       <c r="G7" s="10"/>
       <c r="H7" s="10"/>
       <c r="I7" s="10"/>
-      <c r="J7" s="45"/>
-      <c r="K7" s="45"/>
+      <c r="J7" s="46"/>
+      <c r="K7" s="46"/>
       <c r="L7" s="10"/>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.25">
@@ -8971,8 +9827,8 @@
       <c r="G8" s="10"/>
       <c r="H8" s="10"/>
       <c r="I8" s="10"/>
-      <c r="J8" s="45"/>
-      <c r="K8" s="45"/>
+      <c r="J8" s="46"/>
+      <c r="K8" s="46"/>
       <c r="L8" s="10"/>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.25">
@@ -8988,8 +9844,8 @@
       <c r="G9" s="10"/>
       <c r="H9" s="10"/>
       <c r="I9" s="10"/>
-      <c r="J9" s="45"/>
-      <c r="K9" s="45"/>
+      <c r="J9" s="46"/>
+      <c r="K9" s="46"/>
       <c r="L9" s="10"/>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.25">
@@ -9005,8 +9861,8 @@
       <c r="G10" s="10"/>
       <c r="H10" s="10"/>
       <c r="I10" s="10"/>
-      <c r="J10" s="45"/>
-      <c r="K10" s="45"/>
+      <c r="J10" s="46"/>
+      <c r="K10" s="46"/>
       <c r="L10" s="10"/>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.25">
@@ -9022,8 +9878,8 @@
       <c r="G11" s="10"/>
       <c r="H11" s="10"/>
       <c r="I11" s="10"/>
-      <c r="J11" s="45"/>
-      <c r="K11" s="45"/>
+      <c r="J11" s="46"/>
+      <c r="K11" s="46"/>
       <c r="L11" s="10"/>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.25">
@@ -9515,13 +10371,13 @@
       </c>
       <c r="B11" s="18"/>
       <c r="C11" s="17"/>
-      <c r="D11" s="46"/>
+      <c r="D11" s="47"/>
     </row>
     <row r="12" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="17"/>
       <c r="B12" s="17"/>
       <c r="C12" s="17"/>
-      <c r="D12" s="47"/>
+      <c r="D12" s="48"/>
     </row>
     <row r="13" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="17" t="s">
@@ -9529,7 +10385,7 @@
       </c>
       <c r="B13" s="18"/>
       <c r="C13" s="17"/>
-      <c r="D13" s="48"/>
+      <c r="D13" s="49"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="17"/>
@@ -10606,8 +11462,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:I42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10930,7 +11786,7 @@
       <c r="B26" s="21" t="s">
         <v>136</v>
       </c>
-      <c r="C26" s="49" t="s">
+      <c r="C26" s="23" t="s">
         <v>147</v>
       </c>
       <c r="D26" t="s">
@@ -10960,6 +11816,9 @@
       <c r="B29" s="21" t="s">
         <v>148</v>
       </c>
+      <c r="D29" t="s">
+        <v>200</v>
+      </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
@@ -10968,6 +11827,9 @@
       <c r="B30" s="21" t="s">
         <v>136</v>
       </c>
+      <c r="D30" t="s">
+        <v>201</v>
+      </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
@@ -10976,6 +11838,9 @@
       <c r="B31" s="21" t="s">
         <v>150</v>
       </c>
+      <c r="D31" t="s">
+        <v>202</v>
+      </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
@@ -10993,7 +11858,7 @@
         <v>136</v>
       </c>
       <c r="D33" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -11002,6 +11867,9 @@
       </c>
       <c r="B34" s="21" t="s">
         <v>144</v>
+      </c>
+      <c r="D34" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Préparation d'une formulaire pour aider le remplissage et la collecte d'info (suite)
</commit_message>
<xml_diff>
--- a/President game.xlsx
+++ b/President game.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950" firstSheet="2" activeTab="9"/>
+    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950" firstSheet="3" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Lancement du jeu" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="526" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="562" uniqueCount="263">
   <si>
     <t>Nombres de postes ministeriels</t>
   </si>
@@ -718,13 +718,112 @@
   </si>
   <si>
     <t>Atlantique</t>
+  </si>
+  <si>
+    <t>NON</t>
+  </si>
+  <si>
+    <t>Lac de Guiers, Lac Rose</t>
+  </si>
+  <si>
+    <t>Fleuve Sénégal, Fleuve du Saloum, Fleuve Casamance</t>
+  </si>
+  <si>
+    <t>Division Administratives</t>
+  </si>
+  <si>
+    <t>Régions</t>
+  </si>
+  <si>
+    <t>Diourbel</t>
+  </si>
+  <si>
+    <t>Fatick</t>
+  </si>
+  <si>
+    <t>Kaolack</t>
+  </si>
+  <si>
+    <t>Kolda</t>
+  </si>
+  <si>
+    <t>Louga</t>
+  </si>
+  <si>
+    <t>Matam</t>
+  </si>
+  <si>
+    <t>Saint-Louis</t>
+  </si>
+  <si>
+    <t>Tambacounda</t>
+  </si>
+  <si>
+    <t>Thiès</t>
+  </si>
+  <si>
+    <t>Ziguinchor</t>
+  </si>
+  <si>
+    <t>Populations</t>
+  </si>
+  <si>
+    <t>Départements</t>
+  </si>
+  <si>
+    <t>Communautés rurales</t>
+  </si>
+  <si>
+    <t>Commune d'arrondisment</t>
+  </si>
+  <si>
+    <t>Village</t>
+  </si>
+  <si>
+    <t>Communes</t>
+  </si>
+  <si>
+    <t>13544 (1988)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nette baisse du nombre </t>
+  </si>
+  <si>
+    <t>Histoire Politiques</t>
+  </si>
+  <si>
+    <t>Post Coloniale</t>
+  </si>
+  <si>
+    <t>Pré-Coloniale</t>
+  </si>
+  <si>
+    <t>Période Coloniale</t>
+  </si>
+  <si>
+    <t>subdivision en royaume</t>
+  </si>
+  <si>
+    <t>Islam dans le Nord, majorité anémiste</t>
+  </si>
+  <si>
+    <t>polygamie</t>
+  </si>
+  <si>
+    <t>une seule université coranique</t>
+  </si>
+  <si>
+    <t>(i) Donner  quelques informations de la vie  avant la colonisation en liaison avec l'actuel pays</t>
+  </si>
+  <si>
+    <t>déplacements en Cheval</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -768,8 +867,40 @@
       <name val="Century"/>
       <family val="1"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="12">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -833,6 +964,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1021,10 +1158,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -1059,6 +1197,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1083,6 +1224,24 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1099,24 +1258,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1137,7 +1278,18 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1147,22 +1299,28 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="13" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="14" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="15" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="3" fontId="0" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="3">
@@ -8125,6 +8283,241 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>704850</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>704850</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="5" name="Connecteur droit avec flèche 4"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1466850" y="6724650"/>
+          <a:ext cx="0" cy="133350"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>714375</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>714375</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="6" name="Connecteur droit avec flèche 5"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1476375" y="7058025"/>
+          <a:ext cx="0" cy="133350"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>676275</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>685800</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="7" name="Connecteur droit avec flèche 6"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1438275" y="7486650"/>
+          <a:ext cx="9525" cy="152400"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>704850</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>704850</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="8" name="Connecteur droit avec flèche 7"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1466850" y="7848600"/>
+          <a:ext cx="0" cy="133350"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>638175</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>638175</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="9" name="Connecteur droit avec flèche 8"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1400175" y="8201025"/>
+          <a:ext cx="0" cy="133350"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -8475,91 +8868,91 @@
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
-      <c r="Q5" s="24" t="s">
+      <c r="Q5" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="R5" s="24"/>
-      <c r="S5" s="24"/>
-      <c r="T5" s="24"/>
-      <c r="U5" s="24"/>
-      <c r="V5" s="24"/>
-      <c r="W5" s="24"/>
+      <c r="R5" s="27"/>
+      <c r="S5" s="27"/>
+      <c r="T5" s="27"/>
+      <c r="U5" s="27"/>
+      <c r="V5" s="27"/>
+      <c r="W5" s="27"/>
     </row>
     <row r="6" spans="6:23" x14ac:dyDescent="0.25">
-      <c r="Q6" s="24"/>
-      <c r="R6" s="24"/>
-      <c r="S6" s="24"/>
-      <c r="T6" s="24"/>
-      <c r="U6" s="24"/>
-      <c r="V6" s="24"/>
-      <c r="W6" s="24"/>
+      <c r="Q6" s="27"/>
+      <c r="R6" s="27"/>
+      <c r="S6" s="27"/>
+      <c r="T6" s="27"/>
+      <c r="U6" s="27"/>
+      <c r="V6" s="27"/>
+      <c r="W6" s="27"/>
     </row>
     <row r="7" spans="6:23" x14ac:dyDescent="0.25">
-      <c r="Q7" s="24"/>
-      <c r="R7" s="24"/>
-      <c r="S7" s="24"/>
-      <c r="T7" s="24"/>
-      <c r="U7" s="24"/>
-      <c r="V7" s="24"/>
-      <c r="W7" s="24"/>
+      <c r="Q7" s="27"/>
+      <c r="R7" s="27"/>
+      <c r="S7" s="27"/>
+      <c r="T7" s="27"/>
+      <c r="U7" s="27"/>
+      <c r="V7" s="27"/>
+      <c r="W7" s="27"/>
     </row>
     <row r="9" spans="6:23" x14ac:dyDescent="0.25">
-      <c r="Q9" s="24" t="s">
+      <c r="Q9" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="R9" s="24"/>
-      <c r="S9" s="24"/>
-      <c r="T9" s="24"/>
-      <c r="U9" s="24"/>
-      <c r="V9" s="24"/>
-      <c r="W9" s="24"/>
+      <c r="R9" s="27"/>
+      <c r="S9" s="27"/>
+      <c r="T9" s="27"/>
+      <c r="U9" s="27"/>
+      <c r="V9" s="27"/>
+      <c r="W9" s="27"/>
     </row>
     <row r="10" spans="6:23" x14ac:dyDescent="0.25">
-      <c r="Q10" s="24"/>
-      <c r="R10" s="24"/>
-      <c r="S10" s="24"/>
-      <c r="T10" s="24"/>
-      <c r="U10" s="24"/>
-      <c r="V10" s="24"/>
-      <c r="W10" s="24"/>
+      <c r="Q10" s="27"/>
+      <c r="R10" s="27"/>
+      <c r="S10" s="27"/>
+      <c r="T10" s="27"/>
+      <c r="U10" s="27"/>
+      <c r="V10" s="27"/>
+      <c r="W10" s="27"/>
     </row>
     <row r="11" spans="6:23" x14ac:dyDescent="0.25">
-      <c r="Q11" s="24"/>
-      <c r="R11" s="24"/>
-      <c r="S11" s="24"/>
-      <c r="T11" s="24"/>
-      <c r="U11" s="24"/>
-      <c r="V11" s="24"/>
-      <c r="W11" s="24"/>
+      <c r="Q11" s="27"/>
+      <c r="R11" s="27"/>
+      <c r="S11" s="27"/>
+      <c r="T11" s="27"/>
+      <c r="U11" s="27"/>
+      <c r="V11" s="27"/>
+      <c r="W11" s="27"/>
     </row>
     <row r="13" spans="6:23" x14ac:dyDescent="0.25">
-      <c r="Q13" s="25" t="s">
+      <c r="Q13" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="R13" s="25"/>
-      <c r="S13" s="25"/>
-      <c r="T13" s="25"/>
-      <c r="U13" s="25"/>
-      <c r="V13" s="25"/>
-      <c r="W13" s="25"/>
+      <c r="R13" s="28"/>
+      <c r="S13" s="28"/>
+      <c r="T13" s="28"/>
+      <c r="U13" s="28"/>
+      <c r="V13" s="28"/>
+      <c r="W13" s="28"/>
     </row>
     <row r="14" spans="6:23" x14ac:dyDescent="0.25">
-      <c r="Q14" s="25"/>
-      <c r="R14" s="25"/>
-      <c r="S14" s="25"/>
-      <c r="T14" s="25"/>
-      <c r="U14" s="25"/>
-      <c r="V14" s="25"/>
-      <c r="W14" s="25"/>
+      <c r="Q14" s="28"/>
+      <c r="R14" s="28"/>
+      <c r="S14" s="28"/>
+      <c r="T14" s="28"/>
+      <c r="U14" s="28"/>
+      <c r="V14" s="28"/>
+      <c r="W14" s="28"/>
     </row>
     <row r="15" spans="6:23" x14ac:dyDescent="0.25">
-      <c r="Q15" s="25"/>
-      <c r="R15" s="25"/>
-      <c r="S15" s="25"/>
-      <c r="T15" s="25"/>
-      <c r="U15" s="25"/>
-      <c r="V15" s="25"/>
-      <c r="W15" s="25"/>
+      <c r="Q15" s="28"/>
+      <c r="R15" s="28"/>
+      <c r="S15" s="28"/>
+      <c r="T15" s="28"/>
+      <c r="U15" s="28"/>
+      <c r="V15" s="28"/>
+      <c r="W15" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -8575,550 +8968,2857 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N30"/>
+  <dimension ref="A1:N165"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
+      <selection activeCell="D62" sqref="D62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.42578125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" s="55" t="s">
+      <c r="A1" s="56" t="s">
         <v>205</v>
       </c>
-      <c r="B1" s="55"/>
-      <c r="C1" s="55"/>
-      <c r="D1" s="55"/>
-      <c r="E1" s="55"/>
-      <c r="F1" s="55"/>
-      <c r="G1" s="55"/>
-      <c r="H1" s="55"/>
-      <c r="I1" s="55"/>
-      <c r="J1" s="55"/>
-      <c r="K1" s="55"/>
-      <c r="L1" s="55"/>
-      <c r="M1" s="55"/>
-      <c r="N1" s="55"/>
+      <c r="B1" s="56"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
+      <c r="G1" s="56"/>
+      <c r="H1" s="56"/>
+      <c r="I1" s="56"/>
+      <c r="J1" s="56"/>
+      <c r="K1" s="56"/>
+      <c r="L1" s="56"/>
+      <c r="M1" s="56"/>
+      <c r="N1" s="56"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="55"/>
-      <c r="B2" s="55"/>
-      <c r="C2" s="55"/>
-      <c r="D2" s="55"/>
-      <c r="E2" s="55"/>
-      <c r="F2" s="55"/>
-      <c r="G2" s="55"/>
-      <c r="H2" s="55"/>
-      <c r="I2" s="55"/>
-      <c r="J2" s="55"/>
-      <c r="K2" s="55"/>
-      <c r="L2" s="55"/>
-      <c r="M2" s="55"/>
-      <c r="N2" s="55"/>
+      <c r="A2" s="56"/>
+      <c r="B2" s="56"/>
+      <c r="C2" s="56"/>
+      <c r="D2" s="56"/>
+      <c r="E2" s="56"/>
+      <c r="F2" s="56"/>
+      <c r="G2" s="56"/>
+      <c r="H2" s="56"/>
+      <c r="I2" s="56"/>
+      <c r="J2" s="56"/>
+      <c r="K2" s="56"/>
+      <c r="L2" s="56"/>
+      <c r="M2" s="56"/>
+      <c r="N2" s="56"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" s="50"/>
-      <c r="B3" s="50"/>
-      <c r="C3" s="50"/>
-      <c r="D3" s="50"/>
-      <c r="E3" s="50"/>
-      <c r="F3" s="50"/>
-      <c r="G3" s="50"/>
-      <c r="H3" s="50"/>
-      <c r="I3" s="50"/>
-      <c r="J3" s="50"/>
-      <c r="K3" s="50"/>
-      <c r="L3" s="50"/>
-      <c r="M3" s="50"/>
-      <c r="N3" s="50"/>
+      <c r="A3" s="24"/>
+      <c r="B3" s="24"/>
+      <c r="C3" s="24"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="24"/>
+      <c r="F3" s="24"/>
+      <c r="G3" s="24"/>
+      <c r="H3" s="24"/>
+      <c r="I3" s="24"/>
+      <c r="J3" s="24"/>
+      <c r="K3" s="24"/>
+      <c r="L3" s="24"/>
+      <c r="M3" s="24"/>
+      <c r="N3" s="24"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="50"/>
-      <c r="B4" s="50"/>
-      <c r="C4" s="50"/>
-      <c r="D4" s="50"/>
-      <c r="E4" s="50"/>
-      <c r="F4" s="50"/>
-      <c r="G4" s="50"/>
-      <c r="H4" s="50"/>
-      <c r="I4" s="50"/>
-      <c r="J4" s="50"/>
-      <c r="K4" s="50"/>
-      <c r="L4" s="50"/>
-      <c r="M4" s="50"/>
-      <c r="N4" s="50"/>
+      <c r="A4" s="24"/>
+      <c r="B4" s="24"/>
+      <c r="C4" s="24"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="24"/>
+      <c r="H4" s="24"/>
+      <c r="I4" s="24"/>
+      <c r="J4" s="24"/>
+      <c r="K4" s="24"/>
+      <c r="L4" s="24"/>
+      <c r="M4" s="24"/>
+      <c r="N4" s="24"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" s="50"/>
-      <c r="B5" s="50"/>
-      <c r="C5" s="54" t="s">
+      <c r="A5" s="24"/>
+      <c r="B5" s="24"/>
+      <c r="C5" s="25" t="s">
         <v>208</v>
       </c>
-      <c r="D5" s="50"/>
-      <c r="E5" s="50"/>
-      <c r="F5" s="51" t="s">
+      <c r="D5" s="24"/>
+      <c r="E5" s="24"/>
+      <c r="F5" s="57" t="s">
         <v>206</v>
       </c>
-      <c r="G5" s="52"/>
-      <c r="H5" s="52"/>
-      <c r="I5" s="53"/>
-      <c r="J5" s="50"/>
-      <c r="K5" s="50"/>
-      <c r="L5" s="50"/>
-      <c r="M5" s="50"/>
-      <c r="N5" s="50"/>
+      <c r="G5" s="58"/>
+      <c r="H5" s="58"/>
+      <c r="I5" s="59"/>
+      <c r="J5" s="24"/>
+      <c r="K5" s="24"/>
+      <c r="L5" s="24"/>
+      <c r="M5" s="24"/>
+      <c r="N5" s="24"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="50"/>
-      <c r="B6" s="50"/>
-      <c r="C6" s="54" t="s">
+      <c r="A6" s="24"/>
+      <c r="B6" s="24"/>
+      <c r="C6" s="25" t="s">
         <v>209</v>
       </c>
-      <c r="D6" s="50"/>
-      <c r="E6" s="50"/>
-      <c r="F6" s="51" t="s">
+      <c r="D6" s="24"/>
+      <c r="E6" s="24"/>
+      <c r="F6" s="57" t="s">
         <v>207</v>
       </c>
-      <c r="G6" s="52"/>
-      <c r="H6" s="52"/>
-      <c r="I6" s="53"/>
-      <c r="J6" s="50"/>
-      <c r="K6" s="50"/>
-      <c r="L6" s="50"/>
-      <c r="M6" s="50"/>
-      <c r="N6" s="50"/>
+      <c r="G6" s="58"/>
+      <c r="H6" s="58"/>
+      <c r="I6" s="59"/>
+      <c r="J6" s="24"/>
+      <c r="K6" s="24"/>
+      <c r="L6" s="24"/>
+      <c r="M6" s="24"/>
+      <c r="N6" s="24"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" s="50"/>
-      <c r="B7" s="50"/>
-      <c r="C7" s="54" t="s">
+      <c r="A7" s="24"/>
+      <c r="B7" s="24"/>
+      <c r="C7" s="25" t="s">
         <v>76</v>
       </c>
-      <c r="D7" s="50"/>
-      <c r="E7" s="50"/>
-      <c r="F7" s="51" t="s">
+      <c r="D7" s="24"/>
+      <c r="E7" s="24"/>
+      <c r="F7" s="57" t="s">
         <v>211</v>
       </c>
-      <c r="G7" s="52"/>
-      <c r="H7" s="52"/>
-      <c r="I7" s="53"/>
-      <c r="J7" s="50"/>
-      <c r="K7" s="50"/>
-      <c r="L7" s="50"/>
-      <c r="M7" s="50"/>
-      <c r="N7" s="50"/>
+      <c r="G7" s="58"/>
+      <c r="H7" s="58"/>
+      <c r="I7" s="59"/>
+      <c r="J7" s="24"/>
+      <c r="K7" s="24"/>
+      <c r="L7" s="24"/>
+      <c r="M7" s="24"/>
+      <c r="N7" s="24"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="50"/>
-      <c r="B8" s="50"/>
-      <c r="C8" s="54" t="s">
+      <c r="A8" s="24"/>
+      <c r="B8" s="24"/>
+      <c r="C8" s="25" t="s">
         <v>210</v>
       </c>
-      <c r="D8" s="50"/>
-      <c r="E8" s="50"/>
-      <c r="F8" s="51" t="s">
+      <c r="D8" s="24"/>
+      <c r="E8" s="24"/>
+      <c r="F8" s="57" t="s">
         <v>212</v>
       </c>
-      <c r="G8" s="52"/>
-      <c r="H8" s="52"/>
-      <c r="I8" s="53"/>
-      <c r="J8" s="50"/>
-      <c r="K8" s="50"/>
-      <c r="L8" s="50"/>
-      <c r="M8" s="50"/>
-      <c r="N8" s="50"/>
+      <c r="G8" s="58"/>
+      <c r="H8" s="58"/>
+      <c r="I8" s="59"/>
+      <c r="J8" s="24"/>
+      <c r="K8" s="24"/>
+      <c r="L8" s="24"/>
+      <c r="M8" s="24"/>
+      <c r="N8" s="24"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="50"/>
-      <c r="B9" s="50"/>
-      <c r="C9" s="50"/>
-      <c r="D9" s="50"/>
-      <c r="E9" s="50"/>
-      <c r="F9" s="50"/>
-      <c r="G9" s="50"/>
-      <c r="H9" s="50"/>
-      <c r="I9" s="50"/>
-      <c r="J9" s="50"/>
-      <c r="K9" s="50"/>
-      <c r="L9" s="50"/>
-      <c r="M9" s="50"/>
-      <c r="N9" s="50"/>
+      <c r="A9" s="24"/>
+      <c r="B9" s="24"/>
+      <c r="C9" s="24"/>
+      <c r="D9" s="24"/>
+      <c r="E9" s="24"/>
+      <c r="F9" s="24"/>
+      <c r="G9" s="24"/>
+      <c r="H9" s="24"/>
+      <c r="I9" s="24"/>
+      <c r="J9" s="24"/>
+      <c r="K9" s="24"/>
+      <c r="L9" s="24"/>
+      <c r="M9" s="24"/>
+      <c r="N9" s="24"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" s="50"/>
-      <c r="B10" s="50"/>
-      <c r="C10" s="50"/>
-      <c r="D10" s="50"/>
-      <c r="E10" s="50"/>
-      <c r="F10" s="50"/>
-      <c r="G10" s="50"/>
-      <c r="H10" s="50"/>
-      <c r="I10" s="50"/>
-      <c r="J10" s="50"/>
-      <c r="K10" s="50"/>
-      <c r="L10" s="50"/>
-      <c r="M10" s="50"/>
-      <c r="N10" s="50"/>
+      <c r="A10" s="24"/>
+      <c r="B10" s="24"/>
+      <c r="C10" s="24"/>
+      <c r="D10" s="24"/>
+      <c r="E10" s="24"/>
+      <c r="F10" s="24"/>
+      <c r="G10" s="24"/>
+      <c r="H10" s="24"/>
+      <c r="I10" s="24"/>
+      <c r="J10" s="24"/>
+      <c r="K10" s="24"/>
+      <c r="L10" s="24"/>
+      <c r="M10" s="24"/>
+      <c r="N10" s="24"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" s="50"/>
-      <c r="B11" s="50"/>
-      <c r="C11" s="50"/>
-      <c r="D11" s="50"/>
-      <c r="E11" s="50"/>
-      <c r="F11" s="50"/>
-      <c r="G11" s="50"/>
-      <c r="H11" s="50"/>
-      <c r="I11" s="50"/>
-      <c r="J11" s="50"/>
-      <c r="K11" s="50"/>
-      <c r="L11" s="50"/>
-      <c r="M11" s="50"/>
-      <c r="N11" s="50"/>
+      <c r="A11" s="24"/>
+      <c r="B11" s="24"/>
+      <c r="C11" s="24"/>
+      <c r="D11" s="24"/>
+      <c r="E11" s="24"/>
+      <c r="F11" s="24"/>
+      <c r="G11" s="24"/>
+      <c r="H11" s="24"/>
+      <c r="I11" s="24"/>
+      <c r="J11" s="24"/>
+      <c r="K11" s="24"/>
+      <c r="L11" s="24"/>
+      <c r="M11" s="24"/>
+      <c r="N11" s="24"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" s="50"/>
-      <c r="B12" s="50"/>
-      <c r="C12" s="50"/>
-      <c r="D12" s="50"/>
-      <c r="E12" s="50"/>
-      <c r="F12" s="50"/>
-      <c r="G12" s="50"/>
-      <c r="H12" s="50"/>
-      <c r="I12" s="50"/>
-      <c r="J12" s="50"/>
-      <c r="K12" s="50"/>
-      <c r="L12" s="50"/>
-      <c r="M12" s="50"/>
-      <c r="N12" s="50"/>
+      <c r="A12" s="24"/>
+      <c r="B12" s="24"/>
+      <c r="C12" s="24"/>
+      <c r="D12" s="24"/>
+      <c r="E12" s="24"/>
+      <c r="F12" s="24"/>
+      <c r="G12" s="24"/>
+      <c r="H12" s="24"/>
+      <c r="I12" s="24"/>
+      <c r="J12" s="24"/>
+      <c r="K12" s="24"/>
+      <c r="L12" s="24"/>
+      <c r="M12" s="24"/>
+      <c r="N12" s="24"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A13" s="50"/>
-      <c r="B13" s="50"/>
-      <c r="C13" s="50"/>
-      <c r="D13" s="50"/>
-      <c r="E13" s="50"/>
-      <c r="F13" s="50"/>
-      <c r="G13" s="50"/>
-      <c r="H13" s="50"/>
-      <c r="I13" s="50"/>
-      <c r="J13" s="50"/>
-      <c r="K13" s="50"/>
-      <c r="L13" s="50"/>
-      <c r="M13" s="50"/>
-      <c r="N13" s="50"/>
+      <c r="A13" s="24"/>
+      <c r="B13" s="24"/>
+      <c r="C13" s="24"/>
+      <c r="D13" s="24"/>
+      <c r="E13" s="24"/>
+      <c r="F13" s="24"/>
+      <c r="G13" s="24"/>
+      <c r="H13" s="24"/>
+      <c r="I13" s="24"/>
+      <c r="J13" s="24"/>
+      <c r="K13" s="24"/>
+      <c r="L13" s="24"/>
+      <c r="M13" s="24"/>
+      <c r="N13" s="24"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14" s="50"/>
-      <c r="B14" s="50"/>
-      <c r="C14" s="50"/>
-      <c r="D14" s="50"/>
-      <c r="E14" s="50"/>
-      <c r="F14" s="50"/>
-      <c r="G14" s="50"/>
-      <c r="H14" s="50"/>
-      <c r="I14" s="50"/>
-      <c r="J14" s="50"/>
-      <c r="K14" s="50"/>
-      <c r="L14" s="50"/>
-      <c r="M14" s="50"/>
-      <c r="N14" s="50"/>
+      <c r="A14" s="24"/>
+      <c r="B14" s="24"/>
+      <c r="C14" s="24"/>
+      <c r="D14" s="24"/>
+      <c r="E14" s="24"/>
+      <c r="F14" s="24"/>
+      <c r="G14" s="24"/>
+      <c r="H14" s="24"/>
+      <c r="I14" s="24"/>
+      <c r="J14" s="24"/>
+      <c r="K14" s="24"/>
+      <c r="L14" s="24"/>
+      <c r="M14" s="24"/>
+      <c r="N14" s="24"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" s="55" t="s">
+      <c r="A15" s="56" t="s">
         <v>213</v>
       </c>
-      <c r="B15" s="55"/>
-      <c r="C15" s="55"/>
-      <c r="D15" s="55"/>
-      <c r="E15" s="55"/>
-      <c r="F15" s="55"/>
-      <c r="G15" s="55"/>
-      <c r="H15" s="55"/>
-      <c r="I15" s="55"/>
-      <c r="J15" s="55"/>
-      <c r="K15" s="55"/>
-      <c r="L15" s="55"/>
-      <c r="M15" s="55"/>
-      <c r="N15" s="55"/>
+      <c r="B15" s="56"/>
+      <c r="C15" s="56"/>
+      <c r="D15" s="56"/>
+      <c r="E15" s="56"/>
+      <c r="F15" s="56"/>
+      <c r="G15" s="56"/>
+      <c r="H15" s="56"/>
+      <c r="I15" s="56"/>
+      <c r="J15" s="56"/>
+      <c r="K15" s="56"/>
+      <c r="L15" s="56"/>
+      <c r="M15" s="56"/>
+      <c r="N15" s="56"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" s="55"/>
-      <c r="B16" s="55"/>
-      <c r="C16" s="55"/>
-      <c r="D16" s="55"/>
-      <c r="E16" s="55"/>
-      <c r="F16" s="55"/>
-      <c r="G16" s="55"/>
-      <c r="H16" s="55"/>
-      <c r="I16" s="55"/>
-      <c r="J16" s="55"/>
-      <c r="K16" s="55"/>
-      <c r="L16" s="55"/>
-      <c r="M16" s="55"/>
-      <c r="N16" s="55"/>
+      <c r="A16" s="56"/>
+      <c r="B16" s="56"/>
+      <c r="C16" s="56"/>
+      <c r="D16" s="56"/>
+      <c r="E16" s="56"/>
+      <c r="F16" s="56"/>
+      <c r="G16" s="56"/>
+      <c r="H16" s="56"/>
+      <c r="I16" s="56"/>
+      <c r="J16" s="56"/>
+      <c r="K16" s="56"/>
+      <c r="L16" s="56"/>
+      <c r="M16" s="56"/>
+      <c r="N16" s="56"/>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A17" s="50"/>
-      <c r="B17" s="50"/>
-      <c r="C17" s="50"/>
-      <c r="D17" s="50"/>
-      <c r="E17" s="50"/>
-      <c r="F17" s="50"/>
-      <c r="G17" s="50"/>
-      <c r="H17" s="50"/>
-      <c r="I17" s="50"/>
-      <c r="J17" s="50"/>
-      <c r="K17" s="50"/>
-      <c r="L17" s="50"/>
-      <c r="M17" s="50"/>
-      <c r="N17" s="50"/>
+      <c r="A17" s="24"/>
+      <c r="B17" s="24"/>
+      <c r="C17" s="24"/>
+      <c r="D17" s="24"/>
+      <c r="E17" s="24"/>
+      <c r="F17" s="24"/>
+      <c r="G17" s="24"/>
+      <c r="H17" s="24"/>
+      <c r="I17" s="24"/>
+      <c r="J17" s="24"/>
+      <c r="K17" s="24"/>
+      <c r="L17" s="24"/>
+      <c r="M17" s="24"/>
+      <c r="N17" s="24"/>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A18" s="50"/>
-      <c r="B18" s="50"/>
-      <c r="C18" s="54" t="s">
+      <c r="A18" s="24"/>
+      <c r="B18" s="24"/>
+      <c r="C18" s="25" t="s">
         <v>104</v>
       </c>
-      <c r="D18" s="50"/>
-      <c r="E18" s="50"/>
-      <c r="F18" s="56" t="s">
+      <c r="D18" s="24"/>
+      <c r="E18" s="24"/>
+      <c r="F18" s="26" t="s">
         <v>215</v>
       </c>
-      <c r="G18" s="57" t="s">
+      <c r="G18" s="53" t="s">
         <v>219</v>
       </c>
-      <c r="H18" s="58"/>
-      <c r="I18" s="58"/>
-      <c r="J18" s="58"/>
-      <c r="K18" s="59"/>
-      <c r="L18" s="50"/>
-      <c r="M18" s="50"/>
-      <c r="N18" s="50"/>
+      <c r="H18" s="54"/>
+      <c r="I18" s="54"/>
+      <c r="J18" s="54"/>
+      <c r="K18" s="55"/>
+      <c r="L18" s="24"/>
+      <c r="M18" s="24"/>
+      <c r="N18" s="24"/>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A19" s="50"/>
-      <c r="B19" s="50"/>
-      <c r="C19" s="50"/>
-      <c r="D19" s="50"/>
-      <c r="E19" s="50"/>
-      <c r="F19" s="56" t="s">
+      <c r="A19" s="24"/>
+      <c r="B19" s="24"/>
+      <c r="C19" s="24"/>
+      <c r="D19" s="24"/>
+      <c r="E19" s="24"/>
+      <c r="F19" s="26" t="s">
         <v>214</v>
       </c>
-      <c r="G19" s="57" t="s">
+      <c r="G19" s="53" t="s">
         <v>220</v>
       </c>
-      <c r="H19" s="58"/>
-      <c r="I19" s="58"/>
-      <c r="J19" s="58"/>
-      <c r="K19" s="59"/>
-      <c r="L19" s="50"/>
-      <c r="M19" s="50"/>
-      <c r="N19" s="50"/>
+      <c r="H19" s="54"/>
+      <c r="I19" s="54"/>
+      <c r="J19" s="54"/>
+      <c r="K19" s="55"/>
+      <c r="L19" s="24"/>
+      <c r="M19" s="24"/>
+      <c r="N19" s="24"/>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A20" s="50"/>
-      <c r="B20" s="50"/>
-      <c r="C20" s="50"/>
-      <c r="D20" s="50"/>
-      <c r="E20" s="50"/>
-      <c r="F20" s="56" t="s">
+      <c r="A20" s="24"/>
+      <c r="B20" s="24"/>
+      <c r="C20" s="24"/>
+      <c r="D20" s="24"/>
+      <c r="E20" s="24"/>
+      <c r="F20" s="26" t="s">
         <v>216</v>
       </c>
-      <c r="G20" s="57" t="s">
+      <c r="G20" s="53" t="s">
         <v>221</v>
       </c>
-      <c r="H20" s="58"/>
-      <c r="I20" s="58"/>
-      <c r="J20" s="58"/>
-      <c r="K20" s="59"/>
-      <c r="L20" s="50"/>
-      <c r="M20" s="50"/>
-      <c r="N20" s="50"/>
+      <c r="H20" s="54"/>
+      <c r="I20" s="54"/>
+      <c r="J20" s="54"/>
+      <c r="K20" s="55"/>
+      <c r="L20" s="24"/>
+      <c r="M20" s="24"/>
+      <c r="N20" s="24"/>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A21" s="50"/>
-      <c r="B21" s="50"/>
-      <c r="C21" s="50"/>
-      <c r="D21" s="50"/>
-      <c r="E21" s="50"/>
-      <c r="F21" s="56" t="s">
+      <c r="A21" s="24"/>
+      <c r="B21" s="24"/>
+      <c r="C21" s="24"/>
+      <c r="D21" s="24"/>
+      <c r="E21" s="24"/>
+      <c r="F21" s="26" t="s">
         <v>217</v>
       </c>
-      <c r="G21" s="57" t="s">
+      <c r="G21" s="53" t="s">
         <v>222</v>
       </c>
-      <c r="H21" s="58"/>
-      <c r="I21" s="58"/>
-      <c r="J21" s="58"/>
-      <c r="K21" s="59"/>
-      <c r="L21" s="50"/>
-      <c r="M21" s="50"/>
-      <c r="N21" s="50"/>
+      <c r="H21" s="54"/>
+      <c r="I21" s="54"/>
+      <c r="J21" s="54"/>
+      <c r="K21" s="55"/>
+      <c r="L21" s="24"/>
+      <c r="M21" s="24"/>
+      <c r="N21" s="24"/>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A22" s="50"/>
-      <c r="B22" s="50"/>
-      <c r="C22" s="50"/>
-      <c r="D22" s="50"/>
-      <c r="E22" s="50"/>
-      <c r="F22" s="56" t="s">
+      <c r="A22" s="24"/>
+      <c r="B22" s="24"/>
+      <c r="C22" s="24"/>
+      <c r="D22" s="24"/>
+      <c r="E22" s="24"/>
+      <c r="F22" s="26" t="s">
         <v>218</v>
       </c>
-      <c r="G22" s="57" t="s">
+      <c r="G22" s="53" t="s">
         <v>223</v>
       </c>
-      <c r="H22" s="58"/>
-      <c r="I22" s="58"/>
-      <c r="J22" s="58"/>
-      <c r="K22" s="59"/>
-      <c r="L22" s="50"/>
-      <c r="M22" s="50"/>
-      <c r="N22" s="50"/>
+      <c r="H22" s="54"/>
+      <c r="I22" s="54"/>
+      <c r="J22" s="54"/>
+      <c r="K22" s="55"/>
+      <c r="L22" s="24"/>
+      <c r="M22" s="24"/>
+      <c r="N22" s="24"/>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A23" s="50"/>
-      <c r="B23" s="50"/>
-      <c r="C23" s="50"/>
-      <c r="D23" s="50"/>
-      <c r="E23" s="50"/>
-      <c r="F23" s="50"/>
-      <c r="G23" s="50"/>
-      <c r="H23" s="50"/>
-      <c r="I23" s="50"/>
-      <c r="J23" s="50"/>
-      <c r="K23" s="50"/>
-      <c r="L23" s="50"/>
-      <c r="M23" s="50"/>
-      <c r="N23" s="50"/>
+      <c r="A23" s="24"/>
+      <c r="B23" s="24"/>
+      <c r="C23" s="24"/>
+      <c r="D23" s="24"/>
+      <c r="E23" s="24"/>
+      <c r="F23" s="24"/>
+      <c r="G23" s="24"/>
+      <c r="H23" s="24"/>
+      <c r="I23" s="24"/>
+      <c r="J23" s="24"/>
+      <c r="K23" s="24"/>
+      <c r="L23" s="24"/>
+      <c r="M23" s="24"/>
+      <c r="N23" s="24"/>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A24" s="50"/>
-      <c r="B24" s="50"/>
-      <c r="C24" s="54" t="s">
+      <c r="A24" s="24"/>
+      <c r="B24" s="24"/>
+      <c r="C24" s="25" t="s">
         <v>224</v>
       </c>
-      <c r="D24" s="50"/>
-      <c r="E24" s="50"/>
-      <c r="F24" s="50" t="s">
+      <c r="D24" s="24"/>
+      <c r="E24" s="24"/>
+      <c r="F24" s="24" t="s">
         <v>225</v>
       </c>
-      <c r="G24" s="57" t="s">
+      <c r="G24" s="60" t="s">
         <v>229</v>
       </c>
-      <c r="H24" s="58"/>
-      <c r="I24" s="58"/>
-      <c r="J24" s="58"/>
-      <c r="K24" s="59"/>
-      <c r="L24" s="50"/>
-      <c r="M24" s="50"/>
-      <c r="N24" s="50"/>
+      <c r="H24" s="61"/>
+      <c r="I24" s="61"/>
+      <c r="J24" s="61"/>
+      <c r="K24" s="62"/>
+      <c r="L24" s="24"/>
+      <c r="M24" s="24"/>
+      <c r="N24" s="24"/>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A25" s="50"/>
-      <c r="B25" s="50"/>
-      <c r="C25" s="50"/>
-      <c r="D25" s="50"/>
-      <c r="E25" s="50"/>
-      <c r="F25" s="50" t="s">
+      <c r="A25" s="24"/>
+      <c r="B25" s="24"/>
+      <c r="C25" s="24"/>
+      <c r="D25" s="24"/>
+      <c r="E25" s="24"/>
+      <c r="F25" s="24" t="s">
         <v>226</v>
       </c>
-      <c r="G25" s="50"/>
-      <c r="H25" s="50"/>
-      <c r="I25" s="50"/>
-      <c r="J25" s="50"/>
-      <c r="K25" s="50"/>
-      <c r="L25" s="50"/>
-      <c r="M25" s="50"/>
-      <c r="N25" s="50"/>
+      <c r="G25" s="53" t="s">
+        <v>230</v>
+      </c>
+      <c r="H25" s="54"/>
+      <c r="I25" s="54"/>
+      <c r="J25" s="54"/>
+      <c r="K25" s="55"/>
+      <c r="L25" s="24"/>
+      <c r="M25" s="24"/>
+      <c r="N25" s="24"/>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A26" s="50"/>
-      <c r="B26" s="50"/>
-      <c r="C26" s="50"/>
-      <c r="D26" s="50"/>
-      <c r="E26" s="50"/>
-      <c r="F26" s="50" t="s">
+      <c r="A26" s="24"/>
+      <c r="B26" s="24"/>
+      <c r="C26" s="24"/>
+      <c r="D26" s="24"/>
+      <c r="E26" s="24"/>
+      <c r="F26" s="24" t="s">
         <v>227</v>
       </c>
-      <c r="G26" s="50"/>
-      <c r="H26" s="50"/>
-      <c r="I26" s="50"/>
-      <c r="J26" s="50"/>
-      <c r="K26" s="50"/>
-      <c r="L26" s="50"/>
-      <c r="M26" s="50"/>
-      <c r="N26" s="50"/>
+      <c r="G26" s="53" t="s">
+        <v>232</v>
+      </c>
+      <c r="H26" s="54"/>
+      <c r="I26" s="54"/>
+      <c r="J26" s="54"/>
+      <c r="K26" s="55"/>
+      <c r="L26" s="24"/>
+      <c r="M26" s="24"/>
+      <c r="N26" s="24"/>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A27" s="50"/>
-      <c r="B27" s="50"/>
-      <c r="C27" s="50"/>
-      <c r="D27" s="50"/>
-      <c r="E27" s="50"/>
-      <c r="F27" s="50" t="s">
+      <c r="A27" s="24"/>
+      <c r="B27" s="24"/>
+      <c r="C27" s="24"/>
+      <c r="D27" s="24"/>
+      <c r="E27" s="24"/>
+      <c r="F27" s="24" t="s">
         <v>228</v>
       </c>
-      <c r="G27" s="50"/>
-      <c r="H27" s="50"/>
-      <c r="I27" s="50"/>
-      <c r="J27" s="50"/>
-      <c r="K27" s="50"/>
-      <c r="L27" s="50"/>
-      <c r="M27" s="50"/>
-      <c r="N27" s="50"/>
+      <c r="G27" s="53" t="s">
+        <v>231</v>
+      </c>
+      <c r="H27" s="54"/>
+      <c r="I27" s="54"/>
+      <c r="J27" s="54"/>
+      <c r="K27" s="55"/>
+      <c r="L27" s="24"/>
+      <c r="M27" s="24"/>
+      <c r="N27" s="24"/>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A28" s="50"/>
-      <c r="B28" s="50"/>
-      <c r="C28" s="50"/>
-      <c r="D28" s="50"/>
-      <c r="E28" s="50"/>
-      <c r="F28" s="50"/>
-      <c r="G28" s="50"/>
-      <c r="H28" s="50"/>
-      <c r="I28" s="50"/>
-      <c r="J28" s="50"/>
-      <c r="K28" s="50"/>
-      <c r="L28" s="50"/>
-      <c r="M28" s="50"/>
-      <c r="N28" s="50"/>
+      <c r="A28" s="24"/>
+      <c r="B28" s="24"/>
+      <c r="C28" s="24"/>
+      <c r="D28" s="24"/>
+      <c r="E28" s="24"/>
+      <c r="F28" s="24"/>
+      <c r="G28" s="24"/>
+      <c r="H28" s="24"/>
+      <c r="I28" s="24"/>
+      <c r="J28" s="24"/>
+      <c r="K28" s="24"/>
+      <c r="L28" s="24"/>
+      <c r="M28" s="24"/>
+      <c r="N28" s="24"/>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A29" s="50"/>
-      <c r="B29" s="50"/>
-      <c r="C29" s="50"/>
-      <c r="D29" s="50"/>
-      <c r="E29" s="50"/>
-      <c r="F29" s="50"/>
-      <c r="G29" s="50"/>
-      <c r="H29" s="50"/>
-      <c r="I29" s="50"/>
-      <c r="J29" s="50"/>
-      <c r="K29" s="50"/>
-      <c r="L29" s="50"/>
-      <c r="M29" s="50"/>
-      <c r="N29" s="50"/>
+      <c r="A29" s="24"/>
+      <c r="B29" s="24"/>
+      <c r="C29" s="24"/>
+      <c r="D29" s="24"/>
+      <c r="E29" s="24"/>
+      <c r="F29" s="24"/>
+      <c r="G29" s="24"/>
+      <c r="H29" s="24"/>
+      <c r="I29" s="24"/>
+      <c r="J29" s="24"/>
+      <c r="K29" s="24"/>
+      <c r="L29" s="24"/>
+      <c r="M29" s="24"/>
+      <c r="N29" s="24"/>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A30" s="50"/>
-      <c r="B30" s="50"/>
-      <c r="C30" s="50"/>
-      <c r="D30" s="50"/>
-      <c r="E30" s="50"/>
-      <c r="F30" s="50"/>
-      <c r="G30" s="50"/>
-      <c r="H30" s="50"/>
-      <c r="I30" s="50"/>
-      <c r="J30" s="50"/>
-      <c r="K30" s="50"/>
-      <c r="L30" s="50"/>
-      <c r="M30" s="50"/>
-      <c r="N30" s="50"/>
+      <c r="A30" s="24"/>
+      <c r="B30" s="24"/>
+      <c r="C30" s="24"/>
+      <c r="D30" s="24"/>
+      <c r="E30" s="24"/>
+      <c r="F30" s="24"/>
+      <c r="G30" s="24"/>
+      <c r="H30" s="24"/>
+      <c r="I30" s="24"/>
+      <c r="J30" s="24"/>
+      <c r="K30" s="24"/>
+      <c r="L30" s="24"/>
+      <c r="M30" s="24"/>
+      <c r="N30" s="24"/>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A31" s="56" t="s">
+        <v>233</v>
+      </c>
+      <c r="B31" s="56"/>
+      <c r="C31" s="56"/>
+      <c r="D31" s="56"/>
+      <c r="E31" s="56"/>
+      <c r="F31" s="56"/>
+      <c r="G31" s="56"/>
+      <c r="H31" s="56"/>
+      <c r="I31" s="56"/>
+      <c r="J31" s="56"/>
+      <c r="K31" s="56"/>
+      <c r="L31" s="56"/>
+      <c r="M31" s="56"/>
+      <c r="N31" s="56"/>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A32" s="56"/>
+      <c r="B32" s="56"/>
+      <c r="C32" s="56"/>
+      <c r="D32" s="56"/>
+      <c r="E32" s="56"/>
+      <c r="F32" s="56"/>
+      <c r="G32" s="56"/>
+      <c r="H32" s="56"/>
+      <c r="I32" s="56"/>
+      <c r="J32" s="56"/>
+      <c r="K32" s="56"/>
+      <c r="L32" s="56"/>
+      <c r="M32" s="56"/>
+      <c r="N32" s="56"/>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A33" s="63"/>
+      <c r="B33" s="63"/>
+      <c r="C33" s="63"/>
+      <c r="D33" s="63"/>
+      <c r="E33" s="63"/>
+      <c r="F33" s="63"/>
+      <c r="G33" s="63"/>
+      <c r="H33" s="63"/>
+      <c r="I33" s="63"/>
+      <c r="J33" s="63"/>
+      <c r="K33" s="63"/>
+      <c r="L33" s="63"/>
+      <c r="M33" s="63"/>
+      <c r="N33" s="63"/>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A34" s="63"/>
+      <c r="B34" s="65"/>
+      <c r="C34" s="65"/>
+      <c r="D34" s="65"/>
+      <c r="E34" s="65"/>
+      <c r="F34" s="65"/>
+      <c r="G34" s="65"/>
+      <c r="H34" s="63"/>
+      <c r="I34" s="63"/>
+      <c r="J34" s="63"/>
+      <c r="K34" s="63"/>
+      <c r="L34" s="63"/>
+      <c r="M34" s="63"/>
+      <c r="N34" s="63"/>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A35" s="63"/>
+      <c r="B35" s="69" t="s">
+        <v>234</v>
+      </c>
+      <c r="C35" s="63">
+        <v>14</v>
+      </c>
+      <c r="D35" s="63"/>
+      <c r="E35" s="68" t="s">
+        <v>234</v>
+      </c>
+      <c r="F35" s="68" t="s">
+        <v>76</v>
+      </c>
+      <c r="G35" s="67" t="s">
+        <v>245</v>
+      </c>
+      <c r="H35" s="67"/>
+      <c r="I35" s="67"/>
+      <c r="J35" s="67"/>
+      <c r="K35" s="63"/>
+      <c r="L35" s="63"/>
+      <c r="M35" s="63"/>
+      <c r="N35" s="63"/>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A36" s="63"/>
+      <c r="B36" s="63"/>
+      <c r="C36" s="63"/>
+      <c r="D36" s="63"/>
+      <c r="E36" s="63"/>
+      <c r="F36" s="63"/>
+      <c r="G36" s="63">
+        <v>2015</v>
+      </c>
+      <c r="H36" s="63">
+        <v>200</v>
+      </c>
+      <c r="I36" s="63">
+        <v>1960</v>
+      </c>
+      <c r="J36" s="63">
+        <v>1945</v>
+      </c>
+      <c r="K36" s="63"/>
+      <c r="L36" s="63"/>
+      <c r="M36" s="63"/>
+      <c r="N36" s="63"/>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A37" s="63"/>
+      <c r="B37" s="69" t="s">
+        <v>246</v>
+      </c>
+      <c r="C37" s="63">
+        <v>45</v>
+      </c>
+      <c r="D37" s="63"/>
+      <c r="E37" s="63" t="s">
+        <v>190</v>
+      </c>
+      <c r="F37" s="63">
+        <v>550</v>
+      </c>
+      <c r="G37" s="66">
+        <v>2411528</v>
+      </c>
+      <c r="H37" s="63"/>
+      <c r="I37" s="63"/>
+      <c r="J37" s="63"/>
+      <c r="K37" s="63"/>
+      <c r="L37" s="63"/>
+      <c r="M37" s="63"/>
+      <c r="N37" s="63"/>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A38" s="63"/>
+      <c r="B38" s="63"/>
+      <c r="C38" s="63"/>
+      <c r="D38" s="63"/>
+      <c r="E38" s="63" t="s">
+        <v>235</v>
+      </c>
+      <c r="F38" s="66">
+        <v>4359</v>
+      </c>
+      <c r="G38" s="66">
+        <v>930008</v>
+      </c>
+      <c r="H38" s="63"/>
+      <c r="I38" s="63"/>
+      <c r="J38" s="63"/>
+      <c r="K38" s="63"/>
+      <c r="L38" s="63"/>
+      <c r="M38" s="63"/>
+      <c r="N38" s="63"/>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A39" s="63"/>
+      <c r="B39" s="69" t="s">
+        <v>250</v>
+      </c>
+      <c r="C39" s="63"/>
+      <c r="D39" s="63"/>
+      <c r="E39" s="63" t="s">
+        <v>236</v>
+      </c>
+      <c r="F39" s="66">
+        <v>7935</v>
+      </c>
+      <c r="G39" s="66">
+        <v>639075</v>
+      </c>
+      <c r="H39" s="63"/>
+      <c r="I39" s="63"/>
+      <c r="J39" s="63"/>
+      <c r="K39" s="63"/>
+      <c r="L39" s="63"/>
+      <c r="M39" s="63"/>
+      <c r="N39" s="63"/>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A40" s="63"/>
+      <c r="B40" s="63"/>
+      <c r="C40" s="63"/>
+      <c r="D40" s="63"/>
+      <c r="E40" s="63" t="s">
+        <v>237</v>
+      </c>
+      <c r="F40" s="66">
+        <v>16010</v>
+      </c>
+      <c r="G40" s="66">
+        <v>1128128</v>
+      </c>
+      <c r="H40" s="63"/>
+      <c r="I40" s="63"/>
+      <c r="J40" s="63"/>
+      <c r="K40" s="63"/>
+      <c r="L40" s="63"/>
+      <c r="M40" s="63"/>
+      <c r="N40" s="63"/>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A41" s="63"/>
+      <c r="B41" s="69" t="s">
+        <v>248</v>
+      </c>
+      <c r="C41" s="63">
+        <v>46</v>
+      </c>
+      <c r="D41" s="63"/>
+      <c r="E41" s="63" t="s">
+        <v>238</v>
+      </c>
+      <c r="F41" s="66">
+        <v>21011</v>
+      </c>
+      <c r="G41" s="66">
+        <v>834753</v>
+      </c>
+      <c r="H41" s="63"/>
+      <c r="I41" s="63"/>
+      <c r="J41" s="63"/>
+      <c r="K41" s="63"/>
+      <c r="L41" s="63"/>
+      <c r="M41" s="63"/>
+      <c r="N41" s="63"/>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A42" s="63"/>
+      <c r="B42" s="63"/>
+      <c r="C42" s="63"/>
+      <c r="D42" s="63"/>
+      <c r="E42" s="63" t="s">
+        <v>239</v>
+      </c>
+      <c r="F42" s="66">
+        <v>29188</v>
+      </c>
+      <c r="G42" s="66">
+        <v>559268</v>
+      </c>
+      <c r="H42" s="63"/>
+      <c r="I42" s="63"/>
+      <c r="J42" s="63"/>
+      <c r="K42" s="63"/>
+      <c r="L42" s="63"/>
+      <c r="M42" s="63"/>
+      <c r="N42" s="63"/>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A43" s="63"/>
+      <c r="B43" s="69" t="s">
+        <v>247</v>
+      </c>
+      <c r="C43" s="63">
+        <v>346</v>
+      </c>
+      <c r="D43" s="63"/>
+      <c r="E43" s="63" t="s">
+        <v>240</v>
+      </c>
+      <c r="F43" s="66">
+        <v>25083</v>
+      </c>
+      <c r="G43" s="66">
+        <v>423041</v>
+      </c>
+      <c r="H43" s="63"/>
+      <c r="I43" s="63"/>
+      <c r="J43" s="63"/>
+      <c r="K43" s="63"/>
+      <c r="L43" s="63"/>
+      <c r="M43" s="63"/>
+      <c r="N43" s="63"/>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A44" s="63"/>
+      <c r="B44" s="63"/>
+      <c r="C44" s="63"/>
+      <c r="D44" s="63"/>
+      <c r="E44" s="63" t="s">
+        <v>241</v>
+      </c>
+      <c r="F44" s="66">
+        <v>19044</v>
+      </c>
+      <c r="G44" s="66">
+        <v>863440</v>
+      </c>
+      <c r="H44" s="63"/>
+      <c r="I44" s="63"/>
+      <c r="J44" s="63"/>
+      <c r="K44" s="63"/>
+      <c r="L44" s="63"/>
+      <c r="M44" s="63"/>
+      <c r="N44" s="63"/>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A45" s="63"/>
+      <c r="B45" s="69" t="s">
+        <v>249</v>
+      </c>
+      <c r="C45" s="63" t="s">
+        <v>251</v>
+      </c>
+      <c r="D45" s="63"/>
+      <c r="E45" s="63" t="s">
+        <v>242</v>
+      </c>
+      <c r="F45" s="66">
+        <v>59602</v>
+      </c>
+      <c r="G45" s="66">
+        <v>530332</v>
+      </c>
+      <c r="H45" s="63"/>
+      <c r="I45" s="63"/>
+      <c r="J45" s="63"/>
+      <c r="K45" s="63"/>
+      <c r="L45" s="63"/>
+      <c r="M45" s="63"/>
+      <c r="N45" s="63"/>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A46" s="63"/>
+      <c r="B46" s="63"/>
+      <c r="C46" s="63" t="s">
+        <v>252</v>
+      </c>
+      <c r="D46" s="63"/>
+      <c r="E46" s="63" t="s">
+        <v>243</v>
+      </c>
+      <c r="F46" s="66">
+        <v>6601</v>
+      </c>
+      <c r="G46" s="66">
+        <v>1348637</v>
+      </c>
+      <c r="H46" s="63"/>
+      <c r="I46" s="63"/>
+      <c r="J46" s="63"/>
+      <c r="K46" s="63"/>
+      <c r="L46" s="63"/>
+      <c r="M46" s="63"/>
+      <c r="N46" s="63"/>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A47" s="63"/>
+      <c r="B47" s="63"/>
+      <c r="C47" s="63"/>
+      <c r="D47" s="63"/>
+      <c r="E47" s="63" t="s">
+        <v>244</v>
+      </c>
+      <c r="F47" s="66">
+        <v>7339</v>
+      </c>
+      <c r="G47" s="66">
+        <v>557606</v>
+      </c>
+      <c r="H47" s="63"/>
+      <c r="I47" s="63"/>
+      <c r="J47" s="63"/>
+      <c r="K47" s="63"/>
+      <c r="L47" s="63"/>
+      <c r="M47" s="63"/>
+      <c r="N47" s="63"/>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A48" s="63"/>
+      <c r="B48" s="63"/>
+      <c r="C48" s="63"/>
+      <c r="D48" s="63"/>
+      <c r="E48" s="63"/>
+      <c r="F48" s="63"/>
+      <c r="G48" s="63"/>
+      <c r="H48" s="63"/>
+      <c r="I48" s="63"/>
+      <c r="J48" s="63"/>
+      <c r="K48" s="63"/>
+      <c r="L48" s="63"/>
+      <c r="M48" s="63"/>
+      <c r="N48" s="63"/>
+    </row>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A49" s="63"/>
+      <c r="B49" s="63"/>
+      <c r="C49" s="63"/>
+      <c r="D49" s="63"/>
+      <c r="E49" s="63"/>
+      <c r="F49" s="63"/>
+      <c r="G49" s="63"/>
+      <c r="H49" s="63"/>
+      <c r="I49" s="63"/>
+      <c r="J49" s="63"/>
+      <c r="K49" s="63"/>
+      <c r="L49" s="63"/>
+      <c r="M49" s="63"/>
+      <c r="N49" s="63"/>
+    </row>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A50" s="63"/>
+      <c r="B50" s="63"/>
+      <c r="C50" s="63"/>
+      <c r="D50" s="63"/>
+      <c r="E50" s="63"/>
+      <c r="F50" s="63"/>
+      <c r="G50" s="63"/>
+      <c r="H50" s="63"/>
+      <c r="I50" s="63"/>
+      <c r="J50" s="63"/>
+      <c r="K50" s="63"/>
+      <c r="L50" s="63"/>
+      <c r="M50" s="63"/>
+      <c r="N50" s="63"/>
+    </row>
+    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A51" s="56" t="s">
+        <v>253</v>
+      </c>
+      <c r="B51" s="56"/>
+      <c r="C51" s="56"/>
+      <c r="D51" s="56"/>
+      <c r="E51" s="56"/>
+      <c r="F51" s="56"/>
+      <c r="G51" s="56"/>
+      <c r="H51" s="56"/>
+      <c r="I51" s="56"/>
+      <c r="J51" s="56"/>
+      <c r="K51" s="56"/>
+      <c r="L51" s="56"/>
+      <c r="M51" s="56"/>
+      <c r="N51" s="56"/>
+    </row>
+    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A52" s="56"/>
+      <c r="B52" s="56"/>
+      <c r="C52" s="56"/>
+      <c r="D52" s="56"/>
+      <c r="E52" s="56"/>
+      <c r="F52" s="56"/>
+      <c r="G52" s="56"/>
+      <c r="H52" s="56"/>
+      <c r="I52" s="56"/>
+      <c r="J52" s="56"/>
+      <c r="K52" s="56"/>
+      <c r="L52" s="56"/>
+      <c r="M52" s="56"/>
+      <c r="N52" s="56"/>
+    </row>
+    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A53" s="63"/>
+      <c r="B53" s="63"/>
+      <c r="C53" s="63"/>
+      <c r="D53" s="63"/>
+      <c r="E53" s="63"/>
+      <c r="F53" s="63"/>
+      <c r="G53" s="63"/>
+      <c r="H53" s="63"/>
+      <c r="I53" s="63"/>
+      <c r="J53" s="63"/>
+      <c r="K53" s="63"/>
+      <c r="L53" s="63"/>
+      <c r="M53" s="63"/>
+      <c r="N53" s="63"/>
+    </row>
+    <row r="54" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A54" s="63"/>
+      <c r="B54" s="70" t="s">
+        <v>255</v>
+      </c>
+      <c r="C54" s="63"/>
+      <c r="D54" s="64" t="s">
+        <v>261</v>
+      </c>
+      <c r="E54" s="63"/>
+      <c r="F54" s="63"/>
+      <c r="G54" s="63"/>
+      <c r="H54" s="63"/>
+      <c r="I54" s="63"/>
+      <c r="J54" s="63"/>
+      <c r="K54" s="63"/>
+      <c r="L54" s="63"/>
+      <c r="M54" s="63"/>
+      <c r="N54" s="63"/>
+    </row>
+    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A55" s="63"/>
+      <c r="B55" s="63"/>
+      <c r="C55" s="63"/>
+      <c r="D55" s="63" t="s">
+        <v>257</v>
+      </c>
+      <c r="E55" s="63"/>
+      <c r="F55" s="63"/>
+      <c r="G55" s="63"/>
+      <c r="H55" s="63"/>
+      <c r="I55" s="63"/>
+      <c r="J55" s="63"/>
+      <c r="K55" s="63"/>
+      <c r="L55" s="63"/>
+      <c r="M55" s="63"/>
+      <c r="N55" s="63"/>
+    </row>
+    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A56" s="63"/>
+      <c r="B56" s="63"/>
+      <c r="C56" s="63"/>
+      <c r="D56" s="63" t="s">
+        <v>258</v>
+      </c>
+      <c r="E56" s="63"/>
+      <c r="F56" s="63"/>
+      <c r="G56" s="63"/>
+      <c r="H56" s="63"/>
+      <c r="I56" s="63"/>
+      <c r="J56" s="63"/>
+      <c r="K56" s="63"/>
+      <c r="L56" s="63"/>
+      <c r="M56" s="63"/>
+      <c r="N56" s="63"/>
+    </row>
+    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A57" s="63"/>
+      <c r="B57" s="63"/>
+      <c r="C57" s="63"/>
+      <c r="D57" s="63" t="s">
+        <v>259</v>
+      </c>
+      <c r="E57" s="63"/>
+      <c r="F57" s="63"/>
+      <c r="G57" s="63"/>
+      <c r="H57" s="63"/>
+      <c r="I57" s="63"/>
+      <c r="J57" s="63"/>
+      <c r="K57" s="63"/>
+      <c r="L57" s="63"/>
+      <c r="M57" s="63"/>
+      <c r="N57" s="63"/>
+    </row>
+    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A58" s="63"/>
+      <c r="B58" s="63"/>
+      <c r="C58" s="63"/>
+      <c r="D58" s="63" t="s">
+        <v>260</v>
+      </c>
+      <c r="E58" s="63"/>
+      <c r="F58" s="63"/>
+      <c r="G58" s="63"/>
+      <c r="H58" s="63"/>
+      <c r="I58" s="63"/>
+      <c r="J58" s="63"/>
+      <c r="K58" s="63"/>
+      <c r="L58" s="63"/>
+      <c r="M58" s="63"/>
+      <c r="N58" s="63"/>
+    </row>
+    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A59" s="63"/>
+      <c r="B59" s="63"/>
+      <c r="C59" s="63"/>
+      <c r="D59" s="63" t="s">
+        <v>262</v>
+      </c>
+      <c r="E59" s="63"/>
+      <c r="F59" s="63"/>
+      <c r="G59" s="63"/>
+      <c r="H59" s="63"/>
+      <c r="I59" s="63"/>
+      <c r="J59" s="63"/>
+      <c r="K59" s="63"/>
+      <c r="L59" s="63"/>
+      <c r="M59" s="63"/>
+      <c r="N59" s="63"/>
+    </row>
+    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A60" s="63"/>
+      <c r="B60" s="63"/>
+      <c r="C60" s="63"/>
+      <c r="D60" s="63"/>
+      <c r="E60" s="63"/>
+      <c r="F60" s="63"/>
+      <c r="G60" s="63"/>
+      <c r="H60" s="63"/>
+      <c r="I60" s="63"/>
+      <c r="J60" s="63"/>
+      <c r="K60" s="63"/>
+      <c r="L60" s="63"/>
+      <c r="M60" s="63"/>
+      <c r="N60" s="63"/>
+    </row>
+    <row r="61" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A61" s="63"/>
+      <c r="B61" s="70" t="s">
+        <v>256</v>
+      </c>
+      <c r="C61" s="63"/>
+      <c r="D61" s="63"/>
+      <c r="E61" s="63"/>
+      <c r="F61" s="63"/>
+      <c r="G61" s="63"/>
+      <c r="H61" s="63"/>
+      <c r="I61" s="63"/>
+      <c r="J61" s="63"/>
+      <c r="K61" s="63"/>
+      <c r="L61" s="63"/>
+      <c r="M61" s="63"/>
+      <c r="N61" s="63"/>
+    </row>
+    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A62" s="63"/>
+      <c r="B62" s="63"/>
+      <c r="C62" s="63"/>
+      <c r="D62" s="63"/>
+      <c r="E62" s="63"/>
+      <c r="F62" s="63"/>
+      <c r="G62" s="63"/>
+      <c r="H62" s="63"/>
+      <c r="I62" s="63"/>
+      <c r="J62" s="63"/>
+      <c r="K62" s="63"/>
+      <c r="L62" s="63"/>
+      <c r="M62" s="63"/>
+      <c r="N62" s="63"/>
+    </row>
+    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A63" s="63"/>
+      <c r="B63" s="63"/>
+      <c r="C63" s="63"/>
+      <c r="D63" s="63"/>
+      <c r="E63" s="63"/>
+      <c r="F63" s="63"/>
+      <c r="G63" s="63"/>
+      <c r="H63" s="63"/>
+      <c r="I63" s="63"/>
+      <c r="J63" s="63"/>
+      <c r="K63" s="63"/>
+      <c r="L63" s="63"/>
+      <c r="M63" s="63"/>
+      <c r="N63" s="63"/>
+    </row>
+    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A64" s="63"/>
+      <c r="B64" s="63"/>
+      <c r="C64" s="63"/>
+      <c r="D64" s="63"/>
+      <c r="E64" s="63"/>
+      <c r="F64" s="63"/>
+      <c r="G64" s="63"/>
+      <c r="H64" s="63"/>
+      <c r="I64" s="63"/>
+      <c r="J64" s="63"/>
+      <c r="K64" s="63"/>
+      <c r="L64" s="63"/>
+      <c r="M64" s="63"/>
+      <c r="N64" s="63"/>
+    </row>
+    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A65" s="63"/>
+      <c r="B65" s="63"/>
+      <c r="C65" s="63"/>
+      <c r="D65" s="63"/>
+      <c r="E65" s="63"/>
+      <c r="F65" s="63"/>
+      <c r="G65" s="63"/>
+      <c r="H65" s="63"/>
+      <c r="I65" s="63"/>
+      <c r="J65" s="63"/>
+      <c r="K65" s="63"/>
+      <c r="L65" s="63"/>
+      <c r="M65" s="63"/>
+      <c r="N65" s="63"/>
+    </row>
+    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A66" s="63"/>
+      <c r="B66" s="63"/>
+      <c r="C66" s="63"/>
+      <c r="D66" s="63"/>
+      <c r="E66" s="63"/>
+      <c r="F66" s="63"/>
+      <c r="G66" s="63"/>
+      <c r="H66" s="63"/>
+      <c r="I66" s="63"/>
+      <c r="J66" s="63"/>
+      <c r="K66" s="63"/>
+      <c r="L66" s="63"/>
+      <c r="M66" s="63"/>
+      <c r="N66" s="63"/>
+    </row>
+    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A67" s="63"/>
+      <c r="B67" s="63"/>
+      <c r="C67" s="63"/>
+      <c r="D67" s="63"/>
+      <c r="E67" s="63"/>
+      <c r="F67" s="63"/>
+      <c r="G67" s="63"/>
+      <c r="H67" s="63"/>
+      <c r="I67" s="63"/>
+      <c r="J67" s="63"/>
+      <c r="K67" s="63"/>
+      <c r="L67" s="63"/>
+      <c r="M67" s="63"/>
+      <c r="N67" s="63"/>
+    </row>
+    <row r="68" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A68" s="63"/>
+      <c r="B68" s="70" t="s">
+        <v>254</v>
+      </c>
+      <c r="C68" s="63"/>
+      <c r="D68" s="63"/>
+      <c r="E68" s="63"/>
+      <c r="F68" s="63"/>
+      <c r="G68" s="63"/>
+      <c r="H68" s="63"/>
+      <c r="I68" s="63"/>
+      <c r="J68" s="63"/>
+      <c r="K68" s="63"/>
+      <c r="L68" s="63"/>
+      <c r="M68" s="63"/>
+      <c r="N68" s="63"/>
+    </row>
+    <row r="69" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A69" s="63"/>
+      <c r="B69" s="63"/>
+      <c r="C69" s="63"/>
+      <c r="D69" s="63"/>
+      <c r="E69" s="63"/>
+      <c r="F69" s="63"/>
+      <c r="G69" s="63"/>
+      <c r="H69" s="63"/>
+      <c r="I69" s="63"/>
+      <c r="J69" s="63"/>
+      <c r="K69" s="63"/>
+      <c r="L69" s="63"/>
+      <c r="M69" s="63"/>
+      <c r="N69" s="63"/>
+    </row>
+    <row r="70" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A70" s="63"/>
+      <c r="B70" s="63"/>
+      <c r="C70" s="63"/>
+      <c r="D70" s="63"/>
+      <c r="E70" s="63"/>
+      <c r="F70" s="63"/>
+      <c r="G70" s="63"/>
+      <c r="H70" s="63"/>
+      <c r="I70" s="63"/>
+      <c r="J70" s="63"/>
+      <c r="K70" s="63"/>
+      <c r="L70" s="63"/>
+      <c r="M70" s="63"/>
+      <c r="N70" s="63"/>
+    </row>
+    <row r="71" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A71" s="63"/>
+      <c r="B71" s="63"/>
+      <c r="C71" s="63"/>
+      <c r="D71" s="63"/>
+      <c r="E71" s="63"/>
+      <c r="F71" s="63"/>
+      <c r="G71" s="63"/>
+      <c r="H71" s="63"/>
+      <c r="I71" s="63"/>
+      <c r="J71" s="63"/>
+      <c r="K71" s="63"/>
+      <c r="L71" s="63"/>
+      <c r="M71" s="63"/>
+      <c r="N71" s="63"/>
+    </row>
+    <row r="72" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A72" s="63"/>
+      <c r="B72" s="63"/>
+      <c r="C72" s="63"/>
+      <c r="D72" s="63"/>
+      <c r="E72" s="63"/>
+      <c r="F72" s="63"/>
+      <c r="G72" s="63"/>
+      <c r="H72" s="63"/>
+      <c r="I72" s="63"/>
+      <c r="J72" s="63"/>
+      <c r="K72" s="63"/>
+      <c r="L72" s="63"/>
+      <c r="M72" s="63"/>
+      <c r="N72" s="63"/>
+    </row>
+    <row r="73" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A73" s="63"/>
+      <c r="B73" s="63"/>
+      <c r="C73" s="63"/>
+      <c r="D73" s="63"/>
+      <c r="E73" s="63"/>
+      <c r="F73" s="63"/>
+      <c r="G73" s="63"/>
+      <c r="H73" s="63"/>
+      <c r="I73" s="63"/>
+      <c r="J73" s="63"/>
+      <c r="K73" s="63"/>
+      <c r="L73" s="63"/>
+      <c r="M73" s="63"/>
+      <c r="N73" s="63"/>
+    </row>
+    <row r="74" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A74" s="63"/>
+      <c r="B74" s="63"/>
+      <c r="C74" s="63"/>
+      <c r="D74" s="63"/>
+      <c r="E74" s="63"/>
+      <c r="F74" s="63"/>
+      <c r="G74" s="63"/>
+      <c r="H74" s="63"/>
+      <c r="I74" s="63"/>
+      <c r="J74" s="63"/>
+      <c r="K74" s="63"/>
+      <c r="L74" s="63"/>
+      <c r="M74" s="63"/>
+      <c r="N74" s="63"/>
+    </row>
+    <row r="75" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A75" s="63"/>
+      <c r="B75" s="63"/>
+      <c r="C75" s="63"/>
+      <c r="D75" s="63"/>
+      <c r="E75" s="63"/>
+      <c r="F75" s="63"/>
+      <c r="G75" s="63"/>
+      <c r="H75" s="63"/>
+      <c r="I75" s="63"/>
+      <c r="J75" s="63"/>
+      <c r="K75" s="63"/>
+      <c r="L75" s="63"/>
+      <c r="M75" s="63"/>
+      <c r="N75" s="63"/>
+    </row>
+    <row r="76" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A76" s="63"/>
+      <c r="B76" s="63"/>
+      <c r="C76" s="63"/>
+      <c r="D76" s="63"/>
+      <c r="E76" s="63"/>
+      <c r="F76" s="63"/>
+      <c r="G76" s="63"/>
+      <c r="H76" s="63"/>
+      <c r="I76" s="63"/>
+      <c r="J76" s="63"/>
+      <c r="K76" s="63"/>
+      <c r="L76" s="63"/>
+      <c r="M76" s="63"/>
+      <c r="N76" s="63"/>
+    </row>
+    <row r="77" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A77" s="63"/>
+      <c r="B77" s="63"/>
+      <c r="C77" s="63"/>
+      <c r="D77" s="63"/>
+      <c r="E77" s="63"/>
+      <c r="F77" s="63"/>
+      <c r="G77" s="63"/>
+      <c r="H77" s="63"/>
+      <c r="I77" s="63"/>
+      <c r="J77" s="63"/>
+      <c r="K77" s="63"/>
+      <c r="L77" s="63"/>
+      <c r="M77" s="63"/>
+      <c r="N77" s="63"/>
+    </row>
+    <row r="78" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A78" s="63"/>
+      <c r="B78" s="63"/>
+      <c r="C78" s="63"/>
+      <c r="D78" s="63"/>
+      <c r="E78" s="63"/>
+      <c r="F78" s="63"/>
+      <c r="G78" s="63"/>
+      <c r="H78" s="63"/>
+      <c r="I78" s="63"/>
+      <c r="J78" s="63"/>
+      <c r="K78" s="63"/>
+      <c r="L78" s="63"/>
+      <c r="M78" s="63"/>
+      <c r="N78" s="63"/>
+    </row>
+    <row r="79" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A79" s="63"/>
+      <c r="B79" s="63"/>
+      <c r="C79" s="63"/>
+      <c r="D79" s="63"/>
+      <c r="E79" s="63"/>
+      <c r="F79" s="63"/>
+      <c r="G79" s="63"/>
+      <c r="H79" s="63"/>
+      <c r="I79" s="63"/>
+      <c r="J79" s="63"/>
+      <c r="K79" s="63"/>
+      <c r="L79" s="63"/>
+      <c r="M79" s="63"/>
+      <c r="N79" s="63"/>
+    </row>
+    <row r="80" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A80" s="63"/>
+      <c r="B80" s="63"/>
+      <c r="C80" s="63"/>
+      <c r="D80" s="63"/>
+      <c r="E80" s="63"/>
+      <c r="F80" s="63"/>
+      <c r="G80" s="63"/>
+      <c r="H80" s="63"/>
+      <c r="I80" s="63"/>
+      <c r="J80" s="63"/>
+      <c r="K80" s="63"/>
+      <c r="L80" s="63"/>
+      <c r="M80" s="63"/>
+      <c r="N80" s="63"/>
+    </row>
+    <row r="81" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A81" s="63"/>
+      <c r="B81" s="63"/>
+      <c r="C81" s="63"/>
+      <c r="D81" s="63"/>
+      <c r="E81" s="63"/>
+      <c r="F81" s="63"/>
+      <c r="G81" s="63"/>
+      <c r="H81" s="63"/>
+      <c r="I81" s="63"/>
+      <c r="J81" s="63"/>
+      <c r="K81" s="63"/>
+      <c r="L81" s="63"/>
+      <c r="M81" s="63"/>
+      <c r="N81" s="63"/>
+    </row>
+    <row r="82" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A82" s="63"/>
+      <c r="B82" s="63"/>
+      <c r="C82" s="63"/>
+      <c r="D82" s="63"/>
+      <c r="E82" s="63"/>
+      <c r="F82" s="63"/>
+      <c r="G82" s="63"/>
+      <c r="H82" s="63"/>
+      <c r="I82" s="63"/>
+      <c r="J82" s="63"/>
+      <c r="K82" s="63"/>
+      <c r="L82" s="63"/>
+      <c r="M82" s="63"/>
+      <c r="N82" s="63"/>
+    </row>
+    <row r="83" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A83" s="63"/>
+      <c r="B83" s="63"/>
+      <c r="C83" s="63"/>
+      <c r="D83" s="63"/>
+      <c r="E83" s="63"/>
+      <c r="F83" s="63"/>
+      <c r="G83" s="63"/>
+      <c r="H83" s="63"/>
+      <c r="I83" s="63"/>
+      <c r="J83" s="63"/>
+      <c r="K83" s="63"/>
+      <c r="L83" s="63"/>
+      <c r="M83" s="63"/>
+      <c r="N83" s="63"/>
+    </row>
+    <row r="84" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A84" s="63"/>
+      <c r="B84" s="63"/>
+      <c r="C84" s="63"/>
+      <c r="D84" s="63"/>
+      <c r="E84" s="63"/>
+      <c r="F84" s="63"/>
+      <c r="G84" s="63"/>
+      <c r="H84" s="63"/>
+      <c r="I84" s="63"/>
+      <c r="J84" s="63"/>
+      <c r="K84" s="63"/>
+      <c r="L84" s="63"/>
+      <c r="M84" s="63"/>
+      <c r="N84" s="63"/>
+    </row>
+    <row r="85" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A85" s="63"/>
+      <c r="B85" s="63"/>
+      <c r="C85" s="63"/>
+      <c r="D85" s="63"/>
+      <c r="E85" s="63"/>
+      <c r="F85" s="63"/>
+      <c r="G85" s="63"/>
+      <c r="H85" s="63"/>
+      <c r="I85" s="63"/>
+      <c r="J85" s="63"/>
+      <c r="K85" s="63"/>
+      <c r="L85" s="63"/>
+      <c r="M85" s="63"/>
+      <c r="N85" s="63"/>
+    </row>
+    <row r="86" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A86" s="63"/>
+      <c r="B86" s="63"/>
+      <c r="C86" s="63"/>
+      <c r="D86" s="63"/>
+      <c r="E86" s="63"/>
+      <c r="F86" s="63"/>
+      <c r="G86" s="63"/>
+      <c r="H86" s="63"/>
+      <c r="I86" s="63"/>
+      <c r="J86" s="63"/>
+      <c r="K86" s="63"/>
+      <c r="L86" s="63"/>
+      <c r="M86" s="63"/>
+      <c r="N86" s="63"/>
+    </row>
+    <row r="87" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A87" s="63"/>
+      <c r="B87" s="63"/>
+      <c r="C87" s="63"/>
+      <c r="D87" s="63"/>
+      <c r="E87" s="63"/>
+      <c r="F87" s="63"/>
+      <c r="G87" s="63"/>
+      <c r="H87" s="63"/>
+      <c r="I87" s="63"/>
+      <c r="J87" s="63"/>
+      <c r="K87" s="63"/>
+      <c r="L87" s="63"/>
+      <c r="M87" s="63"/>
+      <c r="N87" s="63"/>
+    </row>
+    <row r="88" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A88" s="63"/>
+      <c r="B88" s="63"/>
+      <c r="C88" s="63"/>
+      <c r="D88" s="63"/>
+      <c r="E88" s="63"/>
+      <c r="F88" s="63"/>
+      <c r="G88" s="63"/>
+      <c r="H88" s="63"/>
+      <c r="I88" s="63"/>
+      <c r="J88" s="63"/>
+      <c r="K88" s="63"/>
+      <c r="L88" s="63"/>
+      <c r="M88" s="63"/>
+      <c r="N88" s="63"/>
+    </row>
+    <row r="89" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A89" s="63"/>
+      <c r="B89" s="63"/>
+      <c r="C89" s="63"/>
+      <c r="D89" s="63"/>
+      <c r="E89" s="63"/>
+      <c r="F89" s="63"/>
+      <c r="G89" s="63"/>
+      <c r="H89" s="63"/>
+      <c r="I89" s="63"/>
+      <c r="J89" s="63"/>
+      <c r="K89" s="63"/>
+      <c r="L89" s="63"/>
+      <c r="M89" s="63"/>
+      <c r="N89" s="63"/>
+    </row>
+    <row r="90" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A90" s="63"/>
+      <c r="B90" s="63"/>
+      <c r="C90" s="63"/>
+      <c r="D90" s="63"/>
+      <c r="E90" s="63"/>
+      <c r="F90" s="63"/>
+      <c r="G90" s="63"/>
+      <c r="H90" s="63"/>
+      <c r="I90" s="63"/>
+      <c r="J90" s="63"/>
+      <c r="K90" s="63"/>
+      <c r="L90" s="63"/>
+      <c r="M90" s="63"/>
+      <c r="N90" s="63"/>
+    </row>
+    <row r="91" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A91" s="63"/>
+      <c r="B91" s="63"/>
+      <c r="C91" s="63"/>
+      <c r="D91" s="63"/>
+      <c r="E91" s="63"/>
+      <c r="F91" s="63"/>
+      <c r="G91" s="63"/>
+      <c r="H91" s="63"/>
+      <c r="I91" s="63"/>
+      <c r="J91" s="63"/>
+      <c r="K91" s="63"/>
+      <c r="L91" s="63"/>
+      <c r="M91" s="63"/>
+      <c r="N91" s="63"/>
+    </row>
+    <row r="92" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A92" s="63"/>
+      <c r="B92" s="63"/>
+      <c r="C92" s="63"/>
+      <c r="D92" s="63"/>
+      <c r="E92" s="63"/>
+      <c r="F92" s="63"/>
+      <c r="G92" s="63"/>
+      <c r="H92" s="63"/>
+      <c r="I92" s="63"/>
+      <c r="J92" s="63"/>
+      <c r="K92" s="63"/>
+      <c r="L92" s="63"/>
+      <c r="M92" s="63"/>
+      <c r="N92" s="63"/>
+    </row>
+    <row r="93" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A93" s="63"/>
+      <c r="B93" s="63"/>
+      <c r="C93" s="63"/>
+      <c r="D93" s="63"/>
+      <c r="E93" s="63"/>
+      <c r="F93" s="63"/>
+      <c r="G93" s="63"/>
+      <c r="H93" s="63"/>
+      <c r="I93" s="63"/>
+      <c r="J93" s="63"/>
+      <c r="K93" s="63"/>
+      <c r="L93" s="63"/>
+      <c r="M93" s="63"/>
+      <c r="N93" s="63"/>
+    </row>
+    <row r="94" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A94" s="63"/>
+      <c r="B94" s="63"/>
+      <c r="C94" s="63"/>
+      <c r="D94" s="63"/>
+      <c r="E94" s="63"/>
+      <c r="F94" s="63"/>
+      <c r="G94" s="63"/>
+      <c r="H94" s="63"/>
+      <c r="I94" s="63"/>
+      <c r="J94" s="63"/>
+      <c r="K94" s="63"/>
+      <c r="L94" s="63"/>
+      <c r="M94" s="63"/>
+      <c r="N94" s="63"/>
+    </row>
+    <row r="95" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A95" s="63"/>
+      <c r="B95" s="63"/>
+      <c r="C95" s="63"/>
+      <c r="D95" s="63"/>
+      <c r="E95" s="63"/>
+      <c r="F95" s="63"/>
+      <c r="G95" s="63"/>
+      <c r="H95" s="63"/>
+      <c r="I95" s="63"/>
+      <c r="J95" s="63"/>
+      <c r="K95" s="63"/>
+      <c r="L95" s="63"/>
+      <c r="M95" s="63"/>
+      <c r="N95" s="63"/>
+    </row>
+    <row r="96" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A96" s="63"/>
+      <c r="B96" s="63"/>
+      <c r="C96" s="63"/>
+      <c r="D96" s="63"/>
+      <c r="E96" s="63"/>
+      <c r="F96" s="63"/>
+      <c r="G96" s="63"/>
+      <c r="H96" s="63"/>
+      <c r="I96" s="63"/>
+      <c r="J96" s="63"/>
+      <c r="K96" s="63"/>
+      <c r="L96" s="63"/>
+      <c r="M96" s="63"/>
+      <c r="N96" s="63"/>
+    </row>
+    <row r="97" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A97" s="63"/>
+      <c r="B97" s="63"/>
+      <c r="C97" s="63"/>
+      <c r="D97" s="63"/>
+      <c r="E97" s="63"/>
+      <c r="F97" s="63"/>
+      <c r="G97" s="63"/>
+      <c r="H97" s="63"/>
+      <c r="I97" s="63"/>
+      <c r="J97" s="63"/>
+      <c r="K97" s="63"/>
+      <c r="L97" s="63"/>
+      <c r="M97" s="63"/>
+      <c r="N97" s="63"/>
+    </row>
+    <row r="98" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A98" s="63"/>
+      <c r="B98" s="63"/>
+      <c r="C98" s="63"/>
+      <c r="D98" s="63"/>
+      <c r="E98" s="63"/>
+      <c r="F98" s="63"/>
+      <c r="G98" s="63"/>
+      <c r="H98" s="63"/>
+      <c r="I98" s="63"/>
+      <c r="J98" s="63"/>
+      <c r="K98" s="63"/>
+      <c r="L98" s="63"/>
+      <c r="M98" s="63"/>
+      <c r="N98" s="63"/>
+    </row>
+    <row r="99" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A99" s="63"/>
+      <c r="B99" s="63"/>
+      <c r="C99" s="63"/>
+      <c r="D99" s="63"/>
+      <c r="E99" s="63"/>
+      <c r="F99" s="63"/>
+      <c r="G99" s="63"/>
+      <c r="H99" s="63"/>
+      <c r="I99" s="63"/>
+      <c r="J99" s="63"/>
+      <c r="K99" s="63"/>
+      <c r="L99" s="63"/>
+      <c r="M99" s="63"/>
+      <c r="N99" s="63"/>
+    </row>
+    <row r="100" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A100" s="63"/>
+      <c r="B100" s="63"/>
+      <c r="C100" s="63"/>
+      <c r="D100" s="63"/>
+      <c r="E100" s="63"/>
+      <c r="F100" s="63"/>
+      <c r="G100" s="63"/>
+      <c r="H100" s="63"/>
+      <c r="I100" s="63"/>
+      <c r="J100" s="63"/>
+      <c r="K100" s="63"/>
+      <c r="L100" s="63"/>
+      <c r="M100" s="63"/>
+      <c r="N100" s="63"/>
+    </row>
+    <row r="101" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A101" s="63"/>
+      <c r="B101" s="63"/>
+      <c r="C101" s="63"/>
+      <c r="D101" s="63"/>
+      <c r="E101" s="63"/>
+      <c r="F101" s="63"/>
+      <c r="G101" s="63"/>
+      <c r="H101" s="63"/>
+      <c r="I101" s="63"/>
+      <c r="J101" s="63"/>
+      <c r="K101" s="63"/>
+      <c r="L101" s="63"/>
+      <c r="M101" s="63"/>
+      <c r="N101" s="63"/>
+    </row>
+    <row r="102" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A102" s="63"/>
+      <c r="B102" s="63"/>
+      <c r="C102" s="63"/>
+      <c r="D102" s="63"/>
+      <c r="E102" s="63"/>
+      <c r="F102" s="63"/>
+      <c r="G102" s="63"/>
+      <c r="H102" s="63"/>
+      <c r="I102" s="63"/>
+      <c r="J102" s="63"/>
+      <c r="K102" s="63"/>
+      <c r="L102" s="63"/>
+      <c r="M102" s="63"/>
+      <c r="N102" s="63"/>
+    </row>
+    <row r="103" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A103" s="63"/>
+      <c r="B103" s="63"/>
+      <c r="C103" s="63"/>
+      <c r="D103" s="63"/>
+      <c r="E103" s="63"/>
+      <c r="F103" s="63"/>
+      <c r="G103" s="63"/>
+      <c r="H103" s="63"/>
+      <c r="I103" s="63"/>
+      <c r="J103" s="63"/>
+      <c r="K103" s="63"/>
+      <c r="L103" s="63"/>
+      <c r="M103" s="63"/>
+      <c r="N103" s="63"/>
+    </row>
+    <row r="104" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A104" s="63"/>
+      <c r="B104" s="63"/>
+      <c r="C104" s="63"/>
+      <c r="D104" s="63"/>
+      <c r="E104" s="63"/>
+      <c r="F104" s="63"/>
+      <c r="G104" s="63"/>
+      <c r="H104" s="63"/>
+      <c r="I104" s="63"/>
+      <c r="J104" s="63"/>
+      <c r="K104" s="63"/>
+      <c r="L104" s="63"/>
+      <c r="M104" s="63"/>
+      <c r="N104" s="63"/>
+    </row>
+    <row r="105" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A105" s="63"/>
+      <c r="B105" s="63"/>
+      <c r="C105" s="63"/>
+      <c r="D105" s="63"/>
+      <c r="E105" s="63"/>
+      <c r="F105" s="63"/>
+      <c r="G105" s="63"/>
+      <c r="H105" s="63"/>
+      <c r="I105" s="63"/>
+      <c r="J105" s="63"/>
+      <c r="K105" s="63"/>
+      <c r="L105" s="63"/>
+      <c r="M105" s="63"/>
+      <c r="N105" s="63"/>
+    </row>
+    <row r="106" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A106" s="63"/>
+      <c r="B106" s="63"/>
+      <c r="C106" s="63"/>
+      <c r="D106" s="63"/>
+      <c r="E106" s="63"/>
+      <c r="F106" s="63"/>
+      <c r="G106" s="63"/>
+      <c r="H106" s="63"/>
+      <c r="I106" s="63"/>
+      <c r="J106" s="63"/>
+      <c r="K106" s="63"/>
+      <c r="L106" s="63"/>
+      <c r="M106" s="63"/>
+      <c r="N106" s="63"/>
+    </row>
+    <row r="107" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A107" s="63"/>
+      <c r="B107" s="63"/>
+      <c r="C107" s="63"/>
+      <c r="D107" s="63"/>
+      <c r="E107" s="63"/>
+      <c r="F107" s="63"/>
+      <c r="G107" s="63"/>
+      <c r="H107" s="63"/>
+      <c r="I107" s="63"/>
+      <c r="J107" s="63"/>
+      <c r="K107" s="63"/>
+      <c r="L107" s="63"/>
+      <c r="M107" s="63"/>
+      <c r="N107" s="63"/>
+    </row>
+    <row r="108" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A108" s="63"/>
+      <c r="B108" s="63"/>
+      <c r="C108" s="63"/>
+      <c r="D108" s="63"/>
+      <c r="E108" s="63"/>
+      <c r="F108" s="63"/>
+      <c r="G108" s="63"/>
+      <c r="H108" s="63"/>
+      <c r="I108" s="63"/>
+      <c r="J108" s="63"/>
+      <c r="K108" s="63"/>
+      <c r="L108" s="63"/>
+      <c r="M108" s="63"/>
+      <c r="N108" s="63"/>
+    </row>
+    <row r="109" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A109" s="63"/>
+      <c r="B109" s="63"/>
+      <c r="C109" s="63"/>
+      <c r="D109" s="63"/>
+      <c r="E109" s="63"/>
+      <c r="F109" s="63"/>
+      <c r="G109" s="63"/>
+      <c r="H109" s="63"/>
+      <c r="I109" s="63"/>
+      <c r="J109" s="63"/>
+      <c r="K109" s="63"/>
+      <c r="L109" s="63"/>
+      <c r="M109" s="63"/>
+      <c r="N109" s="63"/>
+    </row>
+    <row r="110" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A110" s="63"/>
+      <c r="B110" s="63"/>
+      <c r="C110" s="63"/>
+      <c r="D110" s="63"/>
+      <c r="E110" s="63"/>
+      <c r="F110" s="63"/>
+      <c r="G110" s="63"/>
+      <c r="H110" s="63"/>
+      <c r="I110" s="63"/>
+      <c r="J110" s="63"/>
+      <c r="K110" s="63"/>
+      <c r="L110" s="63"/>
+      <c r="M110" s="63"/>
+      <c r="N110" s="63"/>
+    </row>
+    <row r="111" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A111" s="63"/>
+      <c r="B111" s="63"/>
+      <c r="C111" s="63"/>
+      <c r="D111" s="63"/>
+      <c r="E111" s="63"/>
+      <c r="F111" s="63"/>
+      <c r="G111" s="63"/>
+      <c r="H111" s="63"/>
+      <c r="I111" s="63"/>
+      <c r="J111" s="63"/>
+      <c r="K111" s="63"/>
+      <c r="L111" s="63"/>
+      <c r="M111" s="63"/>
+      <c r="N111" s="63"/>
+    </row>
+    <row r="112" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A112" s="63"/>
+      <c r="B112" s="63"/>
+      <c r="C112" s="63"/>
+      <c r="D112" s="63"/>
+      <c r="E112" s="63"/>
+      <c r="F112" s="63"/>
+      <c r="G112" s="63"/>
+      <c r="H112" s="63"/>
+      <c r="I112" s="63"/>
+      <c r="J112" s="63"/>
+      <c r="K112" s="63"/>
+      <c r="L112" s="63"/>
+      <c r="M112" s="63"/>
+      <c r="N112" s="63"/>
+    </row>
+    <row r="113" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A113" s="63"/>
+      <c r="B113" s="63"/>
+      <c r="C113" s="63"/>
+      <c r="D113" s="63"/>
+      <c r="E113" s="63"/>
+      <c r="F113" s="63"/>
+      <c r="G113" s="63"/>
+      <c r="H113" s="63"/>
+      <c r="I113" s="63"/>
+      <c r="J113" s="63"/>
+      <c r="K113" s="63"/>
+      <c r="L113" s="63"/>
+      <c r="M113" s="63"/>
+      <c r="N113" s="63"/>
+    </row>
+    <row r="114" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A114" s="63"/>
+      <c r="B114" s="63"/>
+      <c r="C114" s="63"/>
+      <c r="D114" s="63"/>
+      <c r="E114" s="63"/>
+      <c r="F114" s="63"/>
+      <c r="G114" s="63"/>
+      <c r="H114" s="63"/>
+      <c r="I114" s="63"/>
+      <c r="J114" s="63"/>
+      <c r="K114" s="63"/>
+      <c r="L114" s="63"/>
+      <c r="M114" s="63"/>
+      <c r="N114" s="63"/>
+    </row>
+    <row r="115" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A115" s="63"/>
+      <c r="B115" s="63"/>
+      <c r="C115" s="63"/>
+      <c r="D115" s="63"/>
+      <c r="E115" s="63"/>
+      <c r="F115" s="63"/>
+      <c r="G115" s="63"/>
+      <c r="H115" s="63"/>
+      <c r="I115" s="63"/>
+      <c r="J115" s="63"/>
+      <c r="K115" s="63"/>
+      <c r="L115" s="63"/>
+      <c r="M115" s="63"/>
+      <c r="N115" s="63"/>
+    </row>
+    <row r="116" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A116" s="63"/>
+      <c r="B116" s="63"/>
+      <c r="C116" s="63"/>
+      <c r="D116" s="63"/>
+      <c r="E116" s="63"/>
+      <c r="F116" s="63"/>
+      <c r="G116" s="63"/>
+      <c r="H116" s="63"/>
+      <c r="I116" s="63"/>
+      <c r="J116" s="63"/>
+      <c r="K116" s="63"/>
+      <c r="L116" s="63"/>
+      <c r="M116" s="63"/>
+      <c r="N116" s="63"/>
+    </row>
+    <row r="117" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A117" s="63"/>
+      <c r="B117" s="63"/>
+      <c r="C117" s="63"/>
+      <c r="D117" s="63"/>
+      <c r="E117" s="63"/>
+      <c r="F117" s="63"/>
+      <c r="G117" s="63"/>
+      <c r="H117" s="63"/>
+      <c r="I117" s="63"/>
+      <c r="J117" s="63"/>
+      <c r="K117" s="63"/>
+      <c r="L117" s="63"/>
+      <c r="M117" s="63"/>
+      <c r="N117" s="63"/>
+    </row>
+    <row r="118" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A118" s="63"/>
+      <c r="B118" s="63"/>
+      <c r="C118" s="63"/>
+      <c r="D118" s="63"/>
+      <c r="E118" s="63"/>
+      <c r="F118" s="63"/>
+      <c r="G118" s="63"/>
+      <c r="H118" s="63"/>
+      <c r="I118" s="63"/>
+      <c r="J118" s="63"/>
+      <c r="K118" s="63"/>
+      <c r="L118" s="63"/>
+      <c r="M118" s="63"/>
+      <c r="N118" s="63"/>
+    </row>
+    <row r="119" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A119" s="63"/>
+      <c r="B119" s="63"/>
+      <c r="C119" s="63"/>
+      <c r="D119" s="63"/>
+      <c r="E119" s="63"/>
+      <c r="F119" s="63"/>
+      <c r="G119" s="63"/>
+      <c r="H119" s="63"/>
+      <c r="I119" s="63"/>
+      <c r="J119" s="63"/>
+      <c r="K119" s="63"/>
+      <c r="L119" s="63"/>
+      <c r="M119" s="63"/>
+      <c r="N119" s="63"/>
+    </row>
+    <row r="120" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A120" s="63"/>
+      <c r="B120" s="63"/>
+      <c r="C120" s="63"/>
+      <c r="D120" s="63"/>
+      <c r="E120" s="63"/>
+      <c r="F120" s="63"/>
+      <c r="G120" s="63"/>
+      <c r="H120" s="63"/>
+      <c r="I120" s="63"/>
+      <c r="J120" s="63"/>
+      <c r="K120" s="63"/>
+      <c r="L120" s="63"/>
+      <c r="M120" s="63"/>
+      <c r="N120" s="63"/>
+    </row>
+    <row r="121" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A121" s="63"/>
+      <c r="B121" s="63"/>
+      <c r="C121" s="63"/>
+      <c r="D121" s="63"/>
+      <c r="E121" s="63"/>
+      <c r="F121" s="63"/>
+      <c r="G121" s="63"/>
+      <c r="H121" s="63"/>
+      <c r="I121" s="63"/>
+      <c r="J121" s="63"/>
+      <c r="K121" s="63"/>
+      <c r="L121" s="63"/>
+      <c r="M121" s="63"/>
+      <c r="N121" s="63"/>
+    </row>
+    <row r="122" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A122" s="63"/>
+      <c r="B122" s="63"/>
+      <c r="C122" s="63"/>
+      <c r="D122" s="63"/>
+      <c r="E122" s="63"/>
+      <c r="F122" s="63"/>
+      <c r="G122" s="63"/>
+      <c r="H122" s="63"/>
+      <c r="I122" s="63"/>
+      <c r="J122" s="63"/>
+      <c r="K122" s="63"/>
+      <c r="L122" s="63"/>
+      <c r="M122" s="63"/>
+      <c r="N122" s="63"/>
+    </row>
+    <row r="123" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A123" s="63"/>
+      <c r="B123" s="63"/>
+      <c r="C123" s="63"/>
+      <c r="D123" s="63"/>
+      <c r="E123" s="63"/>
+      <c r="F123" s="63"/>
+      <c r="G123" s="63"/>
+      <c r="H123" s="63"/>
+      <c r="I123" s="63"/>
+      <c r="J123" s="63"/>
+      <c r="K123" s="63"/>
+      <c r="L123" s="63"/>
+      <c r="M123" s="63"/>
+      <c r="N123" s="63"/>
+    </row>
+    <row r="124" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A124" s="63"/>
+      <c r="B124" s="63"/>
+      <c r="C124" s="63"/>
+      <c r="D124" s="63"/>
+      <c r="E124" s="63"/>
+      <c r="F124" s="63"/>
+      <c r="G124" s="63"/>
+      <c r="H124" s="63"/>
+      <c r="I124" s="63"/>
+      <c r="J124" s="63"/>
+      <c r="K124" s="63"/>
+      <c r="L124" s="63"/>
+      <c r="M124" s="63"/>
+      <c r="N124" s="63"/>
+    </row>
+    <row r="125" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A125" s="63"/>
+      <c r="B125" s="63"/>
+      <c r="C125" s="63"/>
+      <c r="D125" s="63"/>
+      <c r="E125" s="63"/>
+      <c r="F125" s="63"/>
+      <c r="G125" s="63"/>
+      <c r="H125" s="63"/>
+      <c r="I125" s="63"/>
+      <c r="J125" s="63"/>
+      <c r="K125" s="63"/>
+      <c r="L125" s="63"/>
+      <c r="M125" s="63"/>
+      <c r="N125" s="63"/>
+    </row>
+    <row r="126" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A126" s="63"/>
+      <c r="B126" s="63"/>
+      <c r="C126" s="63"/>
+      <c r="D126" s="63"/>
+      <c r="E126" s="63"/>
+      <c r="F126" s="63"/>
+      <c r="G126" s="63"/>
+      <c r="H126" s="63"/>
+      <c r="I126" s="63"/>
+      <c r="J126" s="63"/>
+      <c r="K126" s="63"/>
+      <c r="L126" s="63"/>
+      <c r="M126" s="63"/>
+      <c r="N126" s="63"/>
+    </row>
+    <row r="127" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A127" s="63"/>
+      <c r="B127" s="63"/>
+      <c r="C127" s="63"/>
+      <c r="D127" s="63"/>
+      <c r="E127" s="63"/>
+      <c r="F127" s="63"/>
+      <c r="G127" s="63"/>
+      <c r="H127" s="63"/>
+      <c r="I127" s="63"/>
+      <c r="J127" s="63"/>
+      <c r="K127" s="63"/>
+      <c r="L127" s="63"/>
+      <c r="M127" s="63"/>
+      <c r="N127" s="63"/>
+    </row>
+    <row r="128" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A128" s="63"/>
+      <c r="B128" s="63"/>
+      <c r="C128" s="63"/>
+      <c r="D128" s="63"/>
+      <c r="E128" s="63"/>
+      <c r="F128" s="63"/>
+      <c r="G128" s="63"/>
+      <c r="H128" s="63"/>
+      <c r="I128" s="63"/>
+      <c r="J128" s="63"/>
+      <c r="K128" s="63"/>
+      <c r="L128" s="63"/>
+      <c r="M128" s="63"/>
+      <c r="N128" s="63"/>
+    </row>
+    <row r="129" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A129" s="63"/>
+      <c r="B129" s="63"/>
+      <c r="C129" s="63"/>
+      <c r="D129" s="63"/>
+      <c r="E129" s="63"/>
+      <c r="F129" s="63"/>
+      <c r="G129" s="63"/>
+      <c r="H129" s="63"/>
+      <c r="I129" s="63"/>
+      <c r="J129" s="63"/>
+      <c r="K129" s="63"/>
+      <c r="L129" s="63"/>
+      <c r="M129" s="63"/>
+      <c r="N129" s="63"/>
+    </row>
+    <row r="130" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A130" s="63"/>
+      <c r="B130" s="63"/>
+      <c r="C130" s="63"/>
+      <c r="D130" s="63"/>
+      <c r="E130" s="63"/>
+      <c r="F130" s="63"/>
+      <c r="G130" s="63"/>
+      <c r="H130" s="63"/>
+      <c r="I130" s="63"/>
+      <c r="J130" s="63"/>
+      <c r="K130" s="63"/>
+      <c r="L130" s="63"/>
+      <c r="M130" s="63"/>
+      <c r="N130" s="63"/>
+    </row>
+    <row r="131" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A131" s="63"/>
+      <c r="B131" s="63"/>
+      <c r="C131" s="63"/>
+      <c r="D131" s="63"/>
+      <c r="E131" s="63"/>
+      <c r="F131" s="63"/>
+      <c r="G131" s="63"/>
+      <c r="H131" s="63"/>
+      <c r="I131" s="63"/>
+      <c r="J131" s="63"/>
+      <c r="K131" s="63"/>
+      <c r="L131" s="63"/>
+      <c r="M131" s="63"/>
+      <c r="N131" s="63"/>
+    </row>
+    <row r="132" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A132" s="63"/>
+      <c r="B132" s="63"/>
+      <c r="C132" s="63"/>
+      <c r="D132" s="63"/>
+      <c r="E132" s="63"/>
+      <c r="F132" s="63"/>
+      <c r="G132" s="63"/>
+      <c r="H132" s="63"/>
+      <c r="I132" s="63"/>
+      <c r="J132" s="63"/>
+      <c r="K132" s="63"/>
+      <c r="L132" s="63"/>
+      <c r="M132" s="63"/>
+      <c r="N132" s="63"/>
+    </row>
+    <row r="133" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A133" s="63"/>
+      <c r="B133" s="63"/>
+      <c r="C133" s="63"/>
+      <c r="D133" s="63"/>
+      <c r="E133" s="63"/>
+      <c r="F133" s="63"/>
+      <c r="G133" s="63"/>
+      <c r="H133" s="63"/>
+      <c r="I133" s="63"/>
+      <c r="J133" s="63"/>
+      <c r="K133" s="63"/>
+      <c r="L133" s="63"/>
+      <c r="M133" s="63"/>
+      <c r="N133" s="63"/>
+    </row>
+    <row r="134" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A134" s="63"/>
+      <c r="B134" s="63"/>
+      <c r="C134" s="63"/>
+      <c r="D134" s="63"/>
+      <c r="E134" s="63"/>
+      <c r="F134" s="63"/>
+      <c r="G134" s="63"/>
+      <c r="H134" s="63"/>
+      <c r="I134" s="63"/>
+      <c r="J134" s="63"/>
+      <c r="K134" s="63"/>
+      <c r="L134" s="63"/>
+      <c r="M134" s="63"/>
+      <c r="N134" s="63"/>
+    </row>
+    <row r="135" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A135" s="63"/>
+      <c r="B135" s="63"/>
+      <c r="C135" s="63"/>
+      <c r="D135" s="63"/>
+      <c r="E135" s="63"/>
+      <c r="F135" s="63"/>
+      <c r="G135" s="63"/>
+      <c r="H135" s="63"/>
+      <c r="I135" s="63"/>
+      <c r="J135" s="63"/>
+      <c r="K135" s="63"/>
+      <c r="L135" s="63"/>
+      <c r="M135" s="63"/>
+      <c r="N135" s="63"/>
+    </row>
+    <row r="136" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A136" s="63"/>
+      <c r="B136" s="63"/>
+      <c r="C136" s="63"/>
+      <c r="D136" s="63"/>
+      <c r="E136" s="63"/>
+      <c r="F136" s="63"/>
+      <c r="G136" s="63"/>
+      <c r="H136" s="63"/>
+      <c r="I136" s="63"/>
+      <c r="J136" s="63"/>
+      <c r="K136" s="63"/>
+      <c r="L136" s="63"/>
+      <c r="M136" s="63"/>
+      <c r="N136" s="63"/>
+    </row>
+    <row r="137" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A137" s="63"/>
+      <c r="B137" s="63"/>
+      <c r="C137" s="63"/>
+      <c r="D137" s="63"/>
+      <c r="E137" s="63"/>
+      <c r="F137" s="63"/>
+      <c r="G137" s="63"/>
+      <c r="H137" s="63"/>
+      <c r="I137" s="63"/>
+      <c r="J137" s="63"/>
+      <c r="K137" s="63"/>
+      <c r="L137" s="63"/>
+      <c r="M137" s="63"/>
+      <c r="N137" s="63"/>
+    </row>
+    <row r="138" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A138" s="63"/>
+      <c r="B138" s="63"/>
+      <c r="C138" s="63"/>
+      <c r="D138" s="63"/>
+      <c r="E138" s="63"/>
+      <c r="F138" s="63"/>
+      <c r="G138" s="63"/>
+      <c r="H138" s="63"/>
+      <c r="I138" s="63"/>
+      <c r="J138" s="63"/>
+      <c r="K138" s="63"/>
+      <c r="L138" s="63"/>
+      <c r="M138" s="63"/>
+      <c r="N138" s="63"/>
+    </row>
+    <row r="139" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A139" s="63"/>
+      <c r="B139" s="63"/>
+      <c r="C139" s="63"/>
+      <c r="D139" s="63"/>
+      <c r="E139" s="63"/>
+      <c r="F139" s="63"/>
+      <c r="G139" s="63"/>
+      <c r="H139" s="63"/>
+      <c r="I139" s="63"/>
+      <c r="J139" s="63"/>
+      <c r="K139" s="63"/>
+      <c r="L139" s="63"/>
+      <c r="M139" s="63"/>
+      <c r="N139" s="63"/>
+    </row>
+    <row r="140" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A140" s="63"/>
+      <c r="B140" s="63"/>
+      <c r="C140" s="63"/>
+      <c r="D140" s="63"/>
+      <c r="E140" s="63"/>
+      <c r="F140" s="63"/>
+      <c r="G140" s="63"/>
+      <c r="H140" s="63"/>
+      <c r="I140" s="63"/>
+      <c r="J140" s="63"/>
+      <c r="K140" s="63"/>
+      <c r="L140" s="63"/>
+      <c r="M140" s="63"/>
+      <c r="N140" s="63"/>
+    </row>
+    <row r="141" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A141" s="63"/>
+      <c r="B141" s="63"/>
+      <c r="C141" s="63"/>
+      <c r="D141" s="63"/>
+      <c r="E141" s="63"/>
+      <c r="F141" s="63"/>
+      <c r="G141" s="63"/>
+      <c r="H141" s="63"/>
+      <c r="I141" s="63"/>
+      <c r="J141" s="63"/>
+      <c r="K141" s="63"/>
+      <c r="L141" s="63"/>
+      <c r="M141" s="63"/>
+      <c r="N141" s="63"/>
+    </row>
+    <row r="142" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A142" s="63"/>
+      <c r="B142" s="63"/>
+      <c r="C142" s="63"/>
+      <c r="D142" s="63"/>
+      <c r="E142" s="63"/>
+      <c r="F142" s="63"/>
+      <c r="G142" s="63"/>
+      <c r="H142" s="63"/>
+      <c r="I142" s="63"/>
+      <c r="J142" s="63"/>
+      <c r="K142" s="63"/>
+      <c r="L142" s="63"/>
+      <c r="M142" s="63"/>
+      <c r="N142" s="63"/>
+    </row>
+    <row r="143" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A143" s="63"/>
+      <c r="B143" s="63"/>
+      <c r="C143" s="63"/>
+      <c r="D143" s="63"/>
+      <c r="E143" s="63"/>
+      <c r="F143" s="63"/>
+      <c r="G143" s="63"/>
+      <c r="H143" s="63"/>
+      <c r="I143" s="63"/>
+      <c r="J143" s="63"/>
+      <c r="K143" s="63"/>
+      <c r="L143" s="63"/>
+      <c r="M143" s="63"/>
+      <c r="N143" s="63"/>
+    </row>
+    <row r="144" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A144" s="63"/>
+      <c r="B144" s="63"/>
+      <c r="C144" s="63"/>
+      <c r="D144" s="63"/>
+      <c r="E144" s="63"/>
+      <c r="F144" s="63"/>
+      <c r="G144" s="63"/>
+      <c r="H144" s="63"/>
+      <c r="I144" s="63"/>
+      <c r="J144" s="63"/>
+      <c r="K144" s="63"/>
+      <c r="L144" s="63"/>
+      <c r="M144" s="63"/>
+      <c r="N144" s="63"/>
+    </row>
+    <row r="145" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A145" s="63"/>
+      <c r="B145" s="63"/>
+      <c r="C145" s="63"/>
+      <c r="D145" s="63"/>
+      <c r="E145" s="63"/>
+      <c r="F145" s="63"/>
+      <c r="G145" s="63"/>
+      <c r="H145" s="63"/>
+      <c r="I145" s="63"/>
+      <c r="J145" s="63"/>
+      <c r="K145" s="63"/>
+      <c r="L145" s="63"/>
+      <c r="M145" s="63"/>
+      <c r="N145" s="63"/>
+    </row>
+    <row r="146" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A146" s="63"/>
+      <c r="B146" s="63"/>
+      <c r="C146" s="63"/>
+      <c r="D146" s="63"/>
+      <c r="E146" s="63"/>
+      <c r="F146" s="63"/>
+      <c r="G146" s="63"/>
+      <c r="H146" s="63"/>
+      <c r="I146" s="63"/>
+      <c r="J146" s="63"/>
+      <c r="K146" s="63"/>
+      <c r="L146" s="63"/>
+      <c r="M146" s="63"/>
+      <c r="N146" s="63"/>
+    </row>
+    <row r="147" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A147" s="63"/>
+      <c r="B147" s="63"/>
+      <c r="C147" s="63"/>
+      <c r="D147" s="63"/>
+      <c r="E147" s="63"/>
+      <c r="F147" s="63"/>
+      <c r="G147" s="63"/>
+      <c r="H147" s="63"/>
+      <c r="I147" s="63"/>
+      <c r="J147" s="63"/>
+      <c r="K147" s="63"/>
+      <c r="L147" s="63"/>
+      <c r="M147" s="63"/>
+      <c r="N147" s="63"/>
+    </row>
+    <row r="148" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A148" s="63"/>
+      <c r="B148" s="63"/>
+      <c r="C148" s="63"/>
+      <c r="D148" s="63"/>
+      <c r="E148" s="63"/>
+      <c r="F148" s="63"/>
+      <c r="G148" s="63"/>
+      <c r="H148" s="63"/>
+      <c r="I148" s="63"/>
+      <c r="J148" s="63"/>
+      <c r="K148" s="63"/>
+      <c r="L148" s="63"/>
+      <c r="M148" s="63"/>
+      <c r="N148" s="63"/>
+    </row>
+    <row r="149" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A149" s="63"/>
+      <c r="B149" s="63"/>
+      <c r="C149" s="63"/>
+      <c r="D149" s="63"/>
+      <c r="E149" s="63"/>
+      <c r="F149" s="63"/>
+      <c r="G149" s="63"/>
+      <c r="H149" s="63"/>
+      <c r="I149" s="63"/>
+      <c r="J149" s="63"/>
+      <c r="K149" s="63"/>
+      <c r="L149" s="63"/>
+      <c r="M149" s="63"/>
+      <c r="N149" s="63"/>
+    </row>
+    <row r="150" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A150" s="63"/>
+      <c r="B150" s="63"/>
+      <c r="C150" s="63"/>
+      <c r="D150" s="63"/>
+      <c r="E150" s="63"/>
+      <c r="F150" s="63"/>
+      <c r="G150" s="63"/>
+      <c r="H150" s="63"/>
+      <c r="I150" s="63"/>
+      <c r="J150" s="63"/>
+      <c r="K150" s="63"/>
+      <c r="L150" s="63"/>
+      <c r="M150" s="63"/>
+      <c r="N150" s="63"/>
+    </row>
+    <row r="151" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A151" s="63"/>
+      <c r="B151" s="63"/>
+      <c r="C151" s="63"/>
+      <c r="D151" s="63"/>
+      <c r="E151" s="63"/>
+      <c r="F151" s="63"/>
+      <c r="G151" s="63"/>
+      <c r="H151" s="63"/>
+      <c r="I151" s="63"/>
+      <c r="J151" s="63"/>
+      <c r="K151" s="63"/>
+      <c r="L151" s="63"/>
+      <c r="M151" s="63"/>
+      <c r="N151" s="63"/>
+    </row>
+    <row r="152" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A152" s="63"/>
+      <c r="B152" s="63"/>
+      <c r="C152" s="63"/>
+      <c r="D152" s="63"/>
+      <c r="E152" s="63"/>
+      <c r="F152" s="63"/>
+      <c r="G152" s="63"/>
+      <c r="H152" s="63"/>
+      <c r="I152" s="63"/>
+      <c r="J152" s="63"/>
+      <c r="K152" s="63"/>
+      <c r="L152" s="63"/>
+      <c r="M152" s="63"/>
+      <c r="N152" s="63"/>
+    </row>
+    <row r="153" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A153" s="63"/>
+      <c r="B153" s="63"/>
+      <c r="C153" s="63"/>
+      <c r="D153" s="63"/>
+      <c r="E153" s="63"/>
+      <c r="F153" s="63"/>
+      <c r="G153" s="63"/>
+      <c r="H153" s="63"/>
+      <c r="I153" s="63"/>
+      <c r="J153" s="63"/>
+      <c r="K153" s="63"/>
+      <c r="L153" s="63"/>
+      <c r="M153" s="63"/>
+      <c r="N153" s="63"/>
+    </row>
+    <row r="154" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A154" s="63"/>
+      <c r="B154" s="63"/>
+      <c r="C154" s="63"/>
+      <c r="D154" s="63"/>
+      <c r="E154" s="63"/>
+      <c r="F154" s="63"/>
+      <c r="G154" s="63"/>
+      <c r="H154" s="63"/>
+      <c r="I154" s="63"/>
+      <c r="J154" s="63"/>
+      <c r="K154" s="63"/>
+      <c r="L154" s="63"/>
+      <c r="M154" s="63"/>
+      <c r="N154" s="63"/>
+    </row>
+    <row r="155" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A155" s="63"/>
+      <c r="B155" s="63"/>
+      <c r="C155" s="63"/>
+      <c r="D155" s="63"/>
+      <c r="E155" s="63"/>
+      <c r="F155" s="63"/>
+      <c r="G155" s="63"/>
+      <c r="H155" s="63"/>
+      <c r="I155" s="63"/>
+      <c r="J155" s="63"/>
+      <c r="K155" s="63"/>
+      <c r="L155" s="63"/>
+      <c r="M155" s="63"/>
+      <c r="N155" s="63"/>
+    </row>
+    <row r="156" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A156" s="63"/>
+      <c r="B156" s="63"/>
+      <c r="C156" s="63"/>
+      <c r="D156" s="63"/>
+      <c r="E156" s="63"/>
+      <c r="F156" s="63"/>
+      <c r="G156" s="63"/>
+      <c r="H156" s="63"/>
+      <c r="I156" s="63"/>
+      <c r="J156" s="63"/>
+      <c r="K156" s="63"/>
+      <c r="L156" s="63"/>
+      <c r="M156" s="63"/>
+      <c r="N156" s="63"/>
+    </row>
+    <row r="157" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A157" s="63"/>
+      <c r="B157" s="63"/>
+      <c r="C157" s="63"/>
+      <c r="D157" s="63"/>
+      <c r="E157" s="63"/>
+      <c r="F157" s="63"/>
+      <c r="G157" s="63"/>
+      <c r="H157" s="63"/>
+      <c r="I157" s="63"/>
+      <c r="J157" s="63"/>
+      <c r="K157" s="63"/>
+      <c r="L157" s="63"/>
+      <c r="M157" s="63"/>
+      <c r="N157" s="63"/>
+    </row>
+    <row r="158" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A158" s="63"/>
+      <c r="B158" s="63"/>
+      <c r="C158" s="63"/>
+      <c r="D158" s="63"/>
+      <c r="E158" s="63"/>
+      <c r="F158" s="63"/>
+      <c r="G158" s="63"/>
+      <c r="H158" s="63"/>
+      <c r="I158" s="63"/>
+      <c r="J158" s="63"/>
+      <c r="K158" s="63"/>
+      <c r="L158" s="63"/>
+      <c r="M158" s="63"/>
+      <c r="N158" s="63"/>
+    </row>
+    <row r="159" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A159" s="63"/>
+      <c r="B159" s="63"/>
+      <c r="C159" s="63"/>
+      <c r="D159" s="63"/>
+      <c r="E159" s="63"/>
+      <c r="F159" s="63"/>
+      <c r="G159" s="63"/>
+      <c r="H159" s="63"/>
+      <c r="I159" s="63"/>
+      <c r="J159" s="63"/>
+      <c r="K159" s="63"/>
+      <c r="L159" s="63"/>
+      <c r="M159" s="63"/>
+      <c r="N159" s="63"/>
+    </row>
+    <row r="160" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A160" s="63"/>
+      <c r="B160" s="63"/>
+      <c r="C160" s="63"/>
+      <c r="D160" s="63"/>
+      <c r="E160" s="63"/>
+      <c r="F160" s="63"/>
+      <c r="G160" s="63"/>
+      <c r="H160" s="63"/>
+      <c r="I160" s="63"/>
+      <c r="J160" s="63"/>
+      <c r="K160" s="63"/>
+      <c r="L160" s="63"/>
+      <c r="M160" s="63"/>
+      <c r="N160" s="63"/>
+    </row>
+    <row r="161" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A161" s="63"/>
+      <c r="B161" s="63"/>
+      <c r="C161" s="63"/>
+      <c r="D161" s="63"/>
+      <c r="E161" s="63"/>
+      <c r="F161" s="63"/>
+      <c r="G161" s="63"/>
+      <c r="H161" s="63"/>
+      <c r="I161" s="63"/>
+      <c r="J161" s="63"/>
+      <c r="K161" s="63"/>
+      <c r="L161" s="63"/>
+      <c r="M161" s="63"/>
+      <c r="N161" s="63"/>
+    </row>
+    <row r="162" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A162" s="63"/>
+      <c r="B162" s="63"/>
+      <c r="C162" s="63"/>
+      <c r="D162" s="63"/>
+      <c r="E162" s="63"/>
+      <c r="F162" s="63"/>
+      <c r="G162" s="63"/>
+      <c r="H162" s="63"/>
+      <c r="I162" s="63"/>
+      <c r="J162" s="63"/>
+      <c r="K162" s="63"/>
+      <c r="L162" s="63"/>
+      <c r="M162" s="63"/>
+      <c r="N162" s="63"/>
+    </row>
+    <row r="163" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A163" s="63"/>
+      <c r="B163" s="63"/>
+      <c r="C163" s="63"/>
+      <c r="D163" s="63"/>
+      <c r="E163" s="63"/>
+      <c r="F163" s="63"/>
+      <c r="G163" s="63"/>
+      <c r="H163" s="63"/>
+      <c r="I163" s="63"/>
+      <c r="J163" s="63"/>
+      <c r="K163" s="63"/>
+      <c r="L163" s="63"/>
+      <c r="M163" s="63"/>
+      <c r="N163" s="63"/>
+    </row>
+    <row r="164" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A164" s="63"/>
+      <c r="B164" s="63"/>
+      <c r="C164" s="63"/>
+      <c r="D164" s="63"/>
+      <c r="E164" s="63"/>
+      <c r="F164" s="63"/>
+      <c r="G164" s="63"/>
+      <c r="H164" s="63"/>
+      <c r="I164" s="63"/>
+      <c r="J164" s="63"/>
+      <c r="K164" s="63"/>
+      <c r="L164" s="63"/>
+      <c r="M164" s="63"/>
+      <c r="N164" s="63"/>
+    </row>
+    <row r="165" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A165" s="63"/>
+      <c r="B165" s="63"/>
+      <c r="C165" s="63"/>
+      <c r="D165" s="63"/>
+      <c r="E165" s="63"/>
+      <c r="F165" s="63"/>
+      <c r="G165" s="63"/>
+      <c r="H165" s="63"/>
+      <c r="I165" s="63"/>
+      <c r="J165" s="63"/>
+      <c r="K165" s="63"/>
+      <c r="L165" s="63"/>
+      <c r="M165" s="63"/>
+      <c r="N165" s="63"/>
     </row>
   </sheetData>
-  <mergeCells count="12">
+  <mergeCells count="18">
+    <mergeCell ref="A51:N52"/>
+    <mergeCell ref="G25:K25"/>
+    <mergeCell ref="G26:K26"/>
+    <mergeCell ref="G27:K27"/>
+    <mergeCell ref="A31:N32"/>
+    <mergeCell ref="G35:J35"/>
+    <mergeCell ref="F5:I5"/>
+    <mergeCell ref="F6:I6"/>
+    <mergeCell ref="F7:I7"/>
+    <mergeCell ref="F8:I8"/>
+    <mergeCell ref="A1:N2"/>
     <mergeCell ref="G24:K24"/>
     <mergeCell ref="A15:N16"/>
     <mergeCell ref="G18:K18"/>
@@ -9126,12 +11826,10 @@
     <mergeCell ref="G20:K20"/>
     <mergeCell ref="G21:K21"/>
     <mergeCell ref="G22:K22"/>
-    <mergeCell ref="F5:I5"/>
-    <mergeCell ref="F6:I6"/>
-    <mergeCell ref="F7:I7"/>
-    <mergeCell ref="F8:I8"/>
-    <mergeCell ref="A1:N2"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="G24:K24" location="Senegal_Formulaire!P15" display="Atlantique"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
@@ -9154,56 +11852,56 @@
   </cols>
   <sheetData>
     <row r="2" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="H2" s="32" t="s">
+      <c r="H2" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="I2" s="33"/>
-      <c r="J2" s="34"/>
-      <c r="L2" s="26" t="s">
+      <c r="I2" s="42"/>
+      <c r="J2" s="43"/>
+      <c r="L2" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="M2" s="27"/>
-      <c r="N2" s="28"/>
+      <c r="M2" s="30"/>
+      <c r="N2" s="31"/>
     </row>
     <row r="3" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="H3" s="35"/>
-      <c r="I3" s="36"/>
-      <c r="J3" s="37"/>
-      <c r="L3" s="29"/>
-      <c r="M3" s="30"/>
-      <c r="N3" s="31"/>
+      <c r="H3" s="44"/>
+      <c r="I3" s="45"/>
+      <c r="J3" s="46"/>
+      <c r="L3" s="32"/>
+      <c r="M3" s="33"/>
+      <c r="N3" s="34"/>
     </row>
     <row r="5" spans="4:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H5" s="26" t="s">
+      <c r="H5" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="I5" s="27"/>
-      <c r="J5" s="28"/>
-      <c r="L5" s="26" t="s">
+      <c r="I5" s="30"/>
+      <c r="J5" s="31"/>
+      <c r="L5" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="M5" s="27"/>
-      <c r="N5" s="28"/>
+      <c r="M5" s="30"/>
+      <c r="N5" s="31"/>
     </row>
     <row r="6" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="D6" s="38" t="s">
+      <c r="D6" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="E6" s="39"/>
-      <c r="F6" s="40"/>
+      <c r="E6" s="36"/>
+      <c r="F6" s="37"/>
       <c r="G6" s="3"/>
-      <c r="H6" s="29"/>
-      <c r="I6" s="30"/>
-      <c r="J6" s="31"/>
+      <c r="H6" s="32"/>
+      <c r="I6" s="33"/>
+      <c r="J6" s="34"/>
       <c r="K6" s="4"/>
-      <c r="L6" s="29"/>
-      <c r="M6" s="30"/>
-      <c r="N6" s="31"/>
+      <c r="L6" s="32"/>
+      <c r="M6" s="33"/>
+      <c r="N6" s="34"/>
     </row>
     <row r="7" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="D7" s="41"/>
-      <c r="E7" s="42"/>
-      <c r="F7" s="43"/>
+      <c r="D7" s="38"/>
+      <c r="E7" s="39"/>
+      <c r="F7" s="40"/>
       <c r="G7" s="3"/>
       <c r="H7" s="4"/>
       <c r="I7" s="4"/>
@@ -9214,234 +11912,246 @@
       <c r="N7" s="4"/>
     </row>
     <row r="8" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="H8" s="32" t="s">
+      <c r="H8" s="41" t="s">
         <v>5</v>
       </c>
-      <c r="I8" s="33"/>
-      <c r="J8" s="34"/>
-      <c r="L8" s="26" t="s">
+      <c r="I8" s="42"/>
+      <c r="J8" s="43"/>
+      <c r="L8" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="M8" s="27"/>
-      <c r="N8" s="28"/>
+      <c r="M8" s="30"/>
+      <c r="N8" s="31"/>
     </row>
     <row r="9" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="D9" s="44" t="s">
+      <c r="D9" s="47" t="s">
         <v>22</v>
       </c>
-      <c r="E9" s="44"/>
-      <c r="F9" s="44"/>
-      <c r="H9" s="35"/>
-      <c r="I9" s="36"/>
-      <c r="J9" s="37"/>
-      <c r="L9" s="29"/>
-      <c r="M9" s="30"/>
-      <c r="N9" s="31"/>
+      <c r="E9" s="47"/>
+      <c r="F9" s="47"/>
+      <c r="H9" s="44"/>
+      <c r="I9" s="45"/>
+      <c r="J9" s="46"/>
+      <c r="L9" s="32"/>
+      <c r="M9" s="33"/>
+      <c r="N9" s="34"/>
     </row>
     <row r="10" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="D10" s="45"/>
-      <c r="E10" s="45"/>
-      <c r="F10" s="45"/>
+      <c r="D10" s="48"/>
+      <c r="E10" s="48"/>
+      <c r="F10" s="48"/>
     </row>
     <row r="11" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="D11" s="45"/>
-      <c r="E11" s="45"/>
-      <c r="F11" s="45"/>
-      <c r="H11" s="32" t="s">
+      <c r="D11" s="48"/>
+      <c r="E11" s="48"/>
+      <c r="F11" s="48"/>
+      <c r="H11" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="I11" s="33"/>
-      <c r="J11" s="34"/>
-      <c r="L11" s="32" t="s">
+      <c r="I11" s="42"/>
+      <c r="J11" s="43"/>
+      <c r="L11" s="41" t="s">
         <v>18</v>
       </c>
-      <c r="M11" s="33"/>
-      <c r="N11" s="34"/>
+      <c r="M11" s="42"/>
+      <c r="N11" s="43"/>
     </row>
     <row r="12" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="D12" s="45"/>
-      <c r="E12" s="45"/>
-      <c r="F12" s="45"/>
-      <c r="H12" s="35"/>
-      <c r="I12" s="36"/>
-      <c r="J12" s="37"/>
-      <c r="L12" s="35"/>
-      <c r="M12" s="36"/>
-      <c r="N12" s="37"/>
+      <c r="D12" s="48"/>
+      <c r="E12" s="48"/>
+      <c r="F12" s="48"/>
+      <c r="H12" s="44"/>
+      <c r="I12" s="45"/>
+      <c r="J12" s="46"/>
+      <c r="L12" s="44"/>
+      <c r="M12" s="45"/>
+      <c r="N12" s="46"/>
     </row>
     <row r="13" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="D13" s="45"/>
-      <c r="E13" s="45"/>
-      <c r="F13" s="45"/>
+      <c r="D13" s="48"/>
+      <c r="E13" s="48"/>
+      <c r="F13" s="48"/>
     </row>
     <row r="14" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="D14" s="45"/>
-      <c r="E14" s="45"/>
-      <c r="F14" s="45"/>
-      <c r="H14" s="26" t="s">
+      <c r="D14" s="48"/>
+      <c r="E14" s="48"/>
+      <c r="F14" s="48"/>
+      <c r="H14" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="I14" s="27"/>
-      <c r="J14" s="28"/>
-      <c r="L14" s="26" t="s">
+      <c r="I14" s="30"/>
+      <c r="J14" s="31"/>
+      <c r="L14" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="M14" s="27"/>
-      <c r="N14" s="28"/>
+      <c r="M14" s="30"/>
+      <c r="N14" s="31"/>
     </row>
     <row r="15" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="D15" s="45"/>
-      <c r="E15" s="45"/>
-      <c r="F15" s="45"/>
-      <c r="H15" s="29"/>
-      <c r="I15" s="30"/>
-      <c r="J15" s="31"/>
-      <c r="L15" s="29"/>
-      <c r="M15" s="30"/>
-      <c r="N15" s="31"/>
+      <c r="D15" s="48"/>
+      <c r="E15" s="48"/>
+      <c r="F15" s="48"/>
+      <c r="H15" s="32"/>
+      <c r="I15" s="33"/>
+      <c r="J15" s="34"/>
+      <c r="L15" s="32"/>
+      <c r="M15" s="33"/>
+      <c r="N15" s="34"/>
     </row>
     <row r="16" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="D16" s="45"/>
-      <c r="E16" s="45"/>
-      <c r="F16" s="45"/>
+      <c r="D16" s="48"/>
+      <c r="E16" s="48"/>
+      <c r="F16" s="48"/>
     </row>
     <row r="17" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="D17" s="45"/>
-      <c r="E17" s="45"/>
-      <c r="F17" s="45"/>
-      <c r="H17" s="32" t="s">
+      <c r="D17" s="48"/>
+      <c r="E17" s="48"/>
+      <c r="F17" s="48"/>
+      <c r="H17" s="41" t="s">
         <v>13</v>
       </c>
-      <c r="I17" s="33"/>
-      <c r="J17" s="34"/>
-      <c r="L17" s="26" t="s">
+      <c r="I17" s="42"/>
+      <c r="J17" s="43"/>
+      <c r="L17" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="M17" s="27"/>
-      <c r="N17" s="28"/>
+      <c r="M17" s="30"/>
+      <c r="N17" s="31"/>
     </row>
     <row r="18" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="H18" s="35"/>
-      <c r="I18" s="36"/>
-      <c r="J18" s="37"/>
-      <c r="L18" s="29"/>
-      <c r="M18" s="30"/>
-      <c r="N18" s="31"/>
+      <c r="H18" s="44"/>
+      <c r="I18" s="45"/>
+      <c r="J18" s="46"/>
+      <c r="L18" s="32"/>
+      <c r="M18" s="33"/>
+      <c r="N18" s="34"/>
     </row>
     <row r="20" spans="4:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H20" s="32" t="s">
+      <c r="H20" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="I20" s="33"/>
-      <c r="J20" s="34"/>
-      <c r="L20" s="26" t="s">
+      <c r="I20" s="42"/>
+      <c r="J20" s="43"/>
+      <c r="L20" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="M20" s="27"/>
-      <c r="N20" s="28"/>
+      <c r="M20" s="30"/>
+      <c r="N20" s="31"/>
     </row>
     <row r="21" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="H21" s="35"/>
-      <c r="I21" s="36"/>
-      <c r="J21" s="37"/>
-      <c r="L21" s="29"/>
-      <c r="M21" s="30"/>
-      <c r="N21" s="31"/>
+      <c r="H21" s="44"/>
+      <c r="I21" s="45"/>
+      <c r="J21" s="46"/>
+      <c r="L21" s="32"/>
+      <c r="M21" s="33"/>
+      <c r="N21" s="34"/>
     </row>
     <row r="23" spans="4:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H23" s="26" t="s">
+      <c r="H23" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="I23" s="27"/>
-      <c r="J23" s="28"/>
-      <c r="L23" s="26" t="s">
+      <c r="I23" s="30"/>
+      <c r="J23" s="31"/>
+      <c r="L23" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="M23" s="27"/>
-      <c r="N23" s="28"/>
+      <c r="M23" s="30"/>
+      <c r="N23" s="31"/>
     </row>
     <row r="24" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="H24" s="29"/>
-      <c r="I24" s="30"/>
-      <c r="J24" s="31"/>
-      <c r="L24" s="29"/>
-      <c r="M24" s="30"/>
-      <c r="N24" s="31"/>
+      <c r="H24" s="32"/>
+      <c r="I24" s="33"/>
+      <c r="J24" s="34"/>
+      <c r="L24" s="32"/>
+      <c r="M24" s="33"/>
+      <c r="N24" s="34"/>
     </row>
     <row r="26" spans="4:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H26" s="26" t="s">
+      <c r="H26" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="I26" s="27"/>
-      <c r="J26" s="28"/>
-      <c r="L26" s="26" t="s">
+      <c r="I26" s="30"/>
+      <c r="J26" s="31"/>
+      <c r="L26" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="M26" s="27"/>
-      <c r="N26" s="28"/>
+      <c r="M26" s="30"/>
+      <c r="N26" s="31"/>
     </row>
     <row r="27" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="H27" s="29"/>
-      <c r="I27" s="30"/>
-      <c r="J27" s="31"/>
-      <c r="L27" s="29"/>
-      <c r="M27" s="30"/>
-      <c r="N27" s="31"/>
+      <c r="H27" s="32"/>
+      <c r="I27" s="33"/>
+      <c r="J27" s="34"/>
+      <c r="L27" s="32"/>
+      <c r="M27" s="33"/>
+      <c r="N27" s="34"/>
     </row>
     <row r="29" spans="4:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H29" s="26" t="s">
+      <c r="H29" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="I29" s="27"/>
-      <c r="J29" s="28"/>
-      <c r="L29" s="26" t="s">
+      <c r="I29" s="30"/>
+      <c r="J29" s="31"/>
+      <c r="L29" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="M29" s="27"/>
-      <c r="N29" s="28"/>
+      <c r="M29" s="30"/>
+      <c r="N29" s="31"/>
     </row>
     <row r="30" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="H30" s="29"/>
-      <c r="I30" s="30"/>
-      <c r="J30" s="31"/>
-      <c r="L30" s="29"/>
-      <c r="M30" s="30"/>
-      <c r="N30" s="31"/>
+      <c r="H30" s="32"/>
+      <c r="I30" s="33"/>
+      <c r="J30" s="34"/>
+      <c r="L30" s="32"/>
+      <c r="M30" s="33"/>
+      <c r="N30" s="34"/>
     </row>
     <row r="32" spans="4:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H32" s="26" t="s">
+      <c r="H32" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="I32" s="27"/>
-      <c r="J32" s="28"/>
-      <c r="L32" s="26" t="s">
+      <c r="I32" s="30"/>
+      <c r="J32" s="31"/>
+      <c r="L32" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="M32" s="27"/>
-      <c r="N32" s="28"/>
+      <c r="M32" s="30"/>
+      <c r="N32" s="31"/>
     </row>
     <row r="33" spans="8:14" x14ac:dyDescent="0.25">
-      <c r="H33" s="29"/>
-      <c r="I33" s="30"/>
-      <c r="J33" s="31"/>
-      <c r="L33" s="29"/>
-      <c r="M33" s="30"/>
-      <c r="N33" s="31"/>
+      <c r="H33" s="32"/>
+      <c r="I33" s="33"/>
+      <c r="J33" s="34"/>
+      <c r="L33" s="32"/>
+      <c r="M33" s="33"/>
+      <c r="N33" s="34"/>
     </row>
     <row r="35" spans="8:14" x14ac:dyDescent="0.25">
-      <c r="H35" s="26" t="s">
+      <c r="H35" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="I35" s="27"/>
-      <c r="J35" s="28"/>
+      <c r="I35" s="30"/>
+      <c r="J35" s="31"/>
     </row>
     <row r="36" spans="8:14" x14ac:dyDescent="0.25">
-      <c r="H36" s="29"/>
-      <c r="I36" s="30"/>
-      <c r="J36" s="31"/>
+      <c r="H36" s="32"/>
+      <c r="I36" s="33"/>
+      <c r="J36" s="34"/>
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="H35:J36"/>
+    <mergeCell ref="L20:N21"/>
+    <mergeCell ref="L17:N18"/>
+    <mergeCell ref="L23:N24"/>
+    <mergeCell ref="L26:N27"/>
+    <mergeCell ref="L29:N30"/>
+    <mergeCell ref="L32:N33"/>
+    <mergeCell ref="H26:J27"/>
+    <mergeCell ref="H29:J30"/>
+    <mergeCell ref="H32:J33"/>
+    <mergeCell ref="H23:J24"/>
+    <mergeCell ref="H20:J21"/>
     <mergeCell ref="L14:N15"/>
     <mergeCell ref="D6:F7"/>
     <mergeCell ref="H2:J3"/>
@@ -9455,18 +12165,6 @@
     <mergeCell ref="L5:N6"/>
     <mergeCell ref="L8:N9"/>
     <mergeCell ref="L11:N12"/>
-    <mergeCell ref="H35:J36"/>
-    <mergeCell ref="L20:N21"/>
-    <mergeCell ref="L17:N18"/>
-    <mergeCell ref="L23:N24"/>
-    <mergeCell ref="L26:N27"/>
-    <mergeCell ref="L29:N30"/>
-    <mergeCell ref="L32:N33"/>
-    <mergeCell ref="H26:J27"/>
-    <mergeCell ref="H29:J30"/>
-    <mergeCell ref="H32:J33"/>
-    <mergeCell ref="H23:J24"/>
-    <mergeCell ref="H20:J21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -9763,10 +12461,10 @@
       <c r="G4" s="10"/>
       <c r="H4" s="10"/>
       <c r="I4" s="10"/>
-      <c r="J4" s="46" t="s">
+      <c r="J4" s="49" t="s">
         <v>45</v>
       </c>
-      <c r="K4" s="46"/>
+      <c r="K4" s="49"/>
       <c r="L4" s="10"/>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.25">
@@ -9782,8 +12480,8 @@
       <c r="G5" s="10"/>
       <c r="H5" s="10"/>
       <c r="I5" s="10"/>
-      <c r="J5" s="46"/>
-      <c r="K5" s="46"/>
+      <c r="J5" s="49"/>
+      <c r="K5" s="49"/>
       <c r="L5" s="10"/>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.25">
@@ -9799,8 +12497,8 @@
       <c r="G6" s="10"/>
       <c r="H6" s="10"/>
       <c r="I6" s="10"/>
-      <c r="J6" s="46"/>
-      <c r="K6" s="46"/>
+      <c r="J6" s="49"/>
+      <c r="K6" s="49"/>
       <c r="L6" s="10"/>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.25">
@@ -9814,8 +12512,8 @@
       <c r="G7" s="10"/>
       <c r="H7" s="10"/>
       <c r="I7" s="10"/>
-      <c r="J7" s="46"/>
-      <c r="K7" s="46"/>
+      <c r="J7" s="49"/>
+      <c r="K7" s="49"/>
       <c r="L7" s="10"/>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.25">
@@ -9827,8 +12525,8 @@
       <c r="G8" s="10"/>
       <c r="H8" s="10"/>
       <c r="I8" s="10"/>
-      <c r="J8" s="46"/>
-      <c r="K8" s="46"/>
+      <c r="J8" s="49"/>
+      <c r="K8" s="49"/>
       <c r="L8" s="10"/>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.25">
@@ -9844,8 +12542,8 @@
       <c r="G9" s="10"/>
       <c r="H9" s="10"/>
       <c r="I9" s="10"/>
-      <c r="J9" s="46"/>
-      <c r="K9" s="46"/>
+      <c r="J9" s="49"/>
+      <c r="K9" s="49"/>
       <c r="L9" s="10"/>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.25">
@@ -9861,8 +12559,8 @@
       <c r="G10" s="10"/>
       <c r="H10" s="10"/>
       <c r="I10" s="10"/>
-      <c r="J10" s="46"/>
-      <c r="K10" s="46"/>
+      <c r="J10" s="49"/>
+      <c r="K10" s="49"/>
       <c r="L10" s="10"/>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.25">
@@ -9878,8 +12576,8 @@
       <c r="G11" s="10"/>
       <c r="H11" s="10"/>
       <c r="I11" s="10"/>
-      <c r="J11" s="46"/>
-      <c r="K11" s="46"/>
+      <c r="J11" s="49"/>
+      <c r="K11" s="49"/>
       <c r="L11" s="10"/>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.25">
@@ -10371,13 +13069,13 @@
       </c>
       <c r="B11" s="18"/>
       <c r="C11" s="17"/>
-      <c r="D11" s="47"/>
+      <c r="D11" s="50"/>
     </row>
     <row r="12" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="17"/>
       <c r="B12" s="17"/>
       <c r="C12" s="17"/>
-      <c r="D12" s="48"/>
+      <c r="D12" s="51"/>
     </row>
     <row r="13" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="17" t="s">
@@ -10385,7 +13083,7 @@
       </c>
       <c r="B13" s="18"/>
       <c r="C13" s="17"/>
-      <c r="D13" s="49"/>
+      <c r="D13" s="52"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="17"/>

</xml_diff>